<commit_message>
Auto update stocks_data.xlsx [2025-10-22 05:50:11]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,9 +445,19 @@
           <t>2025/10/22</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2025/10/22</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>上证</t>
         </is>
@@ -457,23 +467,543 @@
       <c r="B3" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>63.83</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="n">
         <v>3909.19</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>3907.68</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>50.06</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="n">
         <v>5493.31</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>5490.93</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="C9" s="3" t="n">
+        <v>55.75</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="3" t="n">
+        <v>4587.71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="1" t="n"/>
+    </row>
+    <row r="12">
+      <c r="C12" s="3" t="n">
+        <v>61.67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="3" t="n">
+        <v>7132.24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="1" t="n"/>
+    </row>
+    <row r="15">
+      <c r="C15" s="3" t="n">
+        <v>28.36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSIH30455","current":2671.819,"percent":-0.74,"chg":-19.8325,"timestamp":1761112079000,"volume":18662173920,"amount":4.674621301172E11,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":0.84,"open":2676.3966,"last_close":2691.6515,"high":2685.7779,"low":2663.0872,"avg_price":2671.819,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":22.94,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="1" t="n"/>
+    </row>
+    <row r="18">
+      <c r="C18" s="3" t="n">
+        <v>95.76000000000001</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="3" t="n">
+        <v>6735.35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="1" t="n"/>
+    </row>
+    <row r="21">
+      <c r="C21" s="3" t="n">
+        <v>67.68000000000001</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">var hq_str_znb_SENSEX="印度孟买SENSEX,84426.3400,62.97,0.07,2:12 AM,1759126320,2025-10-21,20:49:06,84484.6700,84363.3700,84665.4400,84286.4000,0";
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="1" t="n"/>
+    </row>
+    <row r="24">
+      <c r="C24" s="3" t="n">
+        <v>85.68000000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">var hq_str_znb_DAX_i="2025-10-21,19909.1400|23880.7200|23830.9900";
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="1" t="n"/>
+    </row>
+    <row r="27">
+      <c r="C27" s="3" t="n">
+        <v>78.34999999999999</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">var hq_str_znb_NKY_i="2025-10-22,39894.5400|44932.6300|47582.1500";
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="1" t="n"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="3" t="n">
+        <v>57.37</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="3" t="n">
+        <v>5632.32</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="1" t="n"/>
+    </row>
+    <row r="33">
+      <c r="C33" s="3" t="n">
+        <v>10.04</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI931468","current":33445.6311,"percent":-0.29,"chg":-95.6521,"timestamp":1761112089000,"volume":427846387,"amount":2.9311508457E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":0.69,"open":33430.6022,"last_close":33541.2832,"high":33600.3149,"low":33370.4102,"avg_price":33445.6311,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":14.59,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="1" t="n"/>
+    </row>
+    <row r="36">
+      <c r="C36" s="3" t="n">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" s="3" t="n">
+        <v>3227.95</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="C38" s="1" t="n"/>
+    </row>
+    <row r="39">
+      <c r="C39" s="3" t="n">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" s="3" t="n">
+        <v>3059.56</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" s="1" t="n"/>
+    </row>
+    <row r="42">
+      <c r="C42" s="3" t="n">
+        <v>19.53</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" s="3" t="n">
+        <v>7395.5</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" s="1" t="n"/>
+    </row>
+    <row r="45">
+      <c r="C45" s="3" t="n">
+        <v>33.2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" s="3" t="n">
+        <v>9012.639999999999</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" s="1" t="n"/>
+    </row>
+    <row r="48">
+      <c r="C48" s="3" t="n">
+        <v>9.710000000000001</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI931068","current":12954.6975,"percent":-0.49,"chg":-63.8982,"timestamp":1761112094000,"volume":558851888,"amount":2.1955451514E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":0.73,"open":12984.1283,"last_close":13018.5957,"high":13045.6187,"low":12951.164,"avg_price":12954.6975,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":-1.24,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" s="1" t="n"/>
+    </row>
+    <row r="51">
+      <c r="C51" s="3" t="n">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI930697","current":12402.5431,"percent":0.54,"chg":66.4424,"timestamp":1761112094000,"volume":1001440912,"amount":2.2975955291E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.66,"open":12276.5158,"last_close":12336.1007,"high":12477.5553,"low":12272.8604,"avg_price":12402.5431,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":10.03,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" s="1" t="n"/>
+    </row>
+    <row r="54">
+      <c r="C54" s="3" t="n">
+        <v>18.98</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" s="3" t="n">
+        <v>9738.559999999999</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="C56" s="1" t="n"/>
+    </row>
+    <row r="57">
+      <c r="C57" s="3" t="n">
+        <v>24.91</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" s="3" t="n">
+        <v>16145.35</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" s="1" t="n"/>
+    </row>
+    <row r="60">
+      <c r="C60" s="3" t="n">
+        <v>33.53</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"HKHSHKBIO","current":17526.85,"percent":null,"chg":null,"timestamp":1761094512996,"volume":507247105,"amount":1.2285698255370003E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":null,"open":null,"last_close":17526.85,"high":null,"low":null,"avg_price":17526.85,"trade_volume":null,"side":0,"is_trade":false,"level":3,"trade_session":2,"trade_type":null,"current_year_percent":null,"trade_unique_id":null,"type":31,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="C62" s="1" t="n"/>
+    </row>
+    <row r="63">
+      <c r="C63" s="3" t="n">
+        <v>21.28</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSIH30533","current":10208.2906,"percent":-1.61,"chg":-167.4857,"timestamp":1761112099000,"volume":244887839,"amount":2.06722357458E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":2.21,"open":10375.7763,"last_close":10375.7763,"high":10376.4832,"low":10146.8529,"avg_price":10208.2906,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":39.04,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="C65" s="1" t="n"/>
+    </row>
+    <row r="66">
+      <c r="C66" s="3" t="n">
+        <v>15.36</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI930641","current":9929.5771,"percent":0.22,"chg":21.5542,"timestamp":1761112104000,"volume":473841987,"amount":7.494386661E9,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.0,"open":9877.1689,"last_close":9908.0229,"high":9968.7218,"low":9870.1155,"avg_price":9929.5771,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":-2.19,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="C68" s="1" t="n"/>
+    </row>
+    <row r="69">
+      <c r="C69" s="3" t="n">
+        <v>21.08</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"HKHSIII","current":3140.3,"percent":-1.79,"chg":-57.39,"timestamp":1761112108000,"volume":718445577,"amount":2.222343658913E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.79,"open":3168.3,"last_close":3197.69,"high":3173.72,"low":3116.58,"avg_price":3140.43,"trade_volume":null,"side":0,"is_trade":false,"level":3,"trade_session":2,"trade_type":null,"current_year_percent":37.0,"trade_unique_id":null,"type":31,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="C71" s="1" t="n"/>
+    </row>
+    <row r="72">
+      <c r="C72" s="3" t="n">
+        <v>44.37</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"HKHSTECH","current":5918.54,"percent":-1.49,"chg":-89.4,"timestamp":1761112110000,"volume":850729315,"amount":3.558474144396E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.87,"open":5958.63,"last_close":6007.94,"high":5979.51,"low":5867.12,"avg_price":5918.82,"trade_volume":null,"side":0,"is_trade":false,"level":3,"trade_session":2,"trade_type":null,"current_year_percent":32.46,"trade_unique_id":null,"type":31,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="C74" s="1" t="n"/>
+    </row>
+    <row r="75">
+      <c r="C75" s="3" t="n">
+        <v>30.39</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="C76" s="3" t="n">
+        <v>9484.940000000001</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="C77" s="1" t="n"/>
+    </row>
+    <row r="78">
+      <c r="C78" s="3" t="n">
+        <v>18.35</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="C79" s="3" t="n">
+        <v>2450.16</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="C80" s="1" t="n"/>
+    </row>
+    <row r="81">
+      <c r="C81" s="3" t="n">
+        <v>55.78</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="C82" s="3" t="n">
+        <v>2634.98</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="C83" s="1" t="n"/>
+    </row>
+    <row r="84">
+      <c r="C84" s="3" t="n">
+        <v>58.79</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="C85" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI931151","current":2699.0428,"percent":-1.69,"chg":-46.337,"timestamp":1761112109000,"volume":1269385838,"amount":2.6148880739000004E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.82,"open":2732.1495,"last_close":2745.3798,"high":2741.0958,"low":2691.2117,"avg_price":2699.0428,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":19.18,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="C86" s="1" t="n"/>
+    </row>
+    <row r="87">
+      <c r="C87" s="3" t="n">
+        <v>51.71</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="C88" s="3" t="n">
+        <v>3782.35</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="C89" s="1" t="n"/>
+    </row>
+    <row r="90">
+      <c r="C90" s="3" t="n">
+        <v>48.63</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI931152","current":2067.7389,"percent":-0.73,"chg":-15.2072,"timestamp":1761112109000,"volume":385967114,"amount":1.4364846442E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.89,"open":2082.7298,"last_close":2082.9461,"high":2106.2871,"low":2066.8571,"avg_price":2067.7389,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":30.27,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="C92" s="1" t="n"/>
+    </row>
+    <row r="93">
+      <c r="C93" s="3" t="n">
+        <v>27.72</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="C94" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"BK0044","current":13766.34,"percent":-0.23,"chg":-32.32,"timestamp":1761112116010,"volume":529172637,"amount":1.157873290149E10,"market_capital":1.506491266833E12,"float_market_capital":1.382395753712E12,"turnover_rate":1.22,"amplitude":0.008834191146096768,"open":13797.76,"last_close":13798.66,"high":13871.32,"low":13749.42,"avg_price":null,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":29.71,"trade_unique_id":null,"type":81,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="C95" s="1" t="n"/>
+    </row>
+    <row r="96">
+      <c r="C96" s="3" t="n">
+        <v>88.04000000000001</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="C97" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSIH30184","current":9255.7456,"percent":-0.01,"chg":-1.1413,"timestamp":1761112114000,"volume":1359520443,"amount":1.00925691884E11,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":3.48,"open":9139.196,"last_close":9256.8869,"high":9353.9583,"low":9031.5413,"avg_price":9255.7456,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":46.71,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="C98" s="1" t="n"/>
+    </row>
+    <row r="99">
+      <c r="C99" s="3" t="n">
+        <v>58.2</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="C100" s="3" t="n">
+        <v>12076.97</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="C101" s="1" t="n"/>
+    </row>
+    <row r="102">
+      <c r="C102" s="3" t="n">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="C103" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI930707","current":2234.2498,"percent":-1.11,"chg":-25.0487,"timestamp":1761112114000,"volume":409147988,"amount":5.319795731E9,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.17,"open":2255.8991,"last_close":2259.2985,"high":2259.5952,"low":2233.0723,"avg_price":2234.2498,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":11.06,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="C104" s="1" t="n"/>
+    </row>
+    <row r="105">
+      <c r="C105" s="3" t="n">
+        <v>30.47</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="C106" s="3" t="n">
+        <v>868.04</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="C107" s="1" t="n"/>
+    </row>
+    <row r="108">
+      <c r="C108" s="3" t="n">
+        <v>29.71</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" s="1" t="inlineStr">
+        <is>
+          <t>{"data":[{"symbol":"CSI930708","current":2655.1198,"percent":-1.56,"chg":-42.0778,"timestamp":1761112119000,"volume":3570049022,"amount":6.758077676799999E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":2.65,"open":2600.2732,"last_close":2697.1976,"high":2671.161,"low":2599.7633,"avg_price":2655.1198,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":65.01,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="C110" s="1" t="n"/>
+    </row>
+    <row r="111">
+      <c r="C111" s="3" t="n">
+        <v>20.62</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="C112" s="3" t="n">
+        <v>4045.61</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="C113" s="1" t="n"/>
+    </row>
+    <row r="114">
+      <c r="C114" s="3" t="n">
+        <v>29.02</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="C115" s="3" t="n">
+        <v>3508.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-10-22 06:25:56]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,11 @@
           <t>2025/10/22</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2025/10/22</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -458,6 +463,11 @@
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>上证</t>
         </is>
@@ -470,6 +480,9 @@
       <c r="C3" s="3" t="n">
         <v>63.83</v>
       </c>
+      <c r="D3" s="3" t="n">
+        <v>63.83</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="n">
@@ -478,10 +491,14 @@
       <c r="C4" s="3" t="n">
         <v>3907.68</v>
       </c>
+      <c r="D4" s="3" t="n">
+        <v>3914.49</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="3" t="n">
@@ -490,6 +507,9 @@
       <c r="C6" s="3" t="n">
         <v>50.06</v>
       </c>
+      <c r="D6" s="3" t="n">
+        <v>50.06</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="n">
@@ -498,40 +518,61 @@
       <c r="C7" s="3" t="n">
         <v>5490.93</v>
       </c>
+      <c r="D7" s="3" t="n">
+        <v>5498.71</v>
+      </c>
     </row>
     <row r="8">
       <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="C9" s="3" t="n">
         <v>55.75</v>
       </c>
+      <c r="D9" s="3" t="n">
+        <v>55.75</v>
+      </c>
     </row>
     <row r="10">
       <c r="C10" s="3" t="n">
         <v>4587.71</v>
       </c>
+      <c r="D10" s="3" t="n">
+        <v>4596.44</v>
+      </c>
     </row>
     <row r="11">
       <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="C12" s="3" t="n">
         <v>61.67</v>
       </c>
+      <c r="D12" s="3" t="n">
+        <v>61.67</v>
+      </c>
     </row>
     <row r="13">
       <c r="C13" s="3" t="n">
         <v>7132.24</v>
       </c>
+      <c r="D13" s="3" t="n">
+        <v>7131.91</v>
+      </c>
     </row>
     <row r="14">
       <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="C15" s="3" t="n">
         <v>28.36</v>
       </c>
+      <c r="D15" s="3" t="n">
+        <v>28.36</v>
+      </c>
     </row>
     <row r="16">
       <c r="C16" s="1" t="inlineStr">
@@ -539,27 +580,41 @@
           <t>{"data":[{"symbol":"CSIH30455","current":2671.819,"percent":-0.74,"chg":-19.8325,"timestamp":1761112079000,"volume":18662173920,"amount":4.674621301172E11,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":0.84,"open":2676.3966,"last_close":2691.6515,"high":2685.7779,"low":2663.0872,"avg_price":2671.819,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":22.94,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D16" s="3" t="n">
+        <v>2675.88</v>
+      </c>
     </row>
     <row r="17">
       <c r="C17" s="1" t="n"/>
+      <c r="D17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="C18" s="3" t="n">
         <v>95.76000000000001</v>
       </c>
+      <c r="D18" s="3" t="n">
+        <v>95.76000000000001</v>
+      </c>
     </row>
     <row r="19">
       <c r="C19" s="3" t="n">
         <v>6735.35</v>
       </c>
+      <c r="D19" s="3" t="n">
+        <v>6735.35</v>
+      </c>
     </row>
     <row r="20">
       <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="C21" s="3" t="n">
         <v>67.68000000000001</v>
       </c>
+      <c r="D21" s="3" t="n">
+        <v>67.68000000000001</v>
+      </c>
     </row>
     <row r="22">
       <c r="C22" s="1" t="inlineStr">
@@ -568,14 +623,21 @@
 </t>
         </is>
       </c>
+      <c r="D22" s="3" t="n">
+        <v>84426.34</v>
+      </c>
     </row>
     <row r="23">
       <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="C24" s="3" t="n">
         <v>85.68000000000001</v>
       </c>
+      <c r="D24" s="3" t="n">
+        <v>85.68000000000001</v>
+      </c>
     </row>
     <row r="25">
       <c r="C25" s="1" t="inlineStr">
@@ -584,14 +646,21 @@
 </t>
         </is>
       </c>
+      <c r="D25" s="3" t="n">
+        <v>19909.14</v>
+      </c>
     </row>
     <row r="26">
       <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="C27" s="3" t="n">
         <v>78.34999999999999</v>
       </c>
+      <c r="D27" s="3" t="n">
+        <v>78.34999999999999</v>
+      </c>
     </row>
     <row r="28">
       <c r="C28" s="1" t="inlineStr">
@@ -600,27 +669,41 @@
 </t>
         </is>
       </c>
+      <c r="D28" s="3" t="n">
+        <v>39894.54</v>
+      </c>
     </row>
     <row r="29">
       <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="C30" s="3" t="n">
         <v>57.37</v>
       </c>
+      <c r="D30" s="3" t="n">
+        <v>57.37</v>
+      </c>
     </row>
     <row r="31">
       <c r="C31" s="3" t="n">
         <v>5632.32</v>
       </c>
+      <c r="D31" s="3" t="n">
+        <v>5649.26</v>
+      </c>
     </row>
     <row r="32">
       <c r="C32" s="1" t="n"/>
+      <c r="D32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="C33" s="3" t="n">
         <v>10.04</v>
       </c>
+      <c r="D33" s="3" t="n">
+        <v>10.04</v>
+      </c>
     </row>
     <row r="34">
       <c r="C34" s="1" t="inlineStr">
@@ -628,66 +711,101 @@
           <t>{"data":[{"symbol":"CSI931468","current":33445.6311,"percent":-0.29,"chg":-95.6521,"timestamp":1761112089000,"volume":427846387,"amount":2.9311508457E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":0.69,"open":33430.6022,"last_close":33541.2832,"high":33600.3149,"low":33370.4102,"avg_price":33445.6311,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":14.59,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D34" s="3" t="n">
+        <v>33455.38</v>
+      </c>
     </row>
     <row r="35">
       <c r="C35" s="1" t="n"/>
+      <c r="D35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="C36" s="3" t="n">
         <v>30.5</v>
       </c>
+      <c r="D36" s="3" t="n">
+        <v>30.5</v>
+      </c>
     </row>
     <row r="37">
       <c r="C37" s="3" t="n">
         <v>3227.95</v>
       </c>
+      <c r="D37" s="3" t="n">
+        <v>3229.07</v>
+      </c>
     </row>
     <row r="38">
       <c r="C38" s="1" t="n"/>
+      <c r="D38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="C39" s="3" t="n">
         <v>48.4</v>
       </c>
+      <c r="D39" s="3" t="n">
+        <v>48.4</v>
+      </c>
     </row>
     <row r="40">
       <c r="C40" s="3" t="n">
         <v>3059.56</v>
       </c>
+      <c r="D40" s="3" t="n">
+        <v>3059.91</v>
+      </c>
     </row>
     <row r="41">
       <c r="C41" s="1" t="n"/>
+      <c r="D41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="C42" s="3" t="n">
         <v>19.53</v>
       </c>
+      <c r="D42" s="3" t="n">
+        <v>19.53</v>
+      </c>
     </row>
     <row r="43">
       <c r="C43" s="3" t="n">
         <v>7395.5</v>
       </c>
+      <c r="D43" s="3" t="n">
+        <v>7397.02</v>
+      </c>
     </row>
     <row r="44">
       <c r="C44" s="1" t="n"/>
+      <c r="D44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="C45" s="3" t="n">
         <v>33.2</v>
       </c>
+      <c r="D45" s="3" t="n">
+        <v>33.2</v>
+      </c>
     </row>
     <row r="46">
       <c r="C46" s="3" t="n">
         <v>9012.639999999999</v>
       </c>
+      <c r="D46" s="3" t="n">
+        <v>9016.719999999999</v>
+      </c>
     </row>
     <row r="47">
       <c r="C47" s="1" t="n"/>
+      <c r="D47" s="1" t="n"/>
     </row>
     <row r="48">
       <c r="C48" s="3" t="n">
         <v>9.710000000000001</v>
       </c>
+      <c r="D48" s="3" t="n">
+        <v>9.710000000000001</v>
+      </c>
     </row>
     <row r="49">
       <c r="C49" s="1" t="inlineStr">
@@ -695,14 +813,21 @@
           <t>{"data":[{"symbol":"CSI931068","current":12954.6975,"percent":-0.49,"chg":-63.8982,"timestamp":1761112094000,"volume":558851888,"amount":2.1955451514E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":0.73,"open":12984.1283,"last_close":13018.5957,"high":13045.6187,"low":12951.164,"avg_price":12954.6975,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":-1.24,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D49" s="3" t="n">
+        <v>12976.73</v>
+      </c>
     </row>
     <row r="50">
       <c r="C50" s="1" t="n"/>
+      <c r="D50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="C51" s="3" t="n">
         <v>22.73</v>
       </c>
+      <c r="D51" s="3" t="n">
+        <v>22.73</v>
+      </c>
     </row>
     <row r="52">
       <c r="C52" s="1" t="inlineStr">
@@ -710,40 +835,61 @@
           <t>{"data":[{"symbol":"CSI930697","current":12402.5431,"percent":0.54,"chg":66.4424,"timestamp":1761112094000,"volume":1001440912,"amount":2.2975955291E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.66,"open":12276.5158,"last_close":12336.1007,"high":12477.5553,"low":12272.8604,"avg_price":12402.5431,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":10.03,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D52" s="3" t="n">
+        <v>12435.27</v>
+      </c>
     </row>
     <row r="53">
       <c r="C53" s="1" t="n"/>
+      <c r="D53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="C54" s="3" t="n">
         <v>18.98</v>
       </c>
+      <c r="D54" s="3" t="n">
+        <v>18.98</v>
+      </c>
     </row>
     <row r="55">
       <c r="C55" s="3" t="n">
         <v>9738.559999999999</v>
       </c>
+      <c r="D55" s="3" t="n">
+        <v>9752.719999999999</v>
+      </c>
     </row>
     <row r="56">
       <c r="C56" s="1" t="n"/>
+      <c r="D56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="C57" s="3" t="n">
         <v>24.91</v>
       </c>
+      <c r="D57" s="3" t="n">
+        <v>24.91</v>
+      </c>
     </row>
     <row r="58">
       <c r="C58" s="3" t="n">
         <v>16145.35</v>
       </c>
+      <c r="D58" s="3" t="n">
+        <v>16165.24</v>
+      </c>
     </row>
     <row r="59">
       <c r="C59" s="1" t="n"/>
+      <c r="D59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="C60" s="3" t="n">
         <v>33.53</v>
       </c>
+      <c r="D60" s="3" t="n">
+        <v>33.53</v>
+      </c>
     </row>
     <row r="61">
       <c r="C61" s="1" t="inlineStr">
@@ -751,14 +897,21 @@
           <t>{"data":[{"symbol":"HKHSHKBIO","current":17526.85,"percent":null,"chg":null,"timestamp":1761094512996,"volume":507247105,"amount":1.2285698255370003E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":null,"open":null,"last_close":17526.85,"high":null,"low":null,"avg_price":17526.85,"trade_volume":null,"side":0,"is_trade":false,"level":3,"trade_session":2,"trade_type":null,"current_year_percent":null,"trade_unique_id":null,"type":31,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D61" s="3" t="n">
+        <v>17526.85</v>
+      </c>
     </row>
     <row r="62">
       <c r="C62" s="1" t="n"/>
+      <c r="D62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="C63" s="3" t="n">
         <v>21.28</v>
       </c>
+      <c r="D63" s="3" t="n">
+        <v>21.28</v>
+      </c>
     </row>
     <row r="64">
       <c r="C64" s="1" t="inlineStr">
@@ -766,14 +919,21 @@
           <t>{"data":[{"symbol":"CSIH30533","current":10208.2906,"percent":-1.61,"chg":-167.4857,"timestamp":1761112099000,"volume":244887839,"amount":2.06722357458E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":2.21,"open":10375.7763,"last_close":10375.7763,"high":10376.4832,"low":10146.8529,"avg_price":10208.2906,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":39.04,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D64" s="3" t="n">
+        <v>10228.42</v>
+      </c>
     </row>
     <row r="65">
       <c r="C65" s="1" t="n"/>
+      <c r="D65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="C66" s="3" t="n">
         <v>15.36</v>
       </c>
+      <c r="D66" s="3" t="n">
+        <v>15.36</v>
+      </c>
     </row>
     <row r="67">
       <c r="C67" s="1" t="inlineStr">
@@ -781,14 +941,21 @@
           <t>{"data":[{"symbol":"CSI930641","current":9929.5771,"percent":0.22,"chg":21.5542,"timestamp":1761112104000,"volume":473841987,"amount":7.494386661E9,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.0,"open":9877.1689,"last_close":9908.0229,"high":9968.7218,"low":9870.1155,"avg_price":9929.5771,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":-2.19,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D67" s="3" t="n">
+        <v>9930.68</v>
+      </c>
     </row>
     <row r="68">
       <c r="C68" s="1" t="n"/>
+      <c r="D68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="C69" s="3" t="n">
         <v>21.08</v>
       </c>
+      <c r="D69" s="3" t="n">
+        <v>21.08</v>
+      </c>
     </row>
     <row r="70">
       <c r="C70" s="1" t="inlineStr">
@@ -796,14 +963,21 @@
           <t>{"data":[{"symbol":"HKHSIII","current":3140.3,"percent":-1.79,"chg":-57.39,"timestamp":1761112108000,"volume":718445577,"amount":2.222343658913E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.79,"open":3168.3,"last_close":3197.69,"high":3173.72,"low":3116.58,"avg_price":3140.43,"trade_volume":null,"side":0,"is_trade":false,"level":3,"trade_session":2,"trade_type":null,"current_year_percent":37.0,"trade_unique_id":null,"type":31,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D70" s="3" t="n">
+        <v>3142.01</v>
+      </c>
     </row>
     <row r="71">
       <c r="C71" s="1" t="n"/>
+      <c r="D71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="C72" s="3" t="n">
         <v>44.37</v>
       </c>
+      <c r="D72" s="3" t="n">
+        <v>44.37</v>
+      </c>
     </row>
     <row r="73">
       <c r="C73" s="1" t="inlineStr">
@@ -811,53 +985,81 @@
           <t>{"data":[{"symbol":"HKHSTECH","current":5918.54,"percent":-1.49,"chg":-89.4,"timestamp":1761112110000,"volume":850729315,"amount":3.558474144396E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.87,"open":5958.63,"last_close":6007.94,"high":5979.51,"low":5867.12,"avg_price":5918.82,"trade_volume":null,"side":0,"is_trade":false,"level":3,"trade_session":2,"trade_type":null,"current_year_percent":32.46,"trade_unique_id":null,"type":31,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D73" s="3" t="n">
+        <v>5926.91</v>
+      </c>
     </row>
     <row r="74">
       <c r="C74" s="1" t="n"/>
+      <c r="D74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="C75" s="3" t="n">
         <v>30.39</v>
       </c>
+      <c r="D75" s="3" t="n">
+        <v>30.39</v>
+      </c>
     </row>
     <row r="76">
       <c r="C76" s="3" t="n">
         <v>9484.940000000001</v>
       </c>
+      <c r="D76" s="3" t="n">
+        <v>9486.709999999999</v>
+      </c>
     </row>
     <row r="77">
       <c r="C77" s="1" t="n"/>
+      <c r="D77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="C78" s="3" t="n">
         <v>18.35</v>
       </c>
+      <c r="D78" s="3" t="n">
+        <v>18.35</v>
+      </c>
     </row>
     <row r="79">
       <c r="C79" s="3" t="n">
         <v>2450.16</v>
       </c>
+      <c r="D79" s="3" t="n">
+        <v>2458.76</v>
+      </c>
     </row>
     <row r="80">
       <c r="C80" s="1" t="n"/>
+      <c r="D80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="C81" s="3" t="n">
         <v>55.78</v>
       </c>
+      <c r="D81" s="3" t="n">
+        <v>55.78</v>
+      </c>
     </row>
     <row r="82">
       <c r="C82" s="3" t="n">
         <v>2634.98</v>
       </c>
+      <c r="D82" s="3" t="n">
+        <v>2635.51</v>
+      </c>
     </row>
     <row r="83">
       <c r="C83" s="1" t="n"/>
+      <c r="D83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="C84" s="3" t="n">
         <v>58.79</v>
       </c>
+      <c r="D84" s="3" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85">
       <c r="C85" s="1" t="inlineStr">
@@ -865,27 +1067,41 @@
           <t>{"data":[{"symbol":"CSI931151","current":2699.0428,"percent":-1.69,"chg":-46.337,"timestamp":1761112109000,"volume":1269385838,"amount":2.6148880739000004E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.82,"open":2732.1495,"last_close":2745.3798,"high":2741.0958,"low":2691.2117,"avg_price":2699.0428,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":19.18,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D85" s="3" t="n">
+        <v>2698.2</v>
+      </c>
     </row>
     <row r="86">
       <c r="C86" s="1" t="n"/>
+      <c r="D86" s="1" t="n"/>
     </row>
     <row r="87">
       <c r="C87" s="3" t="n">
         <v>51.71</v>
       </c>
+      <c r="D87" s="3" t="n">
+        <v>51.71</v>
+      </c>
     </row>
     <row r="88">
       <c r="C88" s="3" t="n">
         <v>3782.35</v>
       </c>
+      <c r="D88" s="3" t="n">
+        <v>3783.74</v>
+      </c>
     </row>
     <row r="89">
       <c r="C89" s="1" t="n"/>
+      <c r="D89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="C90" s="3" t="n">
         <v>48.63</v>
       </c>
+      <c r="D90" s="3" t="n">
+        <v>48.63</v>
+      </c>
     </row>
     <row r="91">
       <c r="C91" s="1" t="inlineStr">
@@ -893,14 +1109,21 @@
           <t>{"data":[{"symbol":"CSI931152","current":2067.7389,"percent":-0.73,"chg":-15.2072,"timestamp":1761112109000,"volume":385967114,"amount":1.4364846442E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.89,"open":2082.7298,"last_close":2082.9461,"high":2106.2871,"low":2066.8571,"avg_price":2067.7389,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":30.27,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D91" s="3" t="n">
+        <v>2067.64</v>
+      </c>
     </row>
     <row r="92">
       <c r="C92" s="1" t="n"/>
+      <c r="D92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="C93" s="3" t="n">
         <v>27.72</v>
       </c>
+      <c r="D93" s="3" t="n">
+        <v>27.72</v>
+      </c>
     </row>
     <row r="94">
       <c r="C94" s="1" t="inlineStr">
@@ -908,14 +1131,21 @@
           <t>{"data":[{"symbol":"BK0044","current":13766.34,"percent":-0.23,"chg":-32.32,"timestamp":1761112116010,"volume":529172637,"amount":1.157873290149E10,"market_capital":1.506491266833E12,"float_market_capital":1.382395753712E12,"turnover_rate":1.22,"amplitude":0.008834191146096768,"open":13797.76,"last_close":13798.66,"high":13871.32,"low":13749.42,"avg_price":null,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":29.71,"trade_unique_id":null,"type":81,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D94" s="3" t="n">
+        <v>13758.07</v>
+      </c>
     </row>
     <row r="95">
       <c r="C95" s="1" t="n"/>
+      <c r="D95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="C96" s="3" t="n">
         <v>88.04000000000001</v>
       </c>
+      <c r="D96" s="3" t="n">
+        <v>88.04000000000001</v>
+      </c>
     </row>
     <row r="97">
       <c r="C97" s="1" t="inlineStr">
@@ -923,27 +1153,41 @@
           <t>{"data":[{"symbol":"CSIH30184","current":9255.7456,"percent":-0.01,"chg":-1.1413,"timestamp":1761112114000,"volume":1359520443,"amount":1.00925691884E11,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":3.48,"open":9139.196,"last_close":9256.8869,"high":9353.9583,"low":9031.5413,"avg_price":9255.7456,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":46.71,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D97" s="3" t="n">
+        <v>9221.57</v>
+      </c>
     </row>
     <row r="98">
       <c r="C98" s="1" t="n"/>
+      <c r="D98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="C99" s="3" t="n">
         <v>58.2</v>
       </c>
+      <c r="D99" s="3" t="n">
+        <v>58.2</v>
+      </c>
     </row>
     <row r="100">
       <c r="C100" s="3" t="n">
         <v>12076.97</v>
       </c>
+      <c r="D100" s="3" t="n">
+        <v>12069.97</v>
+      </c>
     </row>
     <row r="101">
       <c r="C101" s="1" t="n"/>
+      <c r="D101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="C102" s="3" t="n">
         <v>3.09</v>
       </c>
+      <c r="D102" s="3" t="n">
+        <v>3.09</v>
+      </c>
     </row>
     <row r="103">
       <c r="C103" s="1" t="inlineStr">
@@ -951,27 +1195,41 @@
           <t>{"data":[{"symbol":"CSI930707","current":2234.2498,"percent":-1.11,"chg":-25.0487,"timestamp":1761112114000,"volume":409147988,"amount":5.319795731E9,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":1.17,"open":2255.8991,"last_close":2259.2985,"high":2259.5952,"low":2233.0723,"avg_price":2234.2498,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":11.06,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D103" s="3" t="n">
+        <v>2235.14</v>
+      </c>
     </row>
     <row r="104">
       <c r="C104" s="1" t="n"/>
+      <c r="D104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="C105" s="3" t="n">
         <v>30.47</v>
       </c>
+      <c r="D105" s="3" t="n">
+        <v>30.47</v>
+      </c>
     </row>
     <row r="106">
       <c r="C106" s="3" t="n">
         <v>868.04</v>
       </c>
+      <c r="D106" s="3" t="n">
+        <v>869.04</v>
+      </c>
     </row>
     <row r="107">
       <c r="C107" s="1" t="n"/>
+      <c r="D107" s="1" t="n"/>
     </row>
     <row r="108">
       <c r="C108" s="3" t="n">
         <v>29.71</v>
       </c>
+      <c r="D108" s="3" t="n">
+        <v>29.71</v>
+      </c>
     </row>
     <row r="109">
       <c r="C109" s="1" t="inlineStr">
@@ -979,31 +1237,48 @@
           <t>{"data":[{"symbol":"CSI930708","current":2655.1198,"percent":-1.56,"chg":-42.0778,"timestamp":1761112119000,"volume":3570049022,"amount":6.758077676799999E10,"market_capital":null,"float_market_capital":null,"turnover_rate":null,"amplitude":2.65,"open":2600.2732,"last_close":2697.1976,"high":2671.161,"low":2599.7633,"avg_price":2655.1198,"trade_volume":null,"side":0,"is_trade":false,"level":1,"trade_session":null,"trade_type":null,"current_year_percent":65.01,"trade_unique_id":null,"type":26,"bid_appl_seq_num":null,"offer_appl_seq_num":null,"volume_ext":null,"traded_amount_ext":null,"trade_type_v2":null,"yield_to_maturity":null}],"error_code":0,"error_description":null}</t>
         </is>
       </c>
+      <c r="D109" s="3" t="n">
+        <v>2659.06</v>
+      </c>
     </row>
     <row r="110">
       <c r="C110" s="1" t="n"/>
+      <c r="D110" s="1" t="n"/>
     </row>
     <row r="111">
       <c r="C111" s="3" t="n">
         <v>20.62</v>
       </c>
+      <c r="D111" s="3" t="n">
+        <v>20.62</v>
+      </c>
     </row>
     <row r="112">
       <c r="C112" s="3" t="n">
         <v>4045.61</v>
       </c>
+      <c r="D112" s="3" t="n">
+        <v>4050.56</v>
+      </c>
     </row>
     <row r="113">
       <c r="C113" s="1" t="n"/>
+      <c r="D113" s="1" t="n"/>
     </row>
     <row r="114">
       <c r="C114" s="3" t="n">
         <v>29.02</v>
       </c>
+      <c r="D114" s="3" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115">
       <c r="C115" s="3" t="n">
         <v>3508.68</v>
+      </c>
+      <c r="D115" s="3" t="n">
+        <v>3503.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-10-27 04:06:49]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,11 @@
           <t>2025/10/23</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2025/10/27</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -452,496 +457,766 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="n">
         <v>63.83</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>64.56</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="n">
         <v>3888.08</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>3991.35</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="3" t="n">
         <v>50.12</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>50.66</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="n">
         <v>5455.21</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>5650.3</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="3" t="n">
         <v>55.88</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>56.49</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="3" t="n">
         <v>4565.79</v>
       </c>
+      <c r="C10" s="3" t="n">
+        <v>4709.92</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="B12" s="3" t="n">
         <v>61.12</v>
       </c>
+      <c r="C12" s="3" t="n">
+        <v>59.32</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="n">
         <v>7057.93</v>
       </c>
+      <c r="C13" s="3" t="n">
+        <v>7360.02</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="B15" s="3" t="n">
         <v>28.25</v>
       </c>
+      <c r="C15" s="3" t="n">
+        <v>29.82</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="3" t="n">
         <v>2664.94</v>
       </c>
+      <c r="C16" s="3" t="n">
+        <v>2748.84</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="B18" s="3" t="n">
         <v>95.54000000000001</v>
       </c>
+      <c r="C18" s="3" t="n">
+        <v>96.93000000000001</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="3" t="n">
         <v>6699.4</v>
       </c>
+      <c r="C19" s="3" t="n">
+        <v>6791.69</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="B21" s="3" t="n">
         <v>67.68000000000001</v>
       </c>
+      <c r="C21" s="3" t="n">
+        <v>66.84</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="3" t="n">
         <v>84426.34</v>
       </c>
+      <c r="C22" s="3" t="n">
+        <v>84394.91</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="B24" s="3" t="n">
         <v>86.75</v>
       </c>
+      <c r="C24" s="3" t="n">
+        <v>85.68000000000001</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="3" t="n">
         <v>19909.14</v>
       </c>
+      <c r="C25" s="3" t="n">
+        <v>19909.14</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="3" t="n">
         <v>78.48</v>
       </c>
+      <c r="C27" s="3" t="n">
+        <v>78.48999999999999</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="3" t="n">
         <v>39894.54</v>
       </c>
+      <c r="C28" s="3" t="n">
+        <v>39894.54</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="3" t="n">
         <v>57.91</v>
       </c>
+      <c r="C30" s="3" t="n">
+        <v>58.08</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="3" t="n">
         <v>5674.78</v>
       </c>
+      <c r="C31" s="3" t="n">
+        <v>5692.72</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="1" t="n"/>
+      <c r="C32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="3" t="n">
         <v>9.93</v>
       </c>
+      <c r="C33" s="3" t="n">
+        <v>10.55</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="3" t="n">
         <v>33256.2</v>
       </c>
+      <c r="C34" s="3" t="n">
+        <v>33846.15</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="1" t="n"/>
+      <c r="C35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="3" t="n">
         <v>30.26</v>
       </c>
+      <c r="C36" s="3" t="n">
+        <v>31.82</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="3" t="n">
         <v>3195.67</v>
       </c>
+      <c r="C37" s="3" t="n">
+        <v>3416.8</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" s="1" t="n"/>
+      <c r="C38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="B39" s="3" t="n">
         <v>48.97</v>
       </c>
+      <c r="C39" s="3" t="n">
+        <v>50.56</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" s="3" t="n">
         <v>3025.58</v>
       </c>
+      <c r="C40" s="3" t="n">
+        <v>3220.52</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" s="1" t="n"/>
+      <c r="C41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="B42" s="3" t="n">
         <v>19.37</v>
       </c>
+      <c r="C42" s="3" t="n">
+        <v>19.54</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="3" t="n">
         <v>7317.21</v>
       </c>
+      <c r="C43" s="3" t="n">
+        <v>7479.65</v>
+      </c>
     </row>
     <row r="44">
       <c r="B44" s="1" t="n"/>
+      <c r="C44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="B45" s="3" t="n">
         <v>32.25</v>
       </c>
+      <c r="C45" s="3" t="n">
+        <v>32.67</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" s="3" t="n">
         <v>8933.799999999999</v>
       </c>
+      <c r="C46" s="3" t="n">
+        <v>9169.4</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="1" t="n"/>
+      <c r="C47" s="1" t="n"/>
     </row>
     <row r="48">
       <c r="B48" s="3" t="n">
         <v>10.19</v>
       </c>
+      <c r="C48" s="3" t="n">
+        <v>10.3</v>
+      </c>
     </row>
     <row r="49">
       <c r="B49" s="3" t="n">
         <v>12906</v>
       </c>
+      <c r="C49" s="3" t="n">
+        <v>13068.87</v>
+      </c>
     </row>
     <row r="50">
       <c r="B50" s="1" t="n"/>
+      <c r="C50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="B51" s="3" t="n">
         <v>23.87</v>
       </c>
+      <c r="C51" s="3" t="n">
+        <v>24.78</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="3" t="n">
         <v>12376.22</v>
       </c>
+      <c r="C52" s="3" t="n">
+        <v>12608.52</v>
+      </c>
     </row>
     <row r="53">
       <c r="B53" s="1" t="n"/>
+      <c r="C53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="B54" s="3" t="n">
         <v>18.8</v>
       </c>
+      <c r="C54" s="3" t="n">
+        <v>18.23</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" s="3" t="n">
         <v>9711.889999999999</v>
       </c>
+      <c r="C55" s="3" t="n">
+        <v>9609.889999999999</v>
+      </c>
     </row>
     <row r="56">
       <c r="B56" s="1" t="n"/>
+      <c r="C56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="B57" s="3" t="n">
         <v>25.38</v>
       </c>
+      <c r="C57" s="3" t="n">
+        <v>24.89</v>
+      </c>
     </row>
     <row r="58">
       <c r="B58" s="3" t="n">
         <v>16079.06</v>
       </c>
+      <c r="C58" s="3" t="n">
+        <v>16097.1</v>
+      </c>
     </row>
     <row r="59">
       <c r="B59" s="1" t="n"/>
+      <c r="C59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="B60" s="3" t="n">
         <v>33.05</v>
       </c>
+      <c r="C60" s="3" t="n">
+        <v>32.88</v>
+      </c>
     </row>
     <row r="61">
       <c r="B61" s="3" t="n">
         <v>17526.85</v>
       </c>
+      <c r="C61" s="3" t="n">
+        <v>17526.85</v>
+      </c>
     </row>
     <row r="62">
       <c r="B62" s="1" t="n"/>
+      <c r="C62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="B63" s="3" t="n">
         <v>20.79</v>
       </c>
+      <c r="C63" s="3" t="n">
+        <v>21.55</v>
+      </c>
     </row>
     <row r="64">
       <c r="B64" s="3" t="n">
         <v>10218.28</v>
       </c>
+      <c r="C64" s="3" t="n">
+        <v>10670.52</v>
+      </c>
     </row>
     <row r="65">
       <c r="B65" s="1" t="n"/>
+      <c r="C65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="B66" s="3" t="n">
         <v>15.5</v>
       </c>
+      <c r="C66" s="3" t="n">
+        <v>14.64</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" s="3" t="n">
         <v>9838.01</v>
       </c>
+      <c r="C67" s="3" t="n">
+        <v>9831.940000000001</v>
+      </c>
     </row>
     <row r="68">
       <c r="B68" s="1" t="n"/>
+      <c r="C68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="B69" s="3" t="n">
         <v>20.48</v>
       </c>
+      <c r="C69" s="3" t="n">
+        <v>21.39</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" s="3" t="n">
         <v>3120.43</v>
       </c>
+      <c r="C70" s="3" t="n">
+        <v>3286.28</v>
+      </c>
     </row>
     <row r="71">
       <c r="B71" s="1" t="n"/>
+      <c r="C71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="B72" s="3" t="n">
         <v>43.44</v>
       </c>
+      <c r="C72" s="3" t="n">
+        <v>45.06</v>
+      </c>
     </row>
     <row r="73">
       <c r="B73" s="3" t="n">
         <v>5873.33</v>
       </c>
+      <c r="C73" s="3" t="n">
+        <v>6149.34</v>
+      </c>
     </row>
     <row r="74">
       <c r="B74" s="1" t="n"/>
+      <c r="C74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="B75" s="3" t="n">
         <v>29.57</v>
       </c>
+      <c r="C75" s="3" t="n">
+        <v>29.08</v>
+      </c>
     </row>
     <row r="76">
       <c r="B76" s="3" t="n">
         <v>9369.83</v>
       </c>
+      <c r="C76" s="3" t="n">
+        <v>9566.48</v>
+      </c>
     </row>
     <row r="77">
       <c r="B77" s="1" t="n"/>
+      <c r="C77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="B78" s="3" t="n">
         <v>18.43</v>
       </c>
+      <c r="C78" s="3" t="n">
+        <v>18.25</v>
+      </c>
     </row>
     <row r="79">
       <c r="B79" s="3" t="n">
         <v>2449.19</v>
       </c>
+      <c r="C79" s="3" t="n">
+        <v>2473.77</v>
+      </c>
     </row>
     <row r="80">
       <c r="B80" s="1" t="n"/>
+      <c r="C80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="B81" s="3" t="n">
         <v>55.44</v>
       </c>
+      <c r="C81" s="3" t="n">
+        <v>56.1</v>
+      </c>
     </row>
     <row r="82">
       <c r="B82" s="3" t="n">
         <v>2633.89</v>
       </c>
+      <c r="C82" s="3" t="n">
+        <v>2740.32</v>
+      </c>
     </row>
     <row r="83">
       <c r="B83" s="1" t="n"/>
+      <c r="C83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="B84" s="3" t="n">
         <v>58.79</v>
       </c>
+      <c r="C84" s="3" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85">
       <c r="B85" s="3" t="n">
         <v>2686.54</v>
       </c>
+      <c r="C85" s="3" t="n">
+        <v>2780.47</v>
+      </c>
     </row>
     <row r="86">
       <c r="B86" s="1" t="n"/>
+      <c r="C86" s="1" t="n"/>
     </row>
     <row r="87">
       <c r="B87" s="3" t="n">
         <v>51.34</v>
       </c>
+      <c r="C87" s="3" t="n">
+        <v>52.34</v>
+      </c>
     </row>
     <row r="88">
       <c r="B88" s="3" t="n">
         <v>3763.52</v>
       </c>
+      <c r="C88" s="3" t="n">
+        <v>3897.41</v>
+      </c>
     </row>
     <row r="89">
       <c r="B89" s="1" t="n"/>
+      <c r="C89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="B90" s="3" t="n">
         <v>48.07</v>
       </c>
+      <c r="C90" s="3" t="n">
+        <v>47.73</v>
+      </c>
     </row>
     <row r="91">
       <c r="B91" s="3" t="n">
         <v>2028.54</v>
       </c>
+      <c r="C91" s="3" t="n">
+        <v>2090.12</v>
+      </c>
     </row>
     <row r="92">
       <c r="B92" s="1" t="n"/>
+      <c r="C92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="B93" s="3" t="n">
         <v>27.64</v>
       </c>
+      <c r="C93" s="3" t="n">
+        <v>27.69</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" s="3" t="n">
         <v>13597.06</v>
       </c>
+      <c r="C94" s="3" t="n">
+        <v>13845.15</v>
+      </c>
     </row>
     <row r="95">
       <c r="B95" s="1" t="n"/>
+      <c r="C95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="B96" s="3" t="n">
         <v>88.03</v>
       </c>
+      <c r="C96" s="3" t="n">
+        <v>88.23</v>
+      </c>
     </row>
     <row r="97">
       <c r="B97" s="3" t="n">
         <v>9017.07</v>
       </c>
+      <c r="C97" s="3" t="n">
+        <v>9721.639999999999</v>
+      </c>
     </row>
     <row r="98">
       <c r="B98" s="1" t="n"/>
+      <c r="C98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="B99" s="3" t="n">
         <v>57.9</v>
       </c>
+      <c r="C99" s="3" t="n">
+        <v>58.03</v>
+      </c>
     </row>
     <row r="100">
       <c r="B100" s="3" t="n">
         <v>11891.49</v>
       </c>
+      <c r="C100" s="3" t="n">
+        <v>12453</v>
+      </c>
     </row>
     <row r="101">
       <c r="B101" s="1" t="n"/>
+      <c r="C101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="B102" s="3" t="n">
         <v>3.82</v>
       </c>
+      <c r="C102" s="3" t="n">
+        <v>3.93</v>
+      </c>
     </row>
     <row r="103">
       <c r="B103" s="3" t="n">
         <v>2224.95</v>
       </c>
+      <c r="C103" s="3" t="n">
+        <v>2280.36</v>
+      </c>
     </row>
     <row r="104">
       <c r="B104" s="1" t="n"/>
+      <c r="C104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="B105" s="3" t="n">
         <v>29.7</v>
       </c>
+      <c r="C105" s="3" t="n">
+        <v>30.94</v>
+      </c>
     </row>
     <row r="106">
       <c r="B106" s="3" t="n">
         <v>867.54</v>
       </c>
+      <c r="C106" s="3" t="n">
+        <v>898.88</v>
+      </c>
     </row>
     <row r="107">
       <c r="B107" s="1" t="n"/>
+      <c r="C107" s="1" t="n"/>
     </row>
     <row r="108">
       <c r="B108" s="3" t="n">
         <v>29.64</v>
       </c>
+      <c r="C108" s="3" t="n">
+        <v>29.85</v>
+      </c>
     </row>
     <row r="109">
       <c r="B109" s="3" t="n">
         <v>2648.75</v>
       </c>
+      <c r="C109" s="3" t="n">
+        <v>2793.75</v>
+      </c>
     </row>
     <row r="110">
       <c r="B110" s="1" t="n"/>
+      <c r="C110" s="1" t="n"/>
     </row>
     <row r="111">
       <c r="B111" s="3" t="n">
         <v>20.69</v>
       </c>
+      <c r="C111" s="3" t="n">
+        <v>20.63</v>
+      </c>
     </row>
     <row r="112">
       <c r="B112" s="3" t="n">
         <v>4021</v>
       </c>
+      <c r="C112" s="3" t="n">
+        <v>4083.23</v>
+      </c>
     </row>
     <row r="113">
       <c r="B113" s="1" t="n"/>
+      <c r="C113" s="1" t="n"/>
     </row>
     <row r="114">
       <c r="B114" s="3" t="n">
         <v>29.02</v>
       </c>
+      <c r="C114" s="3" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115">
       <c r="B115" s="3" t="n">
         <v>3442.88</v>
+      </c>
+      <c r="C115" s="3" t="n">
+        <v>3463.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-10-30 03:57:36]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,11 @@
           <t>2025/10/27</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2025/10/30</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -462,6 +467,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="n">
@@ -470,6 +480,9 @@
       <c r="C3" s="3" t="n">
         <v>64.56</v>
       </c>
+      <c r="D3" s="3" t="n">
+        <v>64.75</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="n">
@@ -478,10 +491,14 @@
       <c r="C4" s="3" t="n">
         <v>3991.35</v>
       </c>
+      <c r="D4" s="3" t="n">
+        <v>4018.86</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="3" t="n">
@@ -490,6 +507,9 @@
       <c r="C6" s="3" t="n">
         <v>50.66</v>
       </c>
+      <c r="D6" s="3" t="n">
+        <v>50.68</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="n">
@@ -498,10 +518,14 @@
       <c r="C7" s="3" t="n">
         <v>5650.3</v>
       </c>
+      <c r="D7" s="3" t="n">
+        <v>5706.14</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="3" t="n">
@@ -510,6 +534,9 @@
       <c r="C9" s="3" t="n">
         <v>56.49</v>
       </c>
+      <c r="D9" s="3" t="n">
+        <v>56.62</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="3" t="n">
@@ -518,10 +545,14 @@
       <c r="C10" s="3" t="n">
         <v>4709.92</v>
       </c>
+      <c r="D10" s="3" t="n">
+        <v>4754.15</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="B12" s="3" t="n">
@@ -530,6 +561,9 @@
       <c r="C12" s="3" t="n">
         <v>59.32</v>
       </c>
+      <c r="D12" s="3" t="n">
+        <v>59.23</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="n">
@@ -538,10 +572,14 @@
       <c r="C13" s="3" t="n">
         <v>7360.02</v>
       </c>
+      <c r="D13" s="3" t="n">
+        <v>7457.57</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="B15" s="3" t="n">
@@ -550,6 +588,9 @@
       <c r="C15" s="3" t="n">
         <v>29.82</v>
       </c>
+      <c r="D15" s="3" t="n">
+        <v>30.15</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="3" t="n">
@@ -558,10 +599,14 @@
       <c r="C16" s="3" t="n">
         <v>2748.84</v>
       </c>
+      <c r="D16" s="3" t="n">
+        <v>2764.78</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
+      <c r="D17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="B18" s="3" t="n">
@@ -570,6 +615,9 @@
       <c r="C18" s="3" t="n">
         <v>96.93000000000001</v>
       </c>
+      <c r="D18" s="3" t="n">
+        <v>97.16</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="3" t="n">
@@ -578,10 +626,14 @@
       <c r="C19" s="3" t="n">
         <v>6791.69</v>
       </c>
+      <c r="D19" s="3" t="n">
+        <v>6890.59</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="B21" s="3" t="n">
@@ -590,6 +642,9 @@
       <c r="C21" s="3" t="n">
         <v>66.84</v>
       </c>
+      <c r="D21" s="3" t="n">
+        <v>69.89</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="3" t="n">
@@ -598,10 +653,14 @@
       <c r="C22" s="3" t="n">
         <v>84394.91</v>
       </c>
+      <c r="D22" s="3" t="n">
+        <v>84750.89999999999</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="B24" s="3" t="n">
@@ -610,6 +669,9 @@
       <c r="C24" s="3" t="n">
         <v>85.68000000000001</v>
       </c>
+      <c r="D24" s="3" t="n">
+        <v>85.89</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="3" t="n">
@@ -618,10 +680,14 @@
       <c r="C25" s="3" t="n">
         <v>19909.14</v>
       </c>
+      <c r="D25" s="3" t="n">
+        <v>19909.14</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="3" t="n">
@@ -630,6 +696,9 @@
       <c r="C27" s="3" t="n">
         <v>78.48999999999999</v>
       </c>
+      <c r="D27" s="3" t="n">
+        <v>79.73999999999999</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="3" t="n">
@@ -638,10 +707,14 @@
       <c r="C28" s="3" t="n">
         <v>39894.54</v>
       </c>
+      <c r="D28" s="3" t="n">
+        <v>39894.54</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="1" t="n"/>
       <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="3" t="n">
@@ -650,6 +723,9 @@
       <c r="C30" s="3" t="n">
         <v>58.08</v>
       </c>
+      <c r="D30" s="3" t="n">
+        <v>57.7</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="3" t="n">
@@ -658,10 +734,14 @@
       <c r="C31" s="3" t="n">
         <v>5692.72</v>
       </c>
+      <c r="D31" s="3" t="n">
+        <v>5662.42</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="1" t="n"/>
       <c r="C32" s="1" t="n"/>
+      <c r="D32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="3" t="n">
@@ -670,6 +750,9 @@
       <c r="C33" s="3" t="n">
         <v>10.55</v>
       </c>
+      <c r="D33" s="3" t="n">
+        <v>9.779999999999999</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="3" t="n">
@@ -678,10 +761,14 @@
       <c r="C34" s="3" t="n">
         <v>33846.15</v>
       </c>
+      <c r="D34" s="3" t="n">
+        <v>33753.61</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="n"/>
+      <c r="D35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="3" t="n">
@@ -690,6 +777,9 @@
       <c r="C36" s="3" t="n">
         <v>31.82</v>
       </c>
+      <c r="D36" s="3" t="n">
+        <v>32.94</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="3" t="n">
@@ -698,10 +788,14 @@
       <c r="C37" s="3" t="n">
         <v>3416.8</v>
       </c>
+      <c r="D37" s="3" t="n">
+        <v>3533.61</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="n"/>
+      <c r="D38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="B39" s="3" t="n">
@@ -710,6 +804,9 @@
       <c r="C39" s="3" t="n">
         <v>50.56</v>
       </c>
+      <c r="D39" s="3" t="n">
+        <v>51.54</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" s="3" t="n">
@@ -718,10 +815,14 @@
       <c r="C40" s="3" t="n">
         <v>3220.52</v>
       </c>
+      <c r="D40" s="3" t="n">
+        <v>3316.64</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" s="1" t="n"/>
       <c r="C41" s="1" t="n"/>
+      <c r="D41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="B42" s="3" t="n">
@@ -730,6 +831,9 @@
       <c r="C42" s="3" t="n">
         <v>19.54</v>
       </c>
+      <c r="D42" s="3" t="n">
+        <v>19.3</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="3" t="n">
@@ -738,10 +842,14 @@
       <c r="C43" s="3" t="n">
         <v>7479.65</v>
       </c>
+      <c r="D43" s="3" t="n">
+        <v>7406.51</v>
+      </c>
     </row>
     <row r="44">
       <c r="B44" s="1" t="n"/>
       <c r="C44" s="1" t="n"/>
+      <c r="D44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="B45" s="3" t="n">
@@ -750,6 +858,9 @@
       <c r="C45" s="3" t="n">
         <v>32.67</v>
       </c>
+      <c r="D45" s="3" t="n">
+        <v>29.98</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" s="3" t="n">
@@ -758,10 +869,14 @@
       <c r="C46" s="3" t="n">
         <v>9169.4</v>
       </c>
+      <c r="D46" s="3" t="n">
+        <v>8946.77</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="1" t="n"/>
       <c r="C47" s="1" t="n"/>
+      <c r="D47" s="1" t="n"/>
     </row>
     <row r="48">
       <c r="B48" s="3" t="n">
@@ -770,6 +885,9 @@
       <c r="C48" s="3" t="n">
         <v>10.3</v>
       </c>
+      <c r="D48" s="3" t="n">
+        <v>10.27</v>
+      </c>
     </row>
     <row r="49">
       <c r="B49" s="3" t="n">
@@ -778,10 +896,14 @@
       <c r="C49" s="3" t="n">
         <v>13068.87</v>
       </c>
+      <c r="D49" s="3" t="n">
+        <v>13108.84</v>
+      </c>
     </row>
     <row r="50">
       <c r="B50" s="1" t="n"/>
       <c r="C50" s="1" t="n"/>
+      <c r="D50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="B51" s="3" t="n">
@@ -790,6 +912,9 @@
       <c r="C51" s="3" t="n">
         <v>24.78</v>
       </c>
+      <c r="D51" s="3" t="n">
+        <v>26.07</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="3" t="n">
@@ -798,10 +923,14 @@
       <c r="C52" s="3" t="n">
         <v>12608.52</v>
       </c>
+      <c r="D52" s="3" t="n">
+        <v>12740.21</v>
+      </c>
     </row>
     <row r="53">
       <c r="B53" s="1" t="n"/>
       <c r="C53" s="1" t="n"/>
+      <c r="D53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="B54" s="3" t="n">
@@ -810,6 +939,9 @@
       <c r="C54" s="3" t="n">
         <v>18.23</v>
       </c>
+      <c r="D54" s="3" t="n">
+        <v>17.84</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" s="3" t="n">
@@ -818,10 +950,14 @@
       <c r="C55" s="3" t="n">
         <v>9609.889999999999</v>
       </c>
+      <c r="D55" s="3" t="n">
+        <v>9661.34</v>
+      </c>
     </row>
     <row r="56">
       <c r="B56" s="1" t="n"/>
       <c r="C56" s="1" t="n"/>
+      <c r="D56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="B57" s="3" t="n">
@@ -830,6 +966,9 @@
       <c r="C57" s="3" t="n">
         <v>24.89</v>
       </c>
+      <c r="D57" s="3" t="n">
+        <v>24.54</v>
+      </c>
     </row>
     <row r="58">
       <c r="B58" s="3" t="n">
@@ -838,10 +977,14 @@
       <c r="C58" s="3" t="n">
         <v>16097.1</v>
       </c>
+      <c r="D58" s="3" t="n">
+        <v>16052.78</v>
+      </c>
     </row>
     <row r="59">
       <c r="B59" s="1" t="n"/>
       <c r="C59" s="1" t="n"/>
+      <c r="D59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="B60" s="3" t="n">
@@ -850,6 +993,9 @@
       <c r="C60" s="3" t="n">
         <v>32.88</v>
       </c>
+      <c r="D60" s="3" t="n">
+        <v>32.08</v>
+      </c>
     </row>
     <row r="61">
       <c r="B61" s="3" t="n">
@@ -858,10 +1004,14 @@
       <c r="C61" s="3" t="n">
         <v>17526.85</v>
       </c>
+      <c r="D61" s="3" t="n">
+        <v>17526.85</v>
+      </c>
     </row>
     <row r="62">
       <c r="B62" s="1" t="n"/>
       <c r="C62" s="1" t="n"/>
+      <c r="D62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="B63" s="3" t="n">
@@ -870,6 +1020,9 @@
       <c r="C63" s="3" t="n">
         <v>21.55</v>
       </c>
+      <c r="D63" s="3" t="n">
+        <v>21.85</v>
+      </c>
     </row>
     <row r="64">
       <c r="B64" s="3" t="n">
@@ -878,10 +1031,14 @@
       <c r="C64" s="3" t="n">
         <v>10670.52</v>
       </c>
+      <c r="D64" s="3" t="n">
+        <v>10691.52</v>
+      </c>
     </row>
     <row r="65">
       <c r="B65" s="1" t="n"/>
       <c r="C65" s="1" t="n"/>
+      <c r="D65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="B66" s="3" t="n">
@@ -890,6 +1047,9 @@
       <c r="C66" s="3" t="n">
         <v>14.64</v>
       </c>
+      <c r="D66" s="3" t="n">
+        <v>15.52</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" s="3" t="n">
@@ -898,10 +1058,14 @@
       <c r="C67" s="3" t="n">
         <v>9831.940000000001</v>
       </c>
+      <c r="D67" s="3" t="n">
+        <v>9778.9</v>
+      </c>
     </row>
     <row r="68">
       <c r="B68" s="1" t="n"/>
       <c r="C68" s="1" t="n"/>
+      <c r="D68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="B69" s="3" t="n">
@@ -910,6 +1074,9 @@
       <c r="C69" s="3" t="n">
         <v>21.39</v>
       </c>
+      <c r="D69" s="3" t="n">
+        <v>21.86</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" s="3" t="n">
@@ -918,10 +1085,14 @@
       <c r="C70" s="3" t="n">
         <v>3286.28</v>
       </c>
+      <c r="D70" s="3" t="n">
+        <v>3282.42</v>
+      </c>
     </row>
     <row r="71">
       <c r="B71" s="1" t="n"/>
       <c r="C71" s="1" t="n"/>
+      <c r="D71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="B72" s="3" t="n">
@@ -930,6 +1101,9 @@
       <c r="C72" s="3" t="n">
         <v>45.06</v>
       </c>
+      <c r="D72" s="3" t="n">
+        <v>45.56</v>
+      </c>
     </row>
     <row r="73">
       <c r="B73" s="3" t="n">
@@ -938,10 +1112,14 @@
       <c r="C73" s="3" t="n">
         <v>6149.34</v>
       </c>
+      <c r="D73" s="3" t="n">
+        <v>6109.78</v>
+      </c>
     </row>
     <row r="74">
       <c r="B74" s="1" t="n"/>
       <c r="C74" s="1" t="n"/>
+      <c r="D74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="B75" s="3" t="n">
@@ -950,6 +1128,9 @@
       <c r="C75" s="3" t="n">
         <v>29.08</v>
       </c>
+      <c r="D75" s="3" t="n">
+        <v>27.83</v>
+      </c>
     </row>
     <row r="76">
       <c r="B76" s="3" t="n">
@@ -958,10 +1139,14 @@
       <c r="C76" s="3" t="n">
         <v>9566.48</v>
       </c>
+      <c r="D76" s="3" t="n">
+        <v>9408.66</v>
+      </c>
     </row>
     <row r="77">
       <c r="B77" s="1" t="n"/>
       <c r="C77" s="1" t="n"/>
+      <c r="D77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="B78" s="3" t="n">
@@ -970,6 +1155,9 @@
       <c r="C78" s="3" t="n">
         <v>18.25</v>
       </c>
+      <c r="D78" s="3" t="n">
+        <v>18.93</v>
+      </c>
     </row>
     <row r="79">
       <c r="B79" s="3" t="n">
@@ -978,10 +1166,14 @@
       <c r="C79" s="3" t="n">
         <v>2473.77</v>
       </c>
+      <c r="D79" s="3" t="n">
+        <v>2504.5</v>
+      </c>
     </row>
     <row r="80">
       <c r="B80" s="1" t="n"/>
       <c r="C80" s="1" t="n"/>
+      <c r="D80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="B81" s="3" t="n">
@@ -990,6 +1182,9 @@
       <c r="C81" s="3" t="n">
         <v>56.1</v>
       </c>
+      <c r="D81" s="3" t="n">
+        <v>55.61</v>
+      </c>
     </row>
     <row r="82">
       <c r="B82" s="3" t="n">
@@ -998,10 +1193,14 @@
       <c r="C82" s="3" t="n">
         <v>2740.32</v>
       </c>
+      <c r="D82" s="3" t="n">
+        <v>2961.7</v>
+      </c>
     </row>
     <row r="83">
       <c r="B83" s="1" t="n"/>
       <c r="C83" s="1" t="n"/>
+      <c r="D83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="B84" s="3" t="n">
@@ -1010,6 +1209,9 @@
       <c r="C84" s="3" t="n">
         <v>58.79</v>
       </c>
+      <c r="D84" s="3" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85">
       <c r="B85" s="3" t="n">
@@ -1018,10 +1220,14 @@
       <c r="C85" s="3" t="n">
         <v>2780.47</v>
       </c>
+      <c r="D85" s="3" t="n">
+        <v>3030.02</v>
+      </c>
     </row>
     <row r="86">
       <c r="B86" s="1" t="n"/>
       <c r="C86" s="1" t="n"/>
+      <c r="D86" s="1" t="n"/>
     </row>
     <row r="87">
       <c r="B87" s="3" t="n">
@@ -1030,6 +1236,9 @@
       <c r="C87" s="3" t="n">
         <v>52.34</v>
       </c>
+      <c r="D87" s="3" t="n">
+        <v>52.77</v>
+      </c>
     </row>
     <row r="88">
       <c r="B88" s="3" t="n">
@@ -1038,10 +1247,14 @@
       <c r="C88" s="3" t="n">
         <v>3897.41</v>
       </c>
+      <c r="D88" s="3" t="n">
+        <v>4127.88</v>
+      </c>
     </row>
     <row r="89">
       <c r="B89" s="1" t="n"/>
       <c r="C89" s="1" t="n"/>
+      <c r="D89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="B90" s="3" t="n">
@@ -1050,6 +1263,9 @@
       <c r="C90" s="3" t="n">
         <v>47.73</v>
       </c>
+      <c r="D90" s="3" t="n">
+        <v>45.41</v>
+      </c>
     </row>
     <row r="91">
       <c r="B91" s="3" t="n">
@@ -1058,10 +1274,14 @@
       <c r="C91" s="3" t="n">
         <v>2090.12</v>
       </c>
+      <c r="D91" s="3" t="n">
+        <v>2047.92</v>
+      </c>
     </row>
     <row r="92">
       <c r="B92" s="1" t="n"/>
       <c r="C92" s="1" t="n"/>
+      <c r="D92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="B93" s="3" t="n">
@@ -1070,6 +1290,9 @@
       <c r="C93" s="3" t="n">
         <v>27.69</v>
       </c>
+      <c r="D93" s="3" t="n">
+        <v>27.82</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" s="3" t="n">
@@ -1078,10 +1301,14 @@
       <c r="C94" s="3" t="n">
         <v>13845.15</v>
       </c>
+      <c r="D94" s="3" t="n">
+        <v>13755.79</v>
+      </c>
     </row>
     <row r="95">
       <c r="B95" s="1" t="n"/>
       <c r="C95" s="1" t="n"/>
+      <c r="D95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="B96" s="3" t="n">
@@ -1090,6 +1317,9 @@
       <c r="C96" s="3" t="n">
         <v>88.23</v>
       </c>
+      <c r="D96" s="3" t="n">
+        <v>87.84999999999999</v>
+      </c>
     </row>
     <row r="97">
       <c r="B97" s="3" t="n">
@@ -1098,10 +1328,14 @@
       <c r="C97" s="3" t="n">
         <v>9721.639999999999</v>
       </c>
+      <c r="D97" s="3" t="n">
+        <v>9687.620000000001</v>
+      </c>
     </row>
     <row r="98">
       <c r="B98" s="1" t="n"/>
       <c r="C98" s="1" t="n"/>
+      <c r="D98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="B99" s="3" t="n">
@@ -1110,6 +1344,9 @@
       <c r="C99" s="3" t="n">
         <v>58.03</v>
       </c>
+      <c r="D99" s="3" t="n">
+        <v>56.79</v>
+      </c>
     </row>
     <row r="100">
       <c r="B100" s="3" t="n">
@@ -1118,10 +1355,14 @@
       <c r="C100" s="3" t="n">
         <v>12453</v>
       </c>
+      <c r="D100" s="3" t="n">
+        <v>12602.02</v>
+      </c>
     </row>
     <row r="101">
       <c r="B101" s="1" t="n"/>
       <c r="C101" s="1" t="n"/>
+      <c r="D101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="B102" s="3" t="n">
@@ -1130,6 +1371,9 @@
       <c r="C102" s="3" t="n">
         <v>3.93</v>
       </c>
+      <c r="D102" s="3" t="n">
+        <v>4.4</v>
+      </c>
     </row>
     <row r="103">
       <c r="B103" s="3" t="n">
@@ -1138,10 +1382,14 @@
       <c r="C103" s="3" t="n">
         <v>2280.36</v>
       </c>
+      <c r="D103" s="3" t="n">
+        <v>2258.48</v>
+      </c>
     </row>
     <row r="104">
       <c r="B104" s="1" t="n"/>
       <c r="C104" s="1" t="n"/>
+      <c r="D104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="B105" s="3" t="n">
@@ -1150,6 +1398,9 @@
       <c r="C105" s="3" t="n">
         <v>30.94</v>
       </c>
+      <c r="D105" s="3" t="n">
+        <v>30.64</v>
+      </c>
     </row>
     <row r="106">
       <c r="B106" s="3" t="n">
@@ -1158,10 +1409,14 @@
       <c r="C106" s="3" t="n">
         <v>898.88</v>
       </c>
+      <c r="D106" s="3" t="n">
+        <v>903.78</v>
+      </c>
     </row>
     <row r="107">
       <c r="B107" s="1" t="n"/>
       <c r="C107" s="1" t="n"/>
+      <c r="D107" s="1" t="n"/>
     </row>
     <row r="108">
       <c r="B108" s="3" t="n">
@@ -1170,6 +1425,9 @@
       <c r="C108" s="3" t="n">
         <v>29.85</v>
       </c>
+      <c r="D108" s="3" t="n">
+        <v>29.68</v>
+      </c>
     </row>
     <row r="109">
       <c r="B109" s="3" t="n">
@@ -1178,10 +1436,14 @@
       <c r="C109" s="3" t="n">
         <v>2793.75</v>
       </c>
+      <c r="D109" s="3" t="n">
+        <v>2880.9</v>
+      </c>
     </row>
     <row r="110">
       <c r="B110" s="1" t="n"/>
       <c r="C110" s="1" t="n"/>
+      <c r="D110" s="1" t="n"/>
     </row>
     <row r="111">
       <c r="B111" s="3" t="n">
@@ -1190,6 +1452,9 @@
       <c r="C111" s="3" t="n">
         <v>20.63</v>
       </c>
+      <c r="D111" s="3" t="n">
+        <v>20.55</v>
+      </c>
     </row>
     <row r="112">
       <c r="B112" s="3" t="n">
@@ -1198,10 +1463,14 @@
       <c r="C112" s="3" t="n">
         <v>4083.23</v>
       </c>
+      <c r="D112" s="3" t="n">
+        <v>4055.81</v>
+      </c>
     </row>
     <row r="113">
       <c r="B113" s="1" t="n"/>
       <c r="C113" s="1" t="n"/>
+      <c r="D113" s="1" t="n"/>
     </row>
     <row r="114">
       <c r="B114" s="3" t="n">
@@ -1210,6 +1479,9 @@
       <c r="C114" s="3" t="n">
         <v>29.02</v>
       </c>
+      <c r="D114" s="3" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115">
       <c r="B115" s="3" t="n">
@@ -1217,6 +1489,9 @@
       </c>
       <c r="C115" s="3" t="n">
         <v>3463.09</v>
+      </c>
+      <c r="D115" s="3" t="n">
+        <v>3402.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-03 04:04:47]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,11 @@
           <t>2025/10/30</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/03</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -472,6 +477,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="n">
@@ -483,6 +493,9 @@
       <c r="D3" s="3" t="n">
         <v>64.75</v>
       </c>
+      <c r="E3" s="3" t="n">
+        <v>62.24</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="n">
@@ -493,12 +506,16 @@
       </c>
       <c r="D4" s="3" t="n">
         <v>4018.86</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>3956.72</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="3" t="n">
@@ -510,6 +527,9 @@
       <c r="D6" s="3" t="n">
         <v>50.68</v>
       </c>
+      <c r="E6" s="3" t="n">
+        <v>49.02</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="n">
@@ -520,12 +540,16 @@
       </c>
       <c r="D7" s="3" t="n">
         <v>5706.14</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>5545.87</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="3" t="n">
@@ -537,6 +561,9 @@
       <c r="D9" s="3" t="n">
         <v>56.62</v>
       </c>
+      <c r="E9" s="3" t="n">
+        <v>53.94</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="3" t="n">
@@ -547,12 +574,16 @@
       </c>
       <c r="D10" s="3" t="n">
         <v>4754.15</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>4619.67</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n"/>
+      <c r="E11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="B12" s="3" t="n">
@@ -564,6 +595,9 @@
       <c r="D12" s="3" t="n">
         <v>59.23</v>
       </c>
+      <c r="E12" s="3" t="n">
+        <v>57.54</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="n">
@@ -574,12 +608,16 @@
       </c>
       <c r="D13" s="3" t="n">
         <v>7457.57</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>7255.42</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n"/>
+      <c r="E14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="B15" s="3" t="n">
@@ -591,6 +629,9 @@
       <c r="D15" s="3" t="n">
         <v>30.15</v>
       </c>
+      <c r="E15" s="3" t="n">
+        <v>26.75</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="3" t="n">
@@ -601,12 +642,16 @@
       </c>
       <c r="D16" s="3" t="n">
         <v>2764.78</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>2699.03</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="B18" s="3" t="n">
@@ -618,6 +663,9 @@
       <c r="D18" s="3" t="n">
         <v>97.16</v>
       </c>
+      <c r="E18" s="3" t="n">
+        <v>96.63</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="3" t="n">
@@ -628,12 +676,16 @@
       </c>
       <c r="D19" s="3" t="n">
         <v>6890.59</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>6840.2</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="B21" s="3" t="n">
@@ -645,6 +697,9 @@
       <c r="D21" s="3" t="n">
         <v>69.89</v>
       </c>
+      <c r="E21" s="3" t="n">
+        <v>65.76000000000001</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="3" t="n">
@@ -655,12 +710,16 @@
       </c>
       <c r="D22" s="3" t="n">
         <v>84750.89999999999</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>83935.38</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="B24" s="3" t="n">
@@ -672,6 +731,9 @@
       <c r="D24" s="3" t="n">
         <v>85.89</v>
       </c>
+      <c r="E24" s="3" t="n">
+        <v>85.7</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="3" t="n">
@@ -681,6 +743,9 @@
         <v>19909.14</v>
       </c>
       <c r="D25" s="3" t="n">
+        <v>19909.14</v>
+      </c>
+      <c r="E25" s="3" t="n">
         <v>19909.14</v>
       </c>
     </row>
@@ -688,6 +753,7 @@
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="n"/>
       <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="3" t="n">
@@ -699,6 +765,9 @@
       <c r="D27" s="3" t="n">
         <v>79.73999999999999</v>
       </c>
+      <c r="E27" s="3" t="n">
+        <v>83.77</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="3" t="n">
@@ -708,6 +777,9 @@
         <v>39894.54</v>
       </c>
       <c r="D28" s="3" t="n">
+        <v>39894.54</v>
+      </c>
+      <c r="E28" s="3" t="n">
         <v>39894.54</v>
       </c>
     </row>
@@ -715,6 +787,7 @@
       <c r="B29" s="1" t="n"/>
       <c r="C29" s="1" t="n"/>
       <c r="D29" s="1" t="n"/>
+      <c r="E29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="3" t="n">
@@ -726,6 +799,9 @@
       <c r="D30" s="3" t="n">
         <v>57.7</v>
       </c>
+      <c r="E30" s="3" t="n">
+        <v>57.46</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="3" t="n">
@@ -736,12 +812,16 @@
       </c>
       <c r="D31" s="3" t="n">
         <v>5662.42</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>5665.89</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="1" t="n"/>
       <c r="C32" s="1" t="n"/>
       <c r="D32" s="1" t="n"/>
+      <c r="E32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="3" t="n">
@@ -753,6 +833,9 @@
       <c r="D33" s="3" t="n">
         <v>9.779999999999999</v>
       </c>
+      <c r="E33" s="3" t="n">
+        <v>11.77</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="3" t="n">
@@ -763,12 +846,16 @@
       </c>
       <c r="D34" s="3" t="n">
         <v>33753.61</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>33010.92</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="n"/>
       <c r="D35" s="1" t="n"/>
+      <c r="E35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="3" t="n">
@@ -780,6 +867,9 @@
       <c r="D36" s="3" t="n">
         <v>32.94</v>
       </c>
+      <c r="E36" s="3" t="n">
+        <v>28.98</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="3" t="n">
@@ -790,12 +880,16 @@
       </c>
       <c r="D37" s="3" t="n">
         <v>3533.61</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>3321.04</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="n"/>
       <c r="D38" s="1" t="n"/>
+      <c r="E38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="B39" s="3" t="n">
@@ -807,6 +901,9 @@
       <c r="D39" s="3" t="n">
         <v>51.54</v>
       </c>
+      <c r="E39" s="3" t="n">
+        <v>47.3</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" s="3" t="n">
@@ -817,12 +914,16 @@
       </c>
       <c r="D40" s="3" t="n">
         <v>3316.64</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>3143.95</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="1" t="n"/>
       <c r="C41" s="1" t="n"/>
       <c r="D41" s="1" t="n"/>
+      <c r="E41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="B42" s="3" t="n">
@@ -834,6 +935,9 @@
       <c r="D42" s="3" t="n">
         <v>19.3</v>
       </c>
+      <c r="E42" s="3" t="n">
+        <v>19.05</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="3" t="n">
@@ -844,12 +948,16 @@
       </c>
       <c r="D43" s="3" t="n">
         <v>7406.51</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>7354.49</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="1" t="n"/>
       <c r="C44" s="1" t="n"/>
       <c r="D44" s="1" t="n"/>
+      <c r="E44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="B45" s="3" t="n">
@@ -861,6 +969,9 @@
       <c r="D45" s="3" t="n">
         <v>29.98</v>
       </c>
+      <c r="E45" s="3" t="n">
+        <v>32.5</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" s="3" t="n">
@@ -871,12 +982,16 @@
       </c>
       <c r="D46" s="3" t="n">
         <v>8946.77</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>8889.860000000001</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="1" t="n"/>
       <c r="C47" s="1" t="n"/>
       <c r="D47" s="1" t="n"/>
+      <c r="E47" s="1" t="n"/>
     </row>
     <row r="48">
       <c r="B48" s="3" t="n">
@@ -888,6 +1003,9 @@
       <c r="D48" s="3" t="n">
         <v>10.27</v>
       </c>
+      <c r="E48" s="3" t="n">
+        <v>13.2</v>
+      </c>
     </row>
     <row r="49">
       <c r="B49" s="3" t="n">
@@ -898,12 +1016,16 @@
       </c>
       <c r="D49" s="3" t="n">
         <v>13108.84</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>12997.93</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="1" t="n"/>
       <c r="C50" s="1" t="n"/>
       <c r="D50" s="1" t="n"/>
+      <c r="E50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="B51" s="3" t="n">
@@ -915,6 +1037,9 @@
       <c r="D51" s="3" t="n">
         <v>26.07</v>
       </c>
+      <c r="E51" s="3" t="n">
+        <v>24.96</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="3" t="n">
@@ -925,12 +1050,16 @@
       </c>
       <c r="D52" s="3" t="n">
         <v>12740.21</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>12426.7</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="1" t="n"/>
       <c r="C53" s="1" t="n"/>
       <c r="D53" s="1" t="n"/>
+      <c r="E53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="B54" s="3" t="n">
@@ -942,6 +1071,9 @@
       <c r="D54" s="3" t="n">
         <v>17.84</v>
       </c>
+      <c r="E54" s="3" t="n">
+        <v>21.45</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" s="3" t="n">
@@ -952,12 +1084,16 @@
       </c>
       <c r="D55" s="3" t="n">
         <v>9661.34</v>
+      </c>
+      <c r="E55" s="3" t="n">
+        <v>9784.74</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="1" t="n"/>
       <c r="C56" s="1" t="n"/>
       <c r="D56" s="1" t="n"/>
+      <c r="E56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="B57" s="3" t="n">
@@ -969,6 +1105,9 @@
       <c r="D57" s="3" t="n">
         <v>24.54</v>
       </c>
+      <c r="E57" s="3" t="n">
+        <v>26.77</v>
+      </c>
     </row>
     <row r="58">
       <c r="B58" s="3" t="n">
@@ -979,12 +1118,16 @@
       </c>
       <c r="D58" s="3" t="n">
         <v>16052.78</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>16111.26</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" s="1" t="n"/>
       <c r="C59" s="1" t="n"/>
       <c r="D59" s="1" t="n"/>
+      <c r="E59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="B60" s="3" t="n">
@@ -996,6 +1139,9 @@
       <c r="D60" s="3" t="n">
         <v>32.08</v>
       </c>
+      <c r="E60" s="3" t="n">
+        <v>32.17</v>
+      </c>
     </row>
     <row r="61">
       <c r="B61" s="3" t="n">
@@ -1005,6 +1151,9 @@
         <v>17526.85</v>
       </c>
       <c r="D61" s="3" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="E61" s="3" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1012,6 +1161,7 @@
       <c r="B62" s="1" t="n"/>
       <c r="C62" s="1" t="n"/>
       <c r="D62" s="1" t="n"/>
+      <c r="E62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="B63" s="3" t="n">
@@ -1023,6 +1173,9 @@
       <c r="D63" s="3" t="n">
         <v>21.85</v>
       </c>
+      <c r="E63" s="3" t="n">
+        <v>20.84</v>
+      </c>
     </row>
     <row r="64">
       <c r="B64" s="3" t="n">
@@ -1033,12 +1186,16 @@
       </c>
       <c r="D64" s="3" t="n">
         <v>10691.52</v>
+      </c>
+      <c r="E64" s="3" t="n">
+        <v>10263.12</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" s="1" t="n"/>
       <c r="C65" s="1" t="n"/>
       <c r="D65" s="1" t="n"/>
+      <c r="E65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="B66" s="3" t="n">
@@ -1050,6 +1207,9 @@
       <c r="D66" s="3" t="n">
         <v>15.52</v>
       </c>
+      <c r="E66" s="3" t="n">
+        <v>14.8</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" s="3" t="n">
@@ -1060,12 +1220,16 @@
       </c>
       <c r="D67" s="3" t="n">
         <v>9778.9</v>
+      </c>
+      <c r="E67" s="3" t="n">
+        <v>9907.07</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" s="1" t="n"/>
       <c r="C68" s="1" t="n"/>
       <c r="D68" s="1" t="n"/>
+      <c r="E68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="B69" s="3" t="n">
@@ -1077,6 +1241,9 @@
       <c r="D69" s="3" t="n">
         <v>21.86</v>
       </c>
+      <c r="E69" s="3" t="n">
+        <v>20.88</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" s="3" t="n">
@@ -1087,12 +1254,16 @@
       </c>
       <c r="D70" s="3" t="n">
         <v>3282.42</v>
+      </c>
+      <c r="E70" s="3" t="n">
+        <v>3164.02</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" s="1" t="n"/>
       <c r="C71" s="1" t="n"/>
       <c r="D71" s="1" t="n"/>
+      <c r="E71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="B72" s="3" t="n">
@@ -1104,6 +1275,9 @@
       <c r="D72" s="3" t="n">
         <v>45.56</v>
       </c>
+      <c r="E72" s="3" t="n">
+        <v>43.63</v>
+      </c>
     </row>
     <row r="73">
       <c r="B73" s="3" t="n">
@@ -1114,12 +1288,16 @@
       </c>
       <c r="D73" s="3" t="n">
         <v>6109.78</v>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>5894.12</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" s="1" t="n"/>
       <c r="C74" s="1" t="n"/>
       <c r="D74" s="1" t="n"/>
+      <c r="E74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="B75" s="3" t="n">
@@ -1131,6 +1309,9 @@
       <c r="D75" s="3" t="n">
         <v>27.83</v>
       </c>
+      <c r="E75" s="3" t="n">
+        <v>29.82</v>
+      </c>
     </row>
     <row r="76">
       <c r="B76" s="3" t="n">
@@ -1141,12 +1322,16 @@
       </c>
       <c r="D76" s="3" t="n">
         <v>9408.66</v>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>9444.360000000001</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" s="1" t="n"/>
       <c r="C77" s="1" t="n"/>
       <c r="D77" s="1" t="n"/>
+      <c r="E77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="B78" s="3" t="n">
@@ -1158,6 +1343,9 @@
       <c r="D78" s="3" t="n">
         <v>18.93</v>
       </c>
+      <c r="E78" s="3" t="n">
+        <v>18.01</v>
+      </c>
     </row>
     <row r="79">
       <c r="B79" s="3" t="n">
@@ -1168,12 +1356,16 @@
       </c>
       <c r="D79" s="3" t="n">
         <v>2504.5</v>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>2422.48</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="1" t="n"/>
       <c r="C80" s="1" t="n"/>
       <c r="D80" s="1" t="n"/>
+      <c r="E80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="B81" s="3" t="n">
@@ -1185,6 +1377,9 @@
       <c r="D81" s="3" t="n">
         <v>55.61</v>
       </c>
+      <c r="E81" s="3" t="n">
+        <v>56.06</v>
+      </c>
     </row>
     <row r="82">
       <c r="B82" s="3" t="n">
@@ -1195,12 +1390,16 @@
       </c>
       <c r="D82" s="3" t="n">
         <v>2961.7</v>
+      </c>
+      <c r="E82" s="3" t="n">
+        <v>2851.5</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" s="1" t="n"/>
       <c r="C83" s="1" t="n"/>
       <c r="D83" s="1" t="n"/>
+      <c r="E83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="B84" s="3" t="n">
@@ -1212,6 +1411,9 @@
       <c r="D84" s="3" t="n">
         <v>58.79</v>
       </c>
+      <c r="E84" s="3" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85">
       <c r="B85" s="3" t="n">
@@ -1222,12 +1424,16 @@
       </c>
       <c r="D85" s="3" t="n">
         <v>3030.02</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>2966.57</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" s="1" t="n"/>
       <c r="C86" s="1" t="n"/>
       <c r="D86" s="1" t="n"/>
+      <c r="E86" s="1" t="n"/>
     </row>
     <row r="87">
       <c r="B87" s="3" t="n">
@@ -1239,6 +1445,9 @@
       <c r="D87" s="3" t="n">
         <v>52.77</v>
       </c>
+      <c r="E87" s="3" t="n">
+        <v>52.78</v>
+      </c>
     </row>
     <row r="88">
       <c r="B88" s="3" t="n">
@@ -1249,12 +1458,16 @@
       </c>
       <c r="D88" s="3" t="n">
         <v>4127.88</v>
+      </c>
+      <c r="E88" s="3" t="n">
+        <v>3909.78</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" s="1" t="n"/>
       <c r="C89" s="1" t="n"/>
       <c r="D89" s="1" t="n"/>
+      <c r="E89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="B90" s="3" t="n">
@@ -1266,6 +1479,9 @@
       <c r="D90" s="3" t="n">
         <v>45.41</v>
       </c>
+      <c r="E90" s="3" t="n">
+        <v>47.79</v>
+      </c>
     </row>
     <row r="91">
       <c r="B91" s="3" t="n">
@@ -1276,12 +1492,16 @@
       </c>
       <c r="D91" s="3" t="n">
         <v>2047.92</v>
+      </c>
+      <c r="E91" s="3" t="n">
+        <v>2083.67</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" s="1" t="n"/>
       <c r="C92" s="1" t="n"/>
       <c r="D92" s="1" t="n"/>
+      <c r="E92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="B93" s="3" t="n">
@@ -1293,6 +1513,9 @@
       <c r="D93" s="3" t="n">
         <v>27.82</v>
       </c>
+      <c r="E93" s="3" t="n">
+        <v>28.1</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" s="3" t="n">
@@ -1303,12 +1526,16 @@
       </c>
       <c r="D94" s="3" t="n">
         <v>13755.79</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>13963.26</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" s="1" t="n"/>
       <c r="C95" s="1" t="n"/>
       <c r="D95" s="1" t="n"/>
+      <c r="E95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="B96" s="3" t="n">
@@ -1320,6 +1547,9 @@
       <c r="D96" s="3" t="n">
         <v>87.84999999999999</v>
       </c>
+      <c r="E96" s="3" t="n">
+        <v>86.69</v>
+      </c>
     </row>
     <row r="97">
       <c r="B97" s="3" t="n">
@@ -1330,12 +1560,16 @@
       </c>
       <c r="D97" s="3" t="n">
         <v>9687.620000000001</v>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>8981.85</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" s="1" t="n"/>
       <c r="C98" s="1" t="n"/>
       <c r="D98" s="1" t="n"/>
+      <c r="E98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="B99" s="3" t="n">
@@ -1347,6 +1581,9 @@
       <c r="D99" s="3" t="n">
         <v>56.79</v>
       </c>
+      <c r="E99" s="3" t="n">
+        <v>56.94</v>
+      </c>
     </row>
     <row r="100">
       <c r="B100" s="3" t="n">
@@ -1357,12 +1594,16 @@
       </c>
       <c r="D100" s="3" t="n">
         <v>12602.02</v>
+      </c>
+      <c r="E100" s="3" t="n">
+        <v>12232.61</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" s="1" t="n"/>
       <c r="C101" s="1" t="n"/>
       <c r="D101" s="1" t="n"/>
+      <c r="E101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="B102" s="3" t="n">
@@ -1374,6 +1615,9 @@
       <c r="D102" s="3" t="n">
         <v>4.4</v>
       </c>
+      <c r="E102" s="3" t="n">
+        <v>5.94</v>
+      </c>
     </row>
     <row r="103">
       <c r="B103" s="3" t="n">
@@ -1384,12 +1628,16 @@
       </c>
       <c r="D103" s="3" t="n">
         <v>2258.48</v>
+      </c>
+      <c r="E103" s="3" t="n">
+        <v>2274.27</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" s="1" t="n"/>
       <c r="C104" s="1" t="n"/>
       <c r="D104" s="1" t="n"/>
+      <c r="E104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="B105" s="3" t="n">
@@ -1401,6 +1649,9 @@
       <c r="D105" s="3" t="n">
         <v>30.64</v>
       </c>
+      <c r="E105" s="3" t="n">
+        <v>26.15</v>
+      </c>
     </row>
     <row r="106">
       <c r="B106" s="3" t="n">
@@ -1411,12 +1662,16 @@
       </c>
       <c r="D106" s="3" t="n">
         <v>903.78</v>
+      </c>
+      <c r="E106" s="3" t="n">
+        <v>873.12</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" s="1" t="n"/>
       <c r="C107" s="1" t="n"/>
       <c r="D107" s="1" t="n"/>
+      <c r="E107" s="1" t="n"/>
     </row>
     <row r="108">
       <c r="B108" s="3" t="n">
@@ -1428,6 +1683,9 @@
       <c r="D108" s="3" t="n">
         <v>29.68</v>
       </c>
+      <c r="E108" s="3" t="n">
+        <v>29.58</v>
+      </c>
     </row>
     <row r="109">
       <c r="B109" s="3" t="n">
@@ -1438,12 +1696,16 @@
       </c>
       <c r="D109" s="3" t="n">
         <v>2880.9</v>
+      </c>
+      <c r="E109" s="3" t="n">
+        <v>2734.02</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" s="1" t="n"/>
       <c r="C110" s="1" t="n"/>
       <c r="D110" s="1" t="n"/>
+      <c r="E110" s="1" t="n"/>
     </row>
     <row r="111">
       <c r="B111" s="3" t="n">
@@ -1455,6 +1717,9 @@
       <c r="D111" s="3" t="n">
         <v>20.55</v>
       </c>
+      <c r="E111" s="3" t="n">
+        <v>21.2</v>
+      </c>
     </row>
     <row r="112">
       <c r="B112" s="3" t="n">
@@ -1465,12 +1730,16 @@
       </c>
       <c r="D112" s="3" t="n">
         <v>4055.81</v>
+      </c>
+      <c r="E112" s="3" t="n">
+        <v>3971.97</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" s="1" t="n"/>
       <c r="C113" s="1" t="n"/>
       <c r="D113" s="1" t="n"/>
+      <c r="E113" s="1" t="n"/>
     </row>
     <row r="114">
       <c r="B114" s="3" t="n">
@@ -1482,6 +1751,9 @@
       <c r="D114" s="3" t="n">
         <v>29.02</v>
       </c>
+      <c r="E114" s="3" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115">
       <c r="B115" s="3" t="n">
@@ -1492,6 +1764,9 @@
       </c>
       <c r="D115" s="3" t="n">
         <v>3402.18</v>
+      </c>
+      <c r="E115" s="3" t="n">
+        <v>3358.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-04 01:06:19]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -431,13 +431,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
@@ -460,6 +468,11 @@
           <t>2025/11/03</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/04</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -482,6 +495,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="n">
@@ -496,6 +514,9 @@
       <c r="E3" s="3" t="n">
         <v>62.24</v>
       </c>
+      <c r="F3" s="3" t="n">
+        <v>62.77</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="n">
@@ -509,6 +530,9 @@
       </c>
       <c r="E4" s="3" t="n">
         <v>3956.72</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>3976.52</v>
       </c>
     </row>
     <row r="5">
@@ -516,6 +540,7 @@
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="1" t="n"/>
+      <c r="F5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="3" t="n">
@@ -530,6 +555,9 @@
       <c r="E6" s="3" t="n">
         <v>49.02</v>
       </c>
+      <c r="F6" s="3" t="n">
+        <v>49.3</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="n">
@@ -543,6 +571,9 @@
       </c>
       <c r="E7" s="3" t="n">
         <v>5545.87</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>5594.41</v>
       </c>
     </row>
     <row r="8">
@@ -550,6 +581,7 @@
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="n"/>
       <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="3" t="n">
@@ -564,6 +596,9 @@
       <c r="E9" s="3" t="n">
         <v>53.94</v>
       </c>
+      <c r="F9" s="3" t="n">
+        <v>54.75</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="3" t="n">
@@ -577,6 +612,9 @@
       </c>
       <c r="E10" s="3" t="n">
         <v>4619.67</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>4653.4</v>
       </c>
     </row>
     <row r="11">
@@ -584,6 +622,7 @@
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="1" t="n"/>
+      <c r="F11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="B12" s="3" t="n">
@@ -598,6 +637,9 @@
       <c r="E12" s="3" t="n">
         <v>57.54</v>
       </c>
+      <c r="F12" s="3" t="n">
+        <v>57.54</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="n">
@@ -611,6 +653,9 @@
       </c>
       <c r="E13" s="3" t="n">
         <v>7255.42</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>7333.6</v>
       </c>
     </row>
     <row r="14">
@@ -618,6 +663,7 @@
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n"/>
       <c r="E14" s="1" t="n"/>
+      <c r="F14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="B15" s="3" t="n">
@@ -632,6 +678,9 @@
       <c r="E15" s="3" t="n">
         <v>26.75</v>
       </c>
+      <c r="F15" s="3" t="n">
+        <v>26.75</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="3" t="n">
@@ -645,6 +694,9 @@
       </c>
       <c r="E16" s="3" t="n">
         <v>2699.03</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>2715.84</v>
       </c>
     </row>
     <row r="17">
@@ -652,6 +704,7 @@
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n"/>
       <c r="E17" s="1" t="n"/>
+      <c r="F17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="B18" s="3" t="n">
@@ -666,6 +719,9 @@
       <c r="E18" s="3" t="n">
         <v>96.63</v>
       </c>
+      <c r="F18" s="3" t="n">
+        <v>96.63</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="3" t="n">
@@ -679,6 +735,9 @@
       </c>
       <c r="E19" s="3" t="n">
         <v>6840.2</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>6851.97</v>
       </c>
     </row>
     <row r="20">
@@ -686,6 +745,7 @@
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n"/>
       <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="B21" s="3" t="n">
@@ -700,6 +760,9 @@
       <c r="E21" s="3" t="n">
         <v>65.76000000000001</v>
       </c>
+      <c r="F21" s="3" t="n">
+        <v>65.76000000000001</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="3" t="n">
@@ -713,6 +776,9 @@
       </c>
       <c r="E22" s="3" t="n">
         <v>83935.38</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>83978.49000000001</v>
       </c>
     </row>
     <row r="23">
@@ -720,6 +786,7 @@
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="1" t="n"/>
       <c r="E23" s="1" t="n"/>
+      <c r="F23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="B24" s="3" t="n">
@@ -734,6 +801,9 @@
       <c r="E24" s="3" t="n">
         <v>85.7</v>
       </c>
+      <c r="F24" s="3" t="n">
+        <v>85.7</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="3" t="n">
@@ -746,6 +816,9 @@
         <v>19909.14</v>
       </c>
       <c r="E25" s="3" t="n">
+        <v>19909.14</v>
+      </c>
+      <c r="F25" s="3" t="n">
         <v>19909.14</v>
       </c>
     </row>
@@ -754,6 +827,7 @@
       <c r="C26" s="1" t="n"/>
       <c r="D26" s="1" t="n"/>
       <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="3" t="n">
@@ -768,6 +842,9 @@
       <c r="E27" s="3" t="n">
         <v>83.77</v>
       </c>
+      <c r="F27" s="3" t="n">
+        <v>83.77</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="3" t="n">
@@ -780,6 +857,9 @@
         <v>39894.54</v>
       </c>
       <c r="E28" s="3" t="n">
+        <v>39894.54</v>
+      </c>
+      <c r="F28" s="3" t="n">
         <v>39894.54</v>
       </c>
     </row>
@@ -788,6 +868,7 @@
       <c r="C29" s="1" t="n"/>
       <c r="D29" s="1" t="n"/>
       <c r="E29" s="1" t="n"/>
+      <c r="F29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="3" t="n">
@@ -802,6 +883,9 @@
       <c r="E30" s="3" t="n">
         <v>57.46</v>
       </c>
+      <c r="F30" s="3" t="n">
+        <v>58.13</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="3" t="n">
@@ -815,6 +899,9 @@
       </c>
       <c r="E31" s="3" t="n">
         <v>5665.89</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>5678.43</v>
       </c>
     </row>
     <row r="32">
@@ -822,6 +909,7 @@
       <c r="C32" s="1" t="n"/>
       <c r="D32" s="1" t="n"/>
       <c r="E32" s="1" t="n"/>
+      <c r="F32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="3" t="n">
@@ -836,6 +924,9 @@
       <c r="E33" s="3" t="n">
         <v>11.77</v>
       </c>
+      <c r="F33" s="3" t="n">
+        <v>11.57</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="3" t="n">
@@ -849,6 +940,9 @@
       </c>
       <c r="E34" s="3" t="n">
         <v>33010.92</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>33159.23</v>
       </c>
     </row>
     <row r="35">
@@ -856,6 +950,7 @@
       <c r="C35" s="1" t="n"/>
       <c r="D35" s="1" t="n"/>
       <c r="E35" s="1" t="n"/>
+      <c r="F35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="3" t="n">
@@ -870,6 +965,9 @@
       <c r="E36" s="3" t="n">
         <v>28.98</v>
       </c>
+      <c r="F36" s="3" t="n">
+        <v>29.11</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="3" t="n">
@@ -883,6 +981,9 @@
       </c>
       <c r="E37" s="3" t="n">
         <v>3321.04</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>3381.69</v>
       </c>
     </row>
     <row r="38">
@@ -890,6 +991,7 @@
       <c r="C38" s="1" t="n"/>
       <c r="D38" s="1" t="n"/>
       <c r="E38" s="1" t="n"/>
+      <c r="F38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="B39" s="3" t="n">
@@ -904,6 +1006,9 @@
       <c r="E39" s="3" t="n">
         <v>47.3</v>
       </c>
+      <c r="F39" s="3" t="n">
+        <v>47.4</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" s="3" t="n">
@@ -917,6 +1022,9 @@
       </c>
       <c r="E40" s="3" t="n">
         <v>3143.95</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>3196.87</v>
       </c>
     </row>
     <row r="41">
@@ -924,6 +1032,7 @@
       <c r="C41" s="1" t="n"/>
       <c r="D41" s="1" t="n"/>
       <c r="E41" s="1" t="n"/>
+      <c r="F41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="B42" s="3" t="n">
@@ -938,6 +1047,9 @@
       <c r="E42" s="3" t="n">
         <v>19.05</v>
       </c>
+      <c r="F42" s="3" t="n">
+        <v>18.72</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="3" t="n">
@@ -951,6 +1063,9 @@
       </c>
       <c r="E43" s="3" t="n">
         <v>7354.49</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>7354.02</v>
       </c>
     </row>
     <row r="44">
@@ -958,6 +1073,7 @@
       <c r="C44" s="1" t="n"/>
       <c r="D44" s="1" t="n"/>
       <c r="E44" s="1" t="n"/>
+      <c r="F44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="B45" s="3" t="n">
@@ -972,6 +1088,9 @@
       <c r="E45" s="3" t="n">
         <v>32.5</v>
       </c>
+      <c r="F45" s="3" t="n">
+        <v>31.86</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" s="3" t="n">
@@ -985,6 +1104,9 @@
       </c>
       <c r="E46" s="3" t="n">
         <v>8889.860000000001</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <v>8873.77</v>
       </c>
     </row>
     <row r="47">
@@ -992,6 +1114,7 @@
       <c r="C47" s="1" t="n"/>
       <c r="D47" s="1" t="n"/>
       <c r="E47" s="1" t="n"/>
+      <c r="F47" s="1" t="n"/>
     </row>
     <row r="48">
       <c r="B48" s="3" t="n">
@@ -1006,6 +1129,9 @@
       <c r="E48" s="3" t="n">
         <v>13.2</v>
       </c>
+      <c r="F48" s="3" t="n">
+        <v>13.4</v>
+      </c>
     </row>
     <row r="49">
       <c r="B49" s="3" t="n">
@@ -1019,6 +1145,9 @@
       </c>
       <c r="E49" s="3" t="n">
         <v>12997.93</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>13044.63</v>
       </c>
     </row>
     <row r="50">
@@ -1026,6 +1155,7 @@
       <c r="C50" s="1" t="n"/>
       <c r="D50" s="1" t="n"/>
       <c r="E50" s="1" t="n"/>
+      <c r="F50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="B51" s="3" t="n">
@@ -1040,6 +1170,9 @@
       <c r="E51" s="3" t="n">
         <v>24.96</v>
       </c>
+      <c r="F51" s="3" t="n">
+        <v>24.18</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="3" t="n">
@@ -1053,6 +1186,9 @@
       </c>
       <c r="E52" s="3" t="n">
         <v>12426.7</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>12524.11</v>
       </c>
     </row>
     <row r="53">
@@ -1060,6 +1196,7 @@
       <c r="C53" s="1" t="n"/>
       <c r="D53" s="1" t="n"/>
       <c r="E53" s="1" t="n"/>
+      <c r="F53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="B54" s="3" t="n">
@@ -1074,6 +1211,9 @@
       <c r="E54" s="3" t="n">
         <v>21.45</v>
       </c>
+      <c r="F54" s="3" t="n">
+        <v>21.59</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" s="3" t="n">
@@ -1087,6 +1227,9 @@
       </c>
       <c r="E55" s="3" t="n">
         <v>9784.74</v>
+      </c>
+      <c r="F55" s="3" t="n">
+        <v>9792.09</v>
       </c>
     </row>
     <row r="56">
@@ -1094,6 +1237,7 @@
       <c r="C56" s="1" t="n"/>
       <c r="D56" s="1" t="n"/>
       <c r="E56" s="1" t="n"/>
+      <c r="F56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="B57" s="3" t="n">
@@ -1108,6 +1252,9 @@
       <c r="E57" s="3" t="n">
         <v>26.77</v>
       </c>
+      <c r="F57" s="3" t="n">
+        <v>26.86</v>
+      </c>
     </row>
     <row r="58">
       <c r="B58" s="3" t="n">
@@ -1121,6 +1268,9 @@
       </c>
       <c r="E58" s="3" t="n">
         <v>16111.26</v>
+      </c>
+      <c r="F58" s="3" t="n">
+        <v>16143.99</v>
       </c>
     </row>
     <row r="59">
@@ -1128,6 +1278,7 @@
       <c r="C59" s="1" t="n"/>
       <c r="D59" s="1" t="n"/>
       <c r="E59" s="1" t="n"/>
+      <c r="F59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="B60" s="3" t="n">
@@ -1142,6 +1293,9 @@
       <c r="E60" s="3" t="n">
         <v>32.17</v>
       </c>
+      <c r="F60" s="3" t="n">
+        <v>32.17</v>
+      </c>
     </row>
     <row r="61">
       <c r="B61" s="3" t="n">
@@ -1154,6 +1308,9 @@
         <v>17526.85</v>
       </c>
       <c r="E61" s="3" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="F61" s="3" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1162,6 +1319,7 @@
       <c r="C62" s="1" t="n"/>
       <c r="D62" s="1" t="n"/>
       <c r="E62" s="1" t="n"/>
+      <c r="F62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="B63" s="3" t="n">
@@ -1176,6 +1334,9 @@
       <c r="E63" s="3" t="n">
         <v>20.84</v>
       </c>
+      <c r="F63" s="3" t="n">
+        <v>20.84</v>
+      </c>
     </row>
     <row r="64">
       <c r="B64" s="3" t="n">
@@ -1189,6 +1350,9 @@
       </c>
       <c r="E64" s="3" t="n">
         <v>10263.12</v>
+      </c>
+      <c r="F64" s="3" t="n">
+        <v>10293.18</v>
       </c>
     </row>
     <row r="65">
@@ -1196,6 +1360,7 @@
       <c r="C65" s="1" t="n"/>
       <c r="D65" s="1" t="n"/>
       <c r="E65" s="1" t="n"/>
+      <c r="F65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="B66" s="3" t="n">
@@ -1210,6 +1375,9 @@
       <c r="E66" s="3" t="n">
         <v>14.8</v>
       </c>
+      <c r="F66" s="3" t="n">
+        <v>15.19</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" s="3" t="n">
@@ -1223,6 +1391,9 @@
       </c>
       <c r="E67" s="3" t="n">
         <v>9907.07</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>9905.91</v>
       </c>
     </row>
     <row r="68">
@@ -1230,6 +1401,7 @@
       <c r="C68" s="1" t="n"/>
       <c r="D68" s="1" t="n"/>
       <c r="E68" s="1" t="n"/>
+      <c r="F68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="B69" s="3" t="n">
@@ -1244,6 +1416,9 @@
       <c r="E69" s="3" t="n">
         <v>20.88</v>
       </c>
+      <c r="F69" s="3" t="n">
+        <v>20.88</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" s="3" t="n">
@@ -1257,6 +1432,9 @@
       </c>
       <c r="E70" s="3" t="n">
         <v>3164.02</v>
+      </c>
+      <c r="F70" s="3" t="n">
+        <v>3178.1</v>
       </c>
     </row>
     <row r="71">
@@ -1264,6 +1442,7 @@
       <c r="C71" s="1" t="n"/>
       <c r="D71" s="1" t="n"/>
       <c r="E71" s="1" t="n"/>
+      <c r="F71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="B72" s="3" t="n">
@@ -1278,6 +1457,9 @@
       <c r="E72" s="3" t="n">
         <v>43.63</v>
       </c>
+      <c r="F72" s="3" t="n">
+        <v>43.62</v>
+      </c>
     </row>
     <row r="73">
       <c r="B73" s="3" t="n">
@@ -1291,6 +1473,9 @@
       </c>
       <c r="E73" s="3" t="n">
         <v>5894.12</v>
+      </c>
+      <c r="F73" s="3" t="n">
+        <v>5922.48</v>
       </c>
     </row>
     <row r="74">
@@ -1298,6 +1483,7 @@
       <c r="C74" s="1" t="n"/>
       <c r="D74" s="1" t="n"/>
       <c r="E74" s="1" t="n"/>
+      <c r="F74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="B75" s="3" t="n">
@@ -1312,6 +1498,9 @@
       <c r="E75" s="3" t="n">
         <v>29.82</v>
       </c>
+      <c r="F75" s="3" t="n">
+        <v>29.08</v>
+      </c>
     </row>
     <row r="76">
       <c r="B76" s="3" t="n">
@@ -1325,6 +1514,9 @@
       </c>
       <c r="E76" s="3" t="n">
         <v>9444.360000000001</v>
+      </c>
+      <c r="F76" s="3" t="n">
+        <v>9438.25</v>
       </c>
     </row>
     <row r="77">
@@ -1332,6 +1524,7 @@
       <c r="C77" s="1" t="n"/>
       <c r="D77" s="1" t="n"/>
       <c r="E77" s="1" t="n"/>
+      <c r="F77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="B78" s="3" t="n">
@@ -1346,6 +1539,9 @@
       <c r="E78" s="3" t="n">
         <v>18.01</v>
       </c>
+      <c r="F78" s="3" t="n">
+        <v>13.29</v>
+      </c>
     </row>
     <row r="79">
       <c r="B79" s="3" t="n">
@@ -1359,6 +1555,9 @@
       </c>
       <c r="E79" s="3" t="n">
         <v>2422.48</v>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>2412.31</v>
       </c>
     </row>
     <row r="80">
@@ -1366,6 +1565,7 @@
       <c r="C80" s="1" t="n"/>
       <c r="D80" s="1" t="n"/>
       <c r="E80" s="1" t="n"/>
+      <c r="F80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="B81" s="3" t="n">
@@ -1380,6 +1580,9 @@
       <c r="E81" s="3" t="n">
         <v>56.06</v>
       </c>
+      <c r="F81" s="3" t="n">
+        <v>56.14</v>
+      </c>
     </row>
     <row r="82">
       <c r="B82" s="3" t="n">
@@ -1393,6 +1596,9 @@
       </c>
       <c r="E82" s="3" t="n">
         <v>2851.5</v>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>2919.9</v>
       </c>
     </row>
     <row r="83">
@@ -1400,6 +1606,7 @@
       <c r="C83" s="1" t="n"/>
       <c r="D83" s="1" t="n"/>
       <c r="E83" s="1" t="n"/>
+      <c r="F83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="B84" s="3" t="n">
@@ -1414,6 +1621,9 @@
       <c r="E84" s="3" t="n">
         <v>58.79</v>
       </c>
+      <c r="F84" s="3" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85">
       <c r="B85" s="3" t="n">
@@ -1427,6 +1637,9 @@
       </c>
       <c r="E85" s="3" t="n">
         <v>2966.57</v>
+      </c>
+      <c r="F85" s="3" t="n">
+        <v>3054.09</v>
       </c>
     </row>
     <row r="86">
@@ -1434,6 +1647,7 @@
       <c r="C86" s="1" t="n"/>
       <c r="D86" s="1" t="n"/>
       <c r="E86" s="1" t="n"/>
+      <c r="F86" s="1" t="n"/>
     </row>
     <row r="87">
       <c r="B87" s="3" t="n">
@@ -1448,6 +1662,9 @@
       <c r="E87" s="3" t="n">
         <v>52.78</v>
       </c>
+      <c r="F87" s="3" t="n">
+        <v>52.38</v>
+      </c>
     </row>
     <row r="88">
       <c r="B88" s="3" t="n">
@@ -1461,6 +1678,9 @@
       </c>
       <c r="E88" s="3" t="n">
         <v>3909.78</v>
+      </c>
+      <c r="F88" s="3" t="n">
+        <v>3967.85</v>
       </c>
     </row>
     <row r="89">
@@ -1468,6 +1688,7 @@
       <c r="C89" s="1" t="n"/>
       <c r="D89" s="1" t="n"/>
       <c r="E89" s="1" t="n"/>
+      <c r="F89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="B90" s="3" t="n">
@@ -1482,6 +1703,9 @@
       <c r="E90" s="3" t="n">
         <v>47.79</v>
       </c>
+      <c r="F90" s="3" t="n">
+        <v>47.08</v>
+      </c>
     </row>
     <row r="91">
       <c r="B91" s="3" t="n">
@@ -1495,6 +1719,9 @@
       </c>
       <c r="E91" s="3" t="n">
         <v>2083.67</v>
+      </c>
+      <c r="F91" s="3" t="n">
+        <v>2080.33</v>
       </c>
     </row>
     <row r="92">
@@ -1502,6 +1729,7 @@
       <c r="C92" s="1" t="n"/>
       <c r="D92" s="1" t="n"/>
       <c r="E92" s="1" t="n"/>
+      <c r="F92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="B93" s="3" t="n">
@@ -1516,6 +1744,9 @@
       <c r="E93" s="3" t="n">
         <v>28.1</v>
       </c>
+      <c r="F93" s="3" t="n">
+        <v>28.02</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" s="3" t="n">
@@ -1529,6 +1760,9 @@
       </c>
       <c r="E94" s="3" t="n">
         <v>13963.26</v>
+      </c>
+      <c r="F94" s="3" t="n">
+        <v>14014.87</v>
       </c>
     </row>
     <row r="95">
@@ -1536,6 +1770,7 @@
       <c r="C95" s="1" t="n"/>
       <c r="D95" s="1" t="n"/>
       <c r="E95" s="1" t="n"/>
+      <c r="F95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="B96" s="3" t="n">
@@ -1550,6 +1785,9 @@
       <c r="E96" s="3" t="n">
         <v>86.69</v>
       </c>
+      <c r="F96" s="3" t="n">
+        <v>86.36</v>
+      </c>
     </row>
     <row r="97">
       <c r="B97" s="3" t="n">
@@ -1563,6 +1801,9 @@
       </c>
       <c r="E97" s="3" t="n">
         <v>8981.85</v>
+      </c>
+      <c r="F97" s="3" t="n">
+        <v>9121.07</v>
       </c>
     </row>
     <row r="98">
@@ -1570,6 +1811,7 @@
       <c r="C98" s="1" t="n"/>
       <c r="D98" s="1" t="n"/>
       <c r="E98" s="1" t="n"/>
+      <c r="F98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="B99" s="3" t="n">
@@ -1584,6 +1826,9 @@
       <c r="E99" s="3" t="n">
         <v>56.94</v>
       </c>
+      <c r="F99" s="3" t="n">
+        <v>57.02</v>
+      </c>
     </row>
     <row r="100">
       <c r="B100" s="3" t="n">
@@ -1597,6 +1842,9 @@
       </c>
       <c r="E100" s="3" t="n">
         <v>12232.61</v>
+      </c>
+      <c r="F100" s="3" t="n">
+        <v>12359.35</v>
       </c>
     </row>
     <row r="101">
@@ -1604,6 +1852,7 @@
       <c r="C101" s="1" t="n"/>
       <c r="D101" s="1" t="n"/>
       <c r="E101" s="1" t="n"/>
+      <c r="F101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="B102" s="3" t="n">
@@ -1618,6 +1867,9 @@
       <c r="E102" s="3" t="n">
         <v>5.94</v>
       </c>
+      <c r="F102" s="3" t="n">
+        <v>6.08</v>
+      </c>
     </row>
     <row r="103">
       <c r="B103" s="3" t="n">
@@ -1631,6 +1883,9 @@
       </c>
       <c r="E103" s="3" t="n">
         <v>2274.27</v>
+      </c>
+      <c r="F103" s="3" t="n">
+        <v>2283.56</v>
       </c>
     </row>
     <row r="104">
@@ -1638,6 +1893,7 @@
       <c r="C104" s="1" t="n"/>
       <c r="D104" s="1" t="n"/>
       <c r="E104" s="1" t="n"/>
+      <c r="F104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="B105" s="3" t="n">
@@ -1652,6 +1908,9 @@
       <c r="E105" s="3" t="n">
         <v>26.15</v>
       </c>
+      <c r="F105" s="3" t="n">
+        <v>26.06</v>
+      </c>
     </row>
     <row r="106">
       <c r="B106" s="3" t="n">
@@ -1665,6 +1924,9 @@
       </c>
       <c r="E106" s="3" t="n">
         <v>873.12</v>
+      </c>
+      <c r="F106" s="3" t="n">
+        <v>879.7</v>
       </c>
     </row>
     <row r="107">
@@ -1672,6 +1934,7 @@
       <c r="C107" s="1" t="n"/>
       <c r="D107" s="1" t="n"/>
       <c r="E107" s="1" t="n"/>
+      <c r="F107" s="1" t="n"/>
     </row>
     <row r="108">
       <c r="B108" s="3" t="n">
@@ -1686,6 +1949,9 @@
       <c r="E108" s="3" t="n">
         <v>29.58</v>
       </c>
+      <c r="F108" s="3" t="n">
+        <v>29.51</v>
+      </c>
     </row>
     <row r="109">
       <c r="B109" s="3" t="n">
@@ -1699,6 +1965,9 @@
       </c>
       <c r="E109" s="3" t="n">
         <v>2734.02</v>
+      </c>
+      <c r="F109" s="3" t="n">
+        <v>2779.5</v>
       </c>
     </row>
     <row r="110">
@@ -1706,6 +1975,7 @@
       <c r="C110" s="1" t="n"/>
       <c r="D110" s="1" t="n"/>
       <c r="E110" s="1" t="n"/>
+      <c r="F110" s="1" t="n"/>
     </row>
     <row r="111">
       <c r="B111" s="3" t="n">
@@ -1720,6 +1990,9 @@
       <c r="E111" s="3" t="n">
         <v>21.2</v>
       </c>
+      <c r="F111" s="3" t="n">
+        <v>21.37</v>
+      </c>
     </row>
     <row r="112">
       <c r="B112" s="3" t="n">
@@ -1733,6 +2006,9 @@
       </c>
       <c r="E112" s="3" t="n">
         <v>3971.97</v>
+      </c>
+      <c r="F112" s="3" t="n">
+        <v>3998.7</v>
       </c>
     </row>
     <row r="113">
@@ -1740,6 +2016,7 @@
       <c r="C113" s="1" t="n"/>
       <c r="D113" s="1" t="n"/>
       <c r="E113" s="1" t="n"/>
+      <c r="F113" s="1" t="n"/>
     </row>
     <row r="114">
       <c r="B114" s="3" t="n">
@@ -1754,6 +2031,9 @@
       <c r="E114" s="3" t="n">
         <v>29.02</v>
       </c>
+      <c r="F114" s="3" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115">
       <c r="B115" s="3" t="n">
@@ -1767,6 +2047,9 @@
       </c>
       <c r="E115" s="3" t="n">
         <v>3358.45</v>
+      </c>
+      <c r="F115" s="3" t="n">
+        <v>3372.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-10 04:07:12]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -498,6 +498,11 @@
           <t>2025/11/06</t>
         </is>
       </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>2025/11/10</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -525,6 +530,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -542,6 +552,9 @@
       <c r="E3" s="6" t="n">
         <v>62.19</v>
       </c>
+      <c r="F3" s="6" t="n">
+        <v>63.08</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -558,6 +571,9 @@
       </c>
       <c r="E4" s="6" t="n">
         <v>4004.25</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>3996.26</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -566,6 +582,7 @@
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="4" t="n"/>
+      <c r="F5" s="4" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -583,6 +600,9 @@
       <c r="E6" s="6" t="n">
         <v>48.86</v>
       </c>
+      <c r="F6" s="6" t="n">
+        <v>49.74</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -599,6 +619,9 @@
       </c>
       <c r="E7" s="6" t="n">
         <v>5622.59</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>5603.46</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -607,6 +630,7 @@
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="n"/>
       <c r="E8" s="4" t="n"/>
+      <c r="F8" s="4" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -624,6 +648,9 @@
       <c r="E9" s="6" t="n">
         <v>54.53</v>
       </c>
+      <c r="F9" s="6" t="n">
+        <v>55.22</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -640,6 +667,9 @@
       </c>
       <c r="E10" s="6" t="n">
         <v>4686.45</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>4667.62</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -648,6 +678,7 @@
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="4" t="n"/>
+      <c r="F11" s="4" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -665,6 +696,9 @@
       <c r="E12" s="6" t="n">
         <v>57.07</v>
       </c>
+      <c r="F12" s="6" t="n">
+        <v>57.52</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -681,6 +715,9 @@
       </c>
       <c r="E13" s="6" t="n">
         <v>7329.9</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>7293.5</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -689,6 +726,7 @@
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n"/>
       <c r="E14" s="4" t="n"/>
+      <c r="F14" s="4" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -706,6 +744,9 @@
       <c r="E15" s="6" t="n">
         <v>27.11</v>
       </c>
+      <c r="F15" s="6" t="n">
+        <v>27.89</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -722,6 +763,9 @@
       </c>
       <c r="E16" s="6" t="n">
         <v>2737.68</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>2733.36</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -730,6 +774,7 @@
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n"/>
       <c r="E17" s="4" t="n"/>
+      <c r="F17" s="4" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -747,6 +792,9 @@
       <c r="E18" s="6" t="n">
         <v>96.75</v>
       </c>
+      <c r="F18" s="6" t="n">
+        <v>96.12</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -763,6 +811,9 @@
       </c>
       <c r="E19" s="6" t="n">
         <v>6796.29</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>6728.8</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -771,6 +822,7 @@
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n"/>
       <c r="E20" s="4" t="n"/>
+      <c r="F20" s="4" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -788,6 +840,9 @@
       <c r="E21" s="6" t="n">
         <v>62.44</v>
       </c>
+      <c r="F21" s="6" t="n">
+        <v>60.84</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -804,6 +859,9 @@
       </c>
       <c r="E22" s="6" t="n">
         <v>83516.69</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>83511.49000000001</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -812,6 +870,7 @@
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="1" t="n"/>
       <c r="E23" s="4" t="n"/>
+      <c r="F23" s="4" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -829,6 +888,9 @@
       <c r="E24" s="6" t="n">
         <v>85</v>
       </c>
+      <c r="F24" s="6" t="n">
+        <v>84.14</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -844,6 +906,9 @@
         <v>19909.14</v>
       </c>
       <c r="E25" s="6" t="n">
+        <v>19909.14</v>
+      </c>
+      <c r="F25" s="6" t="n">
         <v>19909.14</v>
       </c>
     </row>
@@ -853,6 +918,7 @@
       <c r="C26" s="1" t="n"/>
       <c r="D26" s="1" t="n"/>
       <c r="E26" s="4" t="n"/>
+      <c r="F26" s="4" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -870,6 +936,9 @@
       <c r="E27" s="6" t="n">
         <v>84.44</v>
       </c>
+      <c r="F27" s="6" t="n">
+        <v>79.5</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -885,6 +954,9 @@
         <v>39894.54</v>
       </c>
       <c r="E28" s="6" t="n">
+        <v>39894.54</v>
+      </c>
+      <c r="F28" s="6" t="n">
         <v>39894.54</v>
       </c>
     </row>
@@ -894,6 +966,7 @@
       <c r="C29" s="1" t="n"/>
       <c r="D29" s="1" t="n"/>
       <c r="E29" s="4" t="n"/>
+      <c r="F29" s="4" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -911,6 +984,9 @@
       <c r="E30" s="6" t="n">
         <v>58.54</v>
       </c>
+      <c r="F30" s="6" t="n">
+        <v>58.47</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -927,6 +1003,9 @@
       </c>
       <c r="E31" s="6" t="n">
         <v>5743.07</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>5784.14</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -935,6 +1014,7 @@
       <c r="C32" s="1" t="n"/>
       <c r="D32" s="1" t="n"/>
       <c r="E32" s="4" t="n"/>
+      <c r="F32" s="4" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -952,6 +1032,9 @@
       <c r="E33" s="6" t="n">
         <v>10.73</v>
       </c>
+      <c r="F33" s="6" t="n">
+        <v>11.05</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -968,6 +1051,9 @@
       </c>
       <c r="E34" s="6" t="n">
         <v>32915.64</v>
+      </c>
+      <c r="F34" s="6" t="n">
+        <v>32688.86</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -976,6 +1062,7 @@
       <c r="C35" s="1" t="n"/>
       <c r="D35" s="1" t="n"/>
       <c r="E35" s="4" t="n"/>
+      <c r="F35" s="4" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -993,6 +1080,9 @@
       <c r="E36" s="6" t="n">
         <v>28.88</v>
       </c>
+      <c r="F36" s="6" t="n">
+        <v>29.27</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1009,6 +1099,9 @@
       </c>
       <c r="E37" s="6" t="n">
         <v>3408.39</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <v>3308.8</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1017,6 +1110,7 @@
       <c r="C38" s="1" t="n"/>
       <c r="D38" s="1" t="n"/>
       <c r="E38" s="4" t="n"/>
+      <c r="F38" s="4" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1034,6 +1128,9 @@
       <c r="E39" s="6" t="n">
         <v>46.41</v>
       </c>
+      <c r="F39" s="6" t="n">
+        <v>47.13</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1050,6 +1147,9 @@
       </c>
       <c r="E40" s="6" t="n">
         <v>3210.15</v>
+      </c>
+      <c r="F40" s="6" t="n">
+        <v>3139.88</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1058,6 +1158,7 @@
       <c r="C41" s="1" t="n"/>
       <c r="D41" s="1" t="n"/>
       <c r="E41" s="4" t="n"/>
+      <c r="F41" s="4" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1075,6 +1176,9 @@
       <c r="E42" s="6" t="n">
         <v>17.76</v>
       </c>
+      <c r="F42" s="6" t="n">
+        <v>17.55</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1091,6 +1195,9 @@
       </c>
       <c r="E43" s="6" t="n">
         <v>7217.37</v>
+      </c>
+      <c r="F43" s="6" t="n">
+        <v>7267.61</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1099,6 +1206,7 @@
       <c r="C44" s="1" t="n"/>
       <c r="D44" s="1" t="n"/>
       <c r="E44" s="4" t="n"/>
+      <c r="F44" s="4" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1116,6 +1224,9 @@
       <c r="E45" s="6" t="n">
         <v>29.95</v>
       </c>
+      <c r="F45" s="6" t="n">
+        <v>29.71</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1132,6 +1243,9 @@
       </c>
       <c r="E46" s="6" t="n">
         <v>8720.940000000001</v>
+      </c>
+      <c r="F46" s="6" t="n">
+        <v>8733.940000000001</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1140,6 +1254,7 @@
       <c r="C47" s="1" t="n"/>
       <c r="D47" s="1" t="n"/>
       <c r="E47" s="4" t="n"/>
+      <c r="F47" s="4" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1157,6 +1272,9 @@
       <c r="E48" s="6" t="n">
         <v>11.86</v>
       </c>
+      <c r="F48" s="6" t="n">
+        <v>12.05</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1173,6 +1291,9 @@
       </c>
       <c r="E49" s="6" t="n">
         <v>12913.82</v>
+      </c>
+      <c r="F49" s="6" t="n">
+        <v>13048.27</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1181,6 +1302,7 @@
       <c r="C50" s="1" t="n"/>
       <c r="D50" s="1" t="n"/>
       <c r="E50" s="4" t="n"/>
+      <c r="F50" s="4" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1198,6 +1320,9 @@
       <c r="E51" s="6" t="n">
         <v>23.12</v>
       </c>
+      <c r="F51" s="6" t="n">
+        <v>24.43</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -1214,6 +1339,9 @@
       </c>
       <c r="E52" s="6" t="n">
         <v>12592.17</v>
+      </c>
+      <c r="F52" s="6" t="n">
+        <v>12510.65</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1222,6 +1350,7 @@
       <c r="C53" s="1" t="n"/>
       <c r="D53" s="1" t="n"/>
       <c r="E53" s="4" t="n"/>
+      <c r="F53" s="4" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -1239,6 +1368,9 @@
       <c r="E54" s="6" t="n">
         <v>20.61</v>
       </c>
+      <c r="F54" s="6" t="n">
+        <v>20.86</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -1255,6 +1387,9 @@
       </c>
       <c r="E55" s="6" t="n">
         <v>9629.75</v>
+      </c>
+      <c r="F55" s="6" t="n">
+        <v>9942.389999999999</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -1263,6 +1398,7 @@
       <c r="C56" s="1" t="n"/>
       <c r="D56" s="1" t="n"/>
       <c r="E56" s="4" t="n"/>
+      <c r="F56" s="4" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -1280,6 +1416,9 @@
       <c r="E57" s="6" t="n">
         <v>26.32</v>
       </c>
+      <c r="F57" s="6" t="n">
+        <v>26.45</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -1296,6 +1435,9 @@
       </c>
       <c r="E58" s="6" t="n">
         <v>15941.62</v>
+      </c>
+      <c r="F58" s="6" t="n">
+        <v>16321.19</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -1304,6 +1446,7 @@
       <c r="C59" s="1" t="n"/>
       <c r="D59" s="1" t="n"/>
       <c r="E59" s="4" t="n"/>
+      <c r="F59" s="4" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -1321,6 +1464,9 @@
       <c r="E60" s="6" t="n">
         <v>31.59</v>
       </c>
+      <c r="F60" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -1336,6 +1482,9 @@
         <v>17526.85</v>
       </c>
       <c r="E61" s="6" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="F61" s="6" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1345,6 +1494,7 @@
       <c r="C62" s="1" t="n"/>
       <c r="D62" s="1" t="n"/>
       <c r="E62" s="4" t="n"/>
+      <c r="F62" s="4" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -1362,6 +1512,9 @@
       <c r="E63" s="6" t="n">
         <v>20.55</v>
       </c>
+      <c r="F63" s="6" t="n">
+        <v>20.55</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -1378,6 +1531,9 @@
       </c>
       <c r="E64" s="6" t="n">
         <v>10347.9</v>
+      </c>
+      <c r="F64" s="6" t="n">
+        <v>10253.01</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -1386,6 +1542,7 @@
       <c r="C65" s="1" t="n"/>
       <c r="D65" s="1" t="n"/>
       <c r="E65" s="4" t="n"/>
+      <c r="F65" s="4" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -1403,6 +1560,9 @@
       <c r="E66" s="6" t="n">
         <v>14.59</v>
       </c>
+      <c r="F66" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -1419,6 +1579,9 @@
       </c>
       <c r="E67" s="6" t="n">
         <v>9855.49</v>
+      </c>
+      <c r="F67" s="6" t="n">
+        <v>10099.81</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -1427,6 +1590,7 @@
       <c r="C68" s="1" t="n"/>
       <c r="D68" s="1" t="n"/>
       <c r="E68" s="4" t="n"/>
+      <c r="F68" s="4" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -1444,6 +1608,9 @@
       <c r="E69" s="6" t="n">
         <v>20.34</v>
       </c>
+      <c r="F69" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -1460,6 +1627,9 @@
       </c>
       <c r="E70" s="6" t="n">
         <v>3162.29</v>
+      </c>
+      <c r="F70" s="6" t="n">
+        <v>3119.78</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -1468,6 +1638,7 @@
       <c r="C71" s="1" t="n"/>
       <c r="D71" s="1" t="n"/>
       <c r="E71" s="4" t="n"/>
+      <c r="F71" s="4" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -1485,6 +1656,9 @@
       <c r="E72" s="6" t="n">
         <v>42.56</v>
       </c>
+      <c r="F72" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -1501,6 +1675,9 @@
       </c>
       <c r="E73" s="6" t="n">
         <v>5902.71</v>
+      </c>
+      <c r="F73" s="6" t="n">
+        <v>5844.58</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -1509,6 +1686,7 @@
       <c r="C74" s="1" t="n"/>
       <c r="D74" s="1" t="n"/>
       <c r="E74" s="4" t="n"/>
+      <c r="F74" s="4" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -1526,6 +1704,9 @@
       <c r="E75" s="6" t="n">
         <v>27.29</v>
       </c>
+      <c r="F75" s="6" t="n">
+        <v>26.86</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -1542,6 +1723,9 @@
       </c>
       <c r="E76" s="6" t="n">
         <v>9256.559999999999</v>
+      </c>
+      <c r="F76" s="6" t="n">
+        <v>9289.82</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -1550,6 +1734,7 @@
       <c r="C77" s="1" t="n"/>
       <c r="D77" s="1" t="n"/>
       <c r="E77" s="4" t="n"/>
+      <c r="F77" s="4" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -1567,6 +1752,9 @@
       <c r="E78" s="6" t="n">
         <v>13.35</v>
       </c>
+      <c r="F78" s="6" t="n">
+        <v>13.39</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -1583,6 +1771,9 @@
       </c>
       <c r="E79" s="6" t="n">
         <v>2440.24</v>
+      </c>
+      <c r="F79" s="6" t="n">
+        <v>1317.73</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -1591,6 +1782,7 @@
       <c r="C80" s="1" t="n"/>
       <c r="D80" s="1" t="n"/>
       <c r="E80" s="4" t="n"/>
+      <c r="F80" s="4" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -1608,6 +1800,9 @@
       <c r="E81" s="6" t="n">
         <v>55.41</v>
       </c>
+      <c r="F81" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -1624,6 +1819,9 @@
       </c>
       <c r="E82" s="6" t="n">
         <v>3000.95</v>
+      </c>
+      <c r="F82" s="6" t="n">
+        <v>3035.4</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -1632,6 +1830,7 @@
       <c r="C83" s="1" t="n"/>
       <c r="D83" s="1" t="n"/>
       <c r="E83" s="4" t="n"/>
+      <c r="F83" s="4" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -1649,6 +1848,9 @@
       <c r="E84" s="6" t="n">
         <v>58.79</v>
       </c>
+      <c r="F84" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -1665,6 +1867,9 @@
       </c>
       <c r="E85" s="6" t="n">
         <v>3196.03</v>
+      </c>
+      <c r="F85" s="6" t="n">
+        <v>3230.17</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -1673,6 +1878,7 @@
       <c r="C86" s="1" t="n"/>
       <c r="D86" s="1" t="n"/>
       <c r="E86" s="4" t="n"/>
+      <c r="F86" s="4" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -1690,6 +1896,9 @@
       <c r="E87" s="6" t="n">
         <v>51.78</v>
       </c>
+      <c r="F87" s="6" t="n">
+        <v>53.01</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -1706,6 +1915,9 @@
       </c>
       <c r="E88" s="6" t="n">
         <v>3970.69</v>
+      </c>
+      <c r="F88" s="6" t="n">
+        <v>3988.79</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -1714,6 +1926,7 @@
       <c r="C89" s="1" t="n"/>
       <c r="D89" s="1" t="n"/>
       <c r="E89" s="4" t="n"/>
+      <c r="F89" s="4" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -1731,6 +1944,9 @@
       <c r="E90" s="6" t="n">
         <v>45.64</v>
       </c>
+      <c r="F90" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -1747,6 +1963,9 @@
       </c>
       <c r="E91" s="6" t="n">
         <v>2022.89</v>
+      </c>
+      <c r="F91" s="6" t="n">
+        <v>2011.61</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -1755,6 +1974,7 @@
       <c r="C92" s="1" t="n"/>
       <c r="D92" s="1" t="n"/>
       <c r="E92" s="4" t="n"/>
+      <c r="F92" s="4" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -1772,6 +1992,9 @@
       <c r="E93" s="6" t="n">
         <v>27.66</v>
       </c>
+      <c r="F93" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -1788,6 +2011,9 @@
       </c>
       <c r="E94" s="6" t="n">
         <v>13899.04</v>
+      </c>
+      <c r="F94" s="6" t="n">
+        <v>13989.57</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -1796,6 +2022,7 @@
       <c r="C95" s="1" t="n"/>
       <c r="D95" s="1" t="n"/>
       <c r="E95" s="4" t="n"/>
+      <c r="F95" s="4" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -1813,6 +2040,9 @@
       <c r="E96" s="6" t="n">
         <v>85.83</v>
       </c>
+      <c r="F96" s="6" t="n">
+        <v>86.64</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -1829,6 +2059,9 @@
       </c>
       <c r="E97" s="6" t="n">
         <v>9235.15</v>
+      </c>
+      <c r="F97" s="6" t="n">
+        <v>8996.290000000001</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -1837,6 +2070,7 @@
       <c r="C98" s="1" t="n"/>
       <c r="D98" s="1" t="n"/>
       <c r="E98" s="4" t="n"/>
+      <c r="F98" s="4" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -1854,6 +2088,9 @@
       <c r="E99" s="6" t="n">
         <v>56.8</v>
       </c>
+      <c r="F99" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -1870,6 +2107,9 @@
       </c>
       <c r="E100" s="6" t="n">
         <v>12277.26</v>
+      </c>
+      <c r="F100" s="6" t="n">
+        <v>12116.98</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -1878,6 +2118,7 @@
       <c r="C101" s="1" t="n"/>
       <c r="D101" s="1" t="n"/>
       <c r="E101" s="4" t="n"/>
+      <c r="F101" s="4" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -1895,6 +2136,9 @@
       <c r="E102" s="6" t="n">
         <v>5.86</v>
       </c>
+      <c r="F102" s="6" t="n">
+        <v>5.93</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -1911,6 +2155,9 @@
       </c>
       <c r="E103" s="6" t="n">
         <v>2277.37</v>
+      </c>
+      <c r="F103" s="6" t="n">
+        <v>2317.11</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -1919,6 +2166,7 @@
       <c r="C104" s="1" t="n"/>
       <c r="D104" s="1" t="n"/>
       <c r="E104" s="4" t="n"/>
+      <c r="F104" s="4" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -1936,6 +2184,9 @@
       <c r="E105" s="6" t="n">
         <v>25.93</v>
       </c>
+      <c r="F105" s="6" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -1952,6 +2203,9 @@
       </c>
       <c r="E106" s="6" t="n">
         <v>884.65</v>
+      </c>
+      <c r="F106" s="6" t="n">
+        <v>882.91</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -1960,6 +2214,7 @@
       <c r="C107" s="1" t="n"/>
       <c r="D107" s="1" t="n"/>
       <c r="E107" s="4" t="n"/>
+      <c r="F107" s="4" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -1977,6 +2232,9 @@
       <c r="E108" s="6" t="n">
         <v>29.34</v>
       </c>
+      <c r="F108" s="6" t="n">
+        <v>29.59</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -1993,6 +2251,9 @@
       </c>
       <c r="E109" s="6" t="n">
         <v>2786.8</v>
+      </c>
+      <c r="F109" s="6" t="n">
+        <v>2825.96</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -2001,6 +2262,7 @@
       <c r="C110" s="1" t="n"/>
       <c r="D110" s="1" t="n"/>
       <c r="E110" s="4" t="n"/>
+      <c r="F110" s="4" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -2018,6 +2280,9 @@
       <c r="E111" s="6" t="n">
         <v>21.22</v>
       </c>
+      <c r="F111" s="6" t="n">
+        <v>21.5</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -2034,6 +2299,9 @@
       </c>
       <c r="E112" s="6" t="n">
         <v>4037.97</v>
+      </c>
+      <c r="F112" s="6" t="n">
+        <v>4028.19</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -2042,6 +2310,7 @@
       <c r="C113" s="1" t="n"/>
       <c r="D113" s="1" t="n"/>
       <c r="E113" s="4" t="n"/>
+      <c r="F113" s="4" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -2059,6 +2328,9 @@
       <c r="E114" s="6" t="n">
         <v>29.02</v>
       </c>
+      <c r="F114" s="6" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -2075,6 +2347,9 @@
       </c>
       <c r="E115" s="6" t="n">
         <v>3354.92</v>
+      </c>
+      <c r="F115" s="6" t="n">
+        <v>3350.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-13 04:00:39]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -503,6 +503,11 @@
           <t>2025/11/10</t>
         </is>
       </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>2025/11/13</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -535,6 +540,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -555,6 +565,9 @@
       <c r="F3" s="6" t="n">
         <v>63.08</v>
       </c>
+      <c r="G3" s="6" t="n">
+        <v>63.21</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -574,6 +587,9 @@
       </c>
       <c r="F4" s="6" t="n">
         <v>3996.26</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>4017.94</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -583,6 +599,7 @@
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="4" t="n"/>
       <c r="F5" s="4" t="n"/>
+      <c r="G5" s="4" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -603,6 +620,9 @@
       <c r="F6" s="6" t="n">
         <v>49.74</v>
       </c>
+      <c r="G6" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -622,6 +642,9 @@
       </c>
       <c r="F7" s="6" t="n">
         <v>5603.46</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>5648.68</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -631,6 +654,7 @@
       <c r="D8" s="1" t="n"/>
       <c r="E8" s="4" t="n"/>
       <c r="F8" s="4" t="n"/>
+      <c r="G8" s="4" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -651,6 +675,9 @@
       <c r="F9" s="6" t="n">
         <v>55.22</v>
       </c>
+      <c r="G9" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -670,6 +697,9 @@
       </c>
       <c r="F10" s="6" t="n">
         <v>4667.62</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>4690.71</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -679,6 +709,7 @@
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="4" t="n"/>
       <c r="F11" s="4" t="n"/>
+      <c r="G11" s="4" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -699,6 +730,9 @@
       <c r="F12" s="6" t="n">
         <v>57.52</v>
       </c>
+      <c r="G12" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -718,6 +752,9 @@
       </c>
       <c r="F13" s="6" t="n">
         <v>7293.5</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>7363.44</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -727,6 +764,7 @@
       <c r="D14" s="1" t="n"/>
       <c r="E14" s="4" t="n"/>
       <c r="F14" s="4" t="n"/>
+      <c r="G14" s="4" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -747,6 +785,9 @@
       <c r="F15" s="6" t="n">
         <v>27.89</v>
       </c>
+      <c r="G15" s="6" t="n">
+        <v>29.44</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -766,6 +807,9 @@
       </c>
       <c r="F16" s="6" t="n">
         <v>2733.36</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>2755.62</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -775,6 +819,7 @@
       <c r="D17" s="1" t="n"/>
       <c r="E17" s="4" t="n"/>
       <c r="F17" s="4" t="n"/>
+      <c r="G17" s="4" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -795,6 +840,9 @@
       <c r="F18" s="6" t="n">
         <v>96.12</v>
       </c>
+      <c r="G18" s="6" t="n">
+        <v>96.67</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -814,6 +862,9 @@
       </c>
       <c r="F19" s="6" t="n">
         <v>6728.8</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>6850.92</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -823,6 +874,7 @@
       <c r="D20" s="1" t="n"/>
       <c r="E20" s="4" t="n"/>
       <c r="F20" s="4" t="n"/>
+      <c r="G20" s="4" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -843,6 +895,9 @@
       <c r="F21" s="6" t="n">
         <v>60.84</v>
       </c>
+      <c r="G21" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -862,6 +917,9 @@
       </c>
       <c r="F22" s="6" t="n">
         <v>83511.49000000001</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <v>84525.89</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -871,6 +929,7 @@
       <c r="D23" s="1" t="n"/>
       <c r="E23" s="4" t="n"/>
       <c r="F23" s="4" t="n"/>
+      <c r="G23" s="4" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -891,6 +950,9 @@
       <c r="F24" s="6" t="n">
         <v>84.14</v>
       </c>
+      <c r="G24" s="6" t="n">
+        <v>84.14</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -909,6 +971,9 @@
         <v>19909.14</v>
       </c>
       <c r="F25" s="6" t="n">
+        <v>19909.14</v>
+      </c>
+      <c r="G25" s="6" t="n">
         <v>19909.14</v>
       </c>
     </row>
@@ -919,6 +984,7 @@
       <c r="D26" s="1" t="n"/>
       <c r="E26" s="4" t="n"/>
       <c r="F26" s="4" t="n"/>
+      <c r="G26" s="4" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -939,6 +1005,9 @@
       <c r="F27" s="6" t="n">
         <v>79.5</v>
       </c>
+      <c r="G27" s="6" t="n">
+        <v>71.64</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -957,6 +1026,9 @@
         <v>39894.54</v>
       </c>
       <c r="F28" s="6" t="n">
+        <v>39894.54</v>
+      </c>
+      <c r="G28" s="6" t="n">
         <v>39894.54</v>
       </c>
     </row>
@@ -967,6 +1039,7 @@
       <c r="D29" s="1" t="n"/>
       <c r="E29" s="4" t="n"/>
       <c r="F29" s="4" t="n"/>
+      <c r="G29" s="4" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -987,6 +1060,9 @@
       <c r="F30" s="6" t="n">
         <v>58.47</v>
       </c>
+      <c r="G30" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1006,6 +1082,9 @@
       </c>
       <c r="F31" s="6" t="n">
         <v>5784.14</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>5774</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1015,6 +1094,7 @@
       <c r="D32" s="1" t="n"/>
       <c r="E32" s="4" t="n"/>
       <c r="F32" s="4" t="n"/>
+      <c r="G32" s="4" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1035,6 +1115,9 @@
       <c r="F33" s="6" t="n">
         <v>11.05</v>
       </c>
+      <c r="G33" s="6" t="n">
+        <v>12.61</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1054,6 +1137,9 @@
       </c>
       <c r="F34" s="6" t="n">
         <v>32688.86</v>
+      </c>
+      <c r="G34" s="6" t="n">
+        <v>32685.54</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1063,6 +1149,7 @@
       <c r="D35" s="1" t="n"/>
       <c r="E35" s="4" t="n"/>
       <c r="F35" s="4" t="n"/>
+      <c r="G35" s="4" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1083,6 +1170,9 @@
       <c r="F36" s="6" t="n">
         <v>29.27</v>
       </c>
+      <c r="G36" s="6" t="n">
+        <v>28.23</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1102,6 +1192,9 @@
       </c>
       <c r="F37" s="6" t="n">
         <v>3308.8</v>
+      </c>
+      <c r="G37" s="6" t="n">
+        <v>3381.23</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1111,6 +1204,7 @@
       <c r="D38" s="1" t="n"/>
       <c r="E38" s="4" t="n"/>
       <c r="F38" s="4" t="n"/>
+      <c r="G38" s="4" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1131,6 +1225,9 @@
       <c r="F39" s="6" t="n">
         <v>47.13</v>
       </c>
+      <c r="G39" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1150,6 +1247,9 @@
       </c>
       <c r="F40" s="6" t="n">
         <v>3139.88</v>
+      </c>
+      <c r="G40" s="6" t="n">
+        <v>3205.76</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1159,6 +1259,7 @@
       <c r="D41" s="1" t="n"/>
       <c r="E41" s="4" t="n"/>
       <c r="F41" s="4" t="n"/>
+      <c r="G41" s="4" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1179,6 +1280,9 @@
       <c r="F42" s="6" t="n">
         <v>17.55</v>
       </c>
+      <c r="G42" s="6" t="n">
+        <v>18.21</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1198,6 +1302,9 @@
       </c>
       <c r="F43" s="6" t="n">
         <v>7267.61</v>
+      </c>
+      <c r="G43" s="6" t="n">
+        <v>7305.09</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1207,6 +1314,7 @@
       <c r="D44" s="1" t="n"/>
       <c r="E44" s="4" t="n"/>
       <c r="F44" s="4" t="n"/>
+      <c r="G44" s="4" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1227,6 +1335,9 @@
       <c r="F45" s="6" t="n">
         <v>29.71</v>
       </c>
+      <c r="G45" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1246,6 +1357,9 @@
       </c>
       <c r="F46" s="6" t="n">
         <v>8733.940000000001</v>
+      </c>
+      <c r="G46" s="6" t="n">
+        <v>8880.959999999999</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1255,6 +1369,7 @@
       <c r="D47" s="1" t="n"/>
       <c r="E47" s="4" t="n"/>
       <c r="F47" s="4" t="n"/>
+      <c r="G47" s="4" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1275,6 +1390,9 @@
       <c r="F48" s="6" t="n">
         <v>12.05</v>
       </c>
+      <c r="G48" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1294,6 +1412,9 @@
       </c>
       <c r="F49" s="6" t="n">
         <v>13048.27</v>
+      </c>
+      <c r="G49" s="6" t="n">
+        <v>13055.99</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1303,6 +1424,7 @@
       <c r="D50" s="1" t="n"/>
       <c r="E50" s="4" t="n"/>
       <c r="F50" s="4" t="n"/>
+      <c r="G50" s="4" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1323,6 +1445,9 @@
       <c r="F51" s="6" t="n">
         <v>24.43</v>
       </c>
+      <c r="G51" s="6" t="n">
+        <v>26.04</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -1342,6 +1467,9 @@
       </c>
       <c r="F52" s="6" t="n">
         <v>12510.65</v>
+      </c>
+      <c r="G52" s="6" t="n">
+        <v>12603.71</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1351,6 +1479,7 @@
       <c r="D53" s="1" t="n"/>
       <c r="E53" s="4" t="n"/>
       <c r="F53" s="4" t="n"/>
+      <c r="G53" s="4" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -1371,6 +1500,9 @@
       <c r="F54" s="6" t="n">
         <v>20.86</v>
       </c>
+      <c r="G54" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -1390,6 +1522,9 @@
       </c>
       <c r="F55" s="6" t="n">
         <v>9942.389999999999</v>
+      </c>
+      <c r="G55" s="6" t="n">
+        <v>10004.5</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -1399,6 +1534,7 @@
       <c r="D56" s="1" t="n"/>
       <c r="E56" s="4" t="n"/>
       <c r="F56" s="4" t="n"/>
+      <c r="G56" s="4" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -1419,6 +1555,9 @@
       <c r="F57" s="6" t="n">
         <v>26.45</v>
       </c>
+      <c r="G57" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -1438,6 +1577,9 @@
       </c>
       <c r="F58" s="6" t="n">
         <v>16321.19</v>
+      </c>
+      <c r="G58" s="6" t="n">
+        <v>16387.97</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -1447,6 +1589,7 @@
       <c r="D59" s="1" t="n"/>
       <c r="E59" s="4" t="n"/>
       <c r="F59" s="4" t="n"/>
+      <c r="G59" s="4" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -1467,6 +1610,9 @@
       <c r="F60" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G60" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -1485,6 +1631,9 @@
         <v>17526.85</v>
       </c>
       <c r="F61" s="6" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="G61" s="6" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1495,6 +1644,7 @@
       <c r="D62" s="1" t="n"/>
       <c r="E62" s="4" t="n"/>
       <c r="F62" s="4" t="n"/>
+      <c r="G62" s="4" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -1515,6 +1665,9 @@
       <c r="F63" s="6" t="n">
         <v>20.55</v>
       </c>
+      <c r="G63" s="6" t="n">
+        <v>21.11</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -1534,6 +1687,9 @@
       </c>
       <c r="F64" s="6" t="n">
         <v>10253.01</v>
+      </c>
+      <c r="G64" s="6" t="n">
+        <v>10214.48</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -1543,6 +1699,7 @@
       <c r="D65" s="1" t="n"/>
       <c r="E65" s="4" t="n"/>
       <c r="F65" s="4" t="n"/>
+      <c r="G65" s="4" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -1563,6 +1720,9 @@
       <c r="F66" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G66" s="6" t="n">
+        <v>19.06</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -1582,6 +1742,9 @@
       </c>
       <c r="F67" s="6" t="n">
         <v>10099.81</v>
+      </c>
+      <c r="G67" s="6" t="n">
+        <v>10219.1</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -1591,6 +1754,7 @@
       <c r="D68" s="1" t="n"/>
       <c r="E68" s="4" t="n"/>
       <c r="F68" s="4" t="n"/>
+      <c r="G68" s="4" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -1611,6 +1775,9 @@
       <c r="F69" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G69" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -1630,6 +1797,9 @@
       </c>
       <c r="F70" s="6" t="n">
         <v>3119.78</v>
+      </c>
+      <c r="G70" s="6" t="n">
+        <v>3100.16</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -1639,6 +1809,7 @@
       <c r="D71" s="1" t="n"/>
       <c r="E71" s="4" t="n"/>
       <c r="F71" s="4" t="n"/>
+      <c r="G71" s="4" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -1659,6 +1830,9 @@
       <c r="F72" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G72" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -1678,6 +1852,9 @@
       </c>
       <c r="F73" s="6" t="n">
         <v>5844.58</v>
+      </c>
+      <c r="G73" s="6" t="n">
+        <v>5886.87</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -1687,6 +1864,7 @@
       <c r="D74" s="1" t="n"/>
       <c r="E74" s="4" t="n"/>
       <c r="F74" s="4" t="n"/>
+      <c r="G74" s="4" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -1707,6 +1885,9 @@
       <c r="F75" s="6" t="n">
         <v>26.86</v>
       </c>
+      <c r="G75" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -1726,6 +1907,9 @@
       </c>
       <c r="F76" s="6" t="n">
         <v>9289.82</v>
+      </c>
+      <c r="G76" s="6" t="n">
+        <v>9468.610000000001</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -1735,6 +1919,7 @@
       <c r="D77" s="1" t="n"/>
       <c r="E77" s="4" t="n"/>
       <c r="F77" s="4" t="n"/>
+      <c r="G77" s="4" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -1755,6 +1940,9 @@
       <c r="F78" s="6" t="n">
         <v>13.39</v>
       </c>
+      <c r="G78" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -1774,6 +1962,9 @@
       </c>
       <c r="F79" s="6" t="n">
         <v>1317.73</v>
+      </c>
+      <c r="G79" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -1783,6 +1974,7 @@
       <c r="D80" s="1" t="n"/>
       <c r="E80" s="4" t="n"/>
       <c r="F80" s="4" t="n"/>
+      <c r="G80" s="4" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -1803,6 +1995,9 @@
       <c r="F81" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G81" s="6" t="n">
+        <v>56.04</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -1822,6 +2017,9 @@
       </c>
       <c r="F82" s="6" t="n">
         <v>3035.4</v>
+      </c>
+      <c r="G82" s="6" t="n">
+        <v>3076.44</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -1831,6 +2029,7 @@
       <c r="D83" s="1" t="n"/>
       <c r="E83" s="4" t="n"/>
       <c r="F83" s="4" t="n"/>
+      <c r="G83" s="4" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -1851,6 +2050,9 @@
       <c r="F84" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G84" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -1870,6 +2072,9 @@
       </c>
       <c r="F85" s="6" t="n">
         <v>3230.17</v>
+      </c>
+      <c r="G85" s="6" t="n">
+        <v>3158.76</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -1879,6 +2084,7 @@
       <c r="D86" s="1" t="n"/>
       <c r="E86" s="4" t="n"/>
       <c r="F86" s="4" t="n"/>
+      <c r="G86" s="4" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -1899,6 +2105,9 @@
       <c r="F87" s="6" t="n">
         <v>53.01</v>
       </c>
+      <c r="G87" s="6" t="n">
+        <v>51.86</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -1918,6 +2127,9 @@
       </c>
       <c r="F88" s="6" t="n">
         <v>3988.79</v>
+      </c>
+      <c r="G88" s="6" t="n">
+        <v>4117.83</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -1927,6 +2139,7 @@
       <c r="D89" s="1" t="n"/>
       <c r="E89" s="4" t="n"/>
       <c r="F89" s="4" t="n"/>
+      <c r="G89" s="4" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -1947,6 +2160,9 @@
       <c r="F90" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G90" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -1966,6 +2182,9 @@
       </c>
       <c r="F91" s="6" t="n">
         <v>2011.61</v>
+      </c>
+      <c r="G91" s="6" t="n">
+        <v>2075.4</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -1975,6 +2194,7 @@
       <c r="D92" s="1" t="n"/>
       <c r="E92" s="4" t="n"/>
       <c r="F92" s="4" t="n"/>
+      <c r="G92" s="4" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -1995,6 +2215,9 @@
       <c r="F93" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G93" s="6" t="n">
+        <v>28.25</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -2014,6 +2237,9 @@
       </c>
       <c r="F94" s="6" t="n">
         <v>13989.57</v>
+      </c>
+      <c r="G94" s="6" t="n">
+        <v>14198.75</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -2023,6 +2249,7 @@
       <c r="D95" s="1" t="n"/>
       <c r="E95" s="4" t="n"/>
       <c r="F95" s="4" t="n"/>
+      <c r="G95" s="4" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -2043,6 +2270,9 @@
       <c r="F96" s="6" t="n">
         <v>86.64</v>
       </c>
+      <c r="G96" s="6" t="n">
+        <v>85.78</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -2062,6 +2292,9 @@
       </c>
       <c r="F97" s="6" t="n">
         <v>8996.290000000001</v>
+      </c>
+      <c r="G97" s="6" t="n">
+        <v>9121.799999999999</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -2071,6 +2304,7 @@
       <c r="D98" s="1" t="n"/>
       <c r="E98" s="4" t="n"/>
       <c r="F98" s="4" t="n"/>
+      <c r="G98" s="4" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -2091,6 +2325,9 @@
       <c r="F99" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="G99" s="6" t="n">
+        <v>56.31</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -2110,6 +2347,9 @@
       </c>
       <c r="F100" s="6" t="n">
         <v>12116.98</v>
+      </c>
+      <c r="G100" s="6" t="n">
+        <v>12067.47</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -2119,6 +2359,7 @@
       <c r="D101" s="1" t="n"/>
       <c r="E101" s="4" t="n"/>
       <c r="F101" s="4" t="n"/>
+      <c r="G101" s="4" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -2139,6 +2380,9 @@
       <c r="F102" s="6" t="n">
         <v>5.93</v>
       </c>
+      <c r="G102" s="6" t="n">
+        <v>6.14</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -2158,6 +2402,9 @@
       </c>
       <c r="F103" s="6" t="n">
         <v>2317.11</v>
+      </c>
+      <c r="G103" s="6" t="n">
+        <v>2306.9</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -2167,6 +2414,7 @@
       <c r="D104" s="1" t="n"/>
       <c r="E104" s="4" t="n"/>
       <c r="F104" s="4" t="n"/>
+      <c r="G104" s="4" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -2187,6 +2435,9 @@
       <c r="F105" s="6" t="n">
         <v>26</v>
       </c>
+      <c r="G105" s="6" t="n">
+        <v>25.81</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -2206,6 +2457,9 @@
       </c>
       <c r="F106" s="6" t="n">
         <v>882.91</v>
+      </c>
+      <c r="G106" s="6" t="n">
+        <v>873.11</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -2215,6 +2469,7 @@
       <c r="D107" s="1" t="n"/>
       <c r="E107" s="4" t="n"/>
       <c r="F107" s="4" t="n"/>
+      <c r="G107" s="4" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -2235,6 +2490,9 @@
       <c r="F108" s="6" t="n">
         <v>29.59</v>
       </c>
+      <c r="G108" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -2254,6 +2512,9 @@
       </c>
       <c r="F109" s="6" t="n">
         <v>2825.96</v>
+      </c>
+      <c r="G109" s="6" t="n">
+        <v>2925.23</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -2263,6 +2524,7 @@
       <c r="D110" s="1" t="n"/>
       <c r="E110" s="4" t="n"/>
       <c r="F110" s="4" t="n"/>
+      <c r="G110" s="4" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -2283,6 +2545,9 @@
       <c r="F111" s="6" t="n">
         <v>21.5</v>
       </c>
+      <c r="G111" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -2302,6 +2567,9 @@
       </c>
       <c r="F112" s="6" t="n">
         <v>4028.19</v>
+      </c>
+      <c r="G112" s="6" t="n">
+        <v>4021.92</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -2311,6 +2579,7 @@
       <c r="D113" s="1" t="n"/>
       <c r="E113" s="4" t="n"/>
       <c r="F113" s="4" t="n"/>
+      <c r="G113" s="4" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -2331,6 +2600,9 @@
       <c r="F114" s="6" t="n">
         <v>29.02</v>
       </c>
+      <c r="G114" s="6" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -2350,6 +2622,9 @@
       </c>
       <c r="F115" s="6" t="n">
         <v>3350.35</v>
+      </c>
+      <c r="G115" s="6" t="n">
+        <v>3410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-15 02:10:46]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -508,6 +508,11 @@
           <t>2025/11/13</t>
         </is>
       </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>2025/11/15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -545,6 +550,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -568,6 +578,9 @@
       <c r="G3" s="6" t="n">
         <v>63.21</v>
       </c>
+      <c r="H3" s="6" t="n">
+        <v>63.04</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -590,6 +603,9 @@
       </c>
       <c r="G4" s="6" t="n">
         <v>4017.94</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>3990.49</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -600,6 +616,7 @@
       <c r="E5" s="4" t="n"/>
       <c r="F5" s="4" t="n"/>
       <c r="G5" s="4" t="n"/>
+      <c r="H5" s="4" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -623,6 +640,9 @@
       <c r="G6" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H6" s="6" t="n">
+        <v>49.48</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -645,6 +665,9 @@
       </c>
       <c r="G7" s="6" t="n">
         <v>5648.68</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>5563.5</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -655,6 +678,7 @@
       <c r="E8" s="4" t="n"/>
       <c r="F8" s="4" t="n"/>
       <c r="G8" s="4" t="n"/>
+      <c r="H8" s="4" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -678,6 +702,9 @@
       <c r="G9" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H9" s="6" t="n">
+        <v>54.86</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -700,6 +727,9 @@
       </c>
       <c r="G10" s="6" t="n">
         <v>4690.71</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>4628.14</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -710,6 +740,7 @@
       <c r="E11" s="4" t="n"/>
       <c r="F11" s="4" t="n"/>
       <c r="G11" s="4" t="n"/>
+      <c r="H11" s="4" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -733,6 +764,9 @@
       <c r="G12" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H12" s="6" t="n">
+        <v>57.09</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -755,6 +789,9 @@
       </c>
       <c r="G13" s="6" t="n">
         <v>7363.44</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>7235.46</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -765,6 +802,7 @@
       <c r="E14" s="4" t="n"/>
       <c r="F14" s="4" t="n"/>
       <c r="G14" s="4" t="n"/>
+      <c r="H14" s="4" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -788,6 +826,9 @@
       <c r="G15" s="6" t="n">
         <v>29.44</v>
       </c>
+      <c r="H15" s="6" t="n">
+        <v>30.11</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -810,6 +851,9 @@
       </c>
       <c r="G16" s="6" t="n">
         <v>2755.62</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>2724.97</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -820,6 +864,7 @@
       <c r="E17" s="4" t="n"/>
       <c r="F17" s="4" t="n"/>
       <c r="G17" s="4" t="n"/>
+      <c r="H17" s="4" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -843,6 +888,9 @@
       <c r="G18" s="6" t="n">
         <v>96.67</v>
       </c>
+      <c r="H18" s="6" t="n">
+        <v>96.08</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -865,6 +913,9 @@
       </c>
       <c r="G19" s="6" t="n">
         <v>6850.92</v>
+      </c>
+      <c r="H19" s="6" t="n">
+        <v>6734.11</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -875,6 +926,7 @@
       <c r="E20" s="4" t="n"/>
       <c r="F20" s="4" t="n"/>
       <c r="G20" s="4" t="n"/>
+      <c r="H20" s="4" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -898,6 +950,9 @@
       <c r="G21" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H21" s="6" t="n">
+        <v>63.44</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -920,6 +975,9 @@
       </c>
       <c r="G22" s="6" t="n">
         <v>84525.89</v>
+      </c>
+      <c r="H22" s="6" t="n">
+        <v>84562.78</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -930,6 +988,7 @@
       <c r="E23" s="4" t="n"/>
       <c r="F23" s="4" t="n"/>
       <c r="G23" s="4" t="n"/>
+      <c r="H23" s="4" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -953,6 +1012,9 @@
       <c r="G24" s="6" t="n">
         <v>84.14</v>
       </c>
+      <c r="H24" s="6" t="n">
+        <v>84.14</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -974,6 +1036,9 @@
         <v>19909.14</v>
       </c>
       <c r="G25" s="6" t="n">
+        <v>19909.14</v>
+      </c>
+      <c r="H25" s="6" t="n">
         <v>19909.14</v>
       </c>
     </row>
@@ -985,6 +1050,7 @@
       <c r="E26" s="4" t="n"/>
       <c r="F26" s="4" t="n"/>
       <c r="G26" s="4" t="n"/>
+      <c r="H26" s="4" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1008,6 +1074,9 @@
       <c r="G27" s="6" t="n">
         <v>71.64</v>
       </c>
+      <c r="H27" s="6" t="n">
+        <v>71.64</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1029,6 +1098,9 @@
         <v>39894.54</v>
       </c>
       <c r="G28" s="6" t="n">
+        <v>39894.54</v>
+      </c>
+      <c r="H28" s="6" t="n">
         <v>39894.54</v>
       </c>
     </row>
@@ -1040,6 +1112,7 @@
       <c r="E29" s="4" t="n"/>
       <c r="F29" s="4" t="n"/>
       <c r="G29" s="4" t="n"/>
+      <c r="H29" s="4" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1063,6 +1136,9 @@
       <c r="G30" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H30" s="6" t="n">
+        <v>59.08</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1085,6 +1161,9 @@
       </c>
       <c r="G31" s="6" t="n">
         <v>5774</v>
+      </c>
+      <c r="H31" s="6" t="n">
+        <v>5767.56</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1095,6 +1174,7 @@
       <c r="E32" s="4" t="n"/>
       <c r="F32" s="4" t="n"/>
       <c r="G32" s="4" t="n"/>
+      <c r="H32" s="4" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1118,6 +1198,9 @@
       <c r="G33" s="6" t="n">
         <v>12.61</v>
       </c>
+      <c r="H33" s="6" t="n">
+        <v>11.76</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1140,6 +1223,9 @@
       </c>
       <c r="G34" s="6" t="n">
         <v>32685.54</v>
+      </c>
+      <c r="H34" s="6" t="n">
+        <v>32244.89</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1150,6 +1236,7 @@
       <c r="E35" s="4" t="n"/>
       <c r="F35" s="4" t="n"/>
       <c r="G35" s="4" t="n"/>
+      <c r="H35" s="4" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1173,6 +1260,9 @@
       <c r="G36" s="6" t="n">
         <v>28.23</v>
       </c>
+      <c r="H36" s="6" t="n">
+        <v>28.05</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1195,6 +1285,9 @@
       </c>
       <c r="G37" s="6" t="n">
         <v>3381.23</v>
+      </c>
+      <c r="H37" s="6" t="n">
+        <v>3273.7</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1205,6 +1298,7 @@
       <c r="E38" s="4" t="n"/>
       <c r="F38" s="4" t="n"/>
       <c r="G38" s="4" t="n"/>
+      <c r="H38" s="4" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1228,6 +1322,9 @@
       <c r="G39" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H39" s="6" t="n">
+        <v>45.7</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1250,6 +1347,9 @@
       </c>
       <c r="G40" s="6" t="n">
         <v>3205.76</v>
+      </c>
+      <c r="H40" s="6" t="n">
+        <v>3111.51</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1260,6 +1360,7 @@
       <c r="E41" s="4" t="n"/>
       <c r="F41" s="4" t="n"/>
       <c r="G41" s="4" t="n"/>
+      <c r="H41" s="4" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1283,6 +1384,9 @@
       <c r="G42" s="6" t="n">
         <v>18.21</v>
       </c>
+      <c r="H42" s="6" t="n">
+        <v>18.22</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1305,6 +1409,9 @@
       </c>
       <c r="G43" s="6" t="n">
         <v>7305.09</v>
+      </c>
+      <c r="H43" s="6" t="n">
+        <v>7271.82</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1315,6 +1422,7 @@
       <c r="E44" s="4" t="n"/>
       <c r="F44" s="4" t="n"/>
       <c r="G44" s="4" t="n"/>
+      <c r="H44" s="4" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1338,6 +1446,9 @@
       <c r="G45" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H45" s="6" t="n">
+        <v>31.57</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1360,6 +1471,9 @@
       </c>
       <c r="G46" s="6" t="n">
         <v>8880.959999999999</v>
+      </c>
+      <c r="H46" s="6" t="n">
+        <v>8839.17</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1370,6 +1484,7 @@
       <c r="E47" s="4" t="n"/>
       <c r="F47" s="4" t="n"/>
       <c r="G47" s="4" t="n"/>
+      <c r="H47" s="4" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1393,6 +1508,9 @@
       <c r="G48" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H48" s="6" t="n">
+        <v>13.62</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1415,6 +1533,9 @@
       </c>
       <c r="G49" s="6" t="n">
         <v>13055.99</v>
+      </c>
+      <c r="H49" s="6" t="n">
+        <v>12977.24</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1425,6 +1546,7 @@
       <c r="E50" s="4" t="n"/>
       <c r="F50" s="4" t="n"/>
       <c r="G50" s="4" t="n"/>
+      <c r="H50" s="4" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1448,6 +1570,9 @@
       <c r="G51" s="6" t="n">
         <v>26.04</v>
       </c>
+      <c r="H51" s="6" t="n">
+        <v>25.01</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -1470,6 +1595,9 @@
       </c>
       <c r="G52" s="6" t="n">
         <v>12603.71</v>
+      </c>
+      <c r="H52" s="6" t="n">
+        <v>12439.99</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1480,6 +1608,7 @@
       <c r="E53" s="4" t="n"/>
       <c r="F53" s="4" t="n"/>
       <c r="G53" s="4" t="n"/>
+      <c r="H53" s="4" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -1503,6 +1632,9 @@
       <c r="G54" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H54" s="6" t="n">
+        <v>22.95</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -1525,6 +1657,9 @@
       </c>
       <c r="G55" s="6" t="n">
         <v>10004.5</v>
+      </c>
+      <c r="H55" s="6" t="n">
+        <v>9937.41</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -1535,6 +1670,7 @@
       <c r="E56" s="4" t="n"/>
       <c r="F56" s="4" t="n"/>
       <c r="G56" s="4" t="n"/>
+      <c r="H56" s="4" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -1558,6 +1694,9 @@
       <c r="G57" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H57" s="6" t="n">
+        <v>27.41</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -1580,6 +1719,9 @@
       </c>
       <c r="G58" s="6" t="n">
         <v>16387.97</v>
+      </c>
+      <c r="H58" s="6" t="n">
+        <v>16333.64</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -1590,6 +1732,7 @@
       <c r="E59" s="4" t="n"/>
       <c r="F59" s="4" t="n"/>
       <c r="G59" s="4" t="n"/>
+      <c r="H59" s="4" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -1613,6 +1756,9 @@
       <c r="G60" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H60" s="6" t="n">
+        <v>32.83</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -1634,6 +1780,9 @@
         <v>17526.85</v>
       </c>
       <c r="G61" s="6" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="H61" s="6" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1645,6 +1794,7 @@
       <c r="E62" s="4" t="n"/>
       <c r="F62" s="4" t="n"/>
       <c r="G62" s="4" t="n"/>
+      <c r="H62" s="4" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -1668,6 +1818,9 @@
       <c r="G63" s="6" t="n">
         <v>21.11</v>
       </c>
+      <c r="H63" s="6" t="n">
+        <v>21.07</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -1690,6 +1843,9 @@
       </c>
       <c r="G64" s="6" t="n">
         <v>10214.48</v>
+      </c>
+      <c r="H64" s="6" t="n">
+        <v>10102.71</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -1700,6 +1856,7 @@
       <c r="E65" s="4" t="n"/>
       <c r="F65" s="4" t="n"/>
       <c r="G65" s="4" t="n"/>
+      <c r="H65" s="4" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -1723,6 +1880,9 @@
       <c r="G66" s="6" t="n">
         <v>19.06</v>
       </c>
+      <c r="H66" s="6" t="n">
+        <v>19.84</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -1745,6 +1905,9 @@
       </c>
       <c r="G67" s="6" t="n">
         <v>10219.1</v>
+      </c>
+      <c r="H67" s="6" t="n">
+        <v>10352.68</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -1755,6 +1918,7 @@
       <c r="E68" s="4" t="n"/>
       <c r="F68" s="4" t="n"/>
       <c r="G68" s="4" t="n"/>
+      <c r="H68" s="4" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -1778,6 +1942,9 @@
       <c r="G69" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H69" s="6" t="n">
+        <v>21.2</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -1800,6 +1967,9 @@
       </c>
       <c r="G70" s="6" t="n">
         <v>3100.16</v>
+      </c>
+      <c r="H70" s="6" t="n">
+        <v>3044.37</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -1810,6 +1980,7 @@
       <c r="E71" s="4" t="n"/>
       <c r="F71" s="4" t="n"/>
       <c r="G71" s="4" t="n"/>
+      <c r="H71" s="4" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -1833,6 +2004,9 @@
       <c r="G72" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H72" s="6" t="n">
+        <v>42.42</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -1855,6 +2029,9 @@
       </c>
       <c r="G73" s="6" t="n">
         <v>5886.87</v>
+      </c>
+      <c r="H73" s="6" t="n">
+        <v>5812.8</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -1865,6 +2042,7 @@
       <c r="E74" s="4" t="n"/>
       <c r="F74" s="4" t="n"/>
       <c r="G74" s="4" t="n"/>
+      <c r="H74" s="4" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -1888,6 +2066,9 @@
       <c r="G75" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H75" s="6" t="n">
+        <v>28.12</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -1910,6 +2091,9 @@
       </c>
       <c r="G76" s="6" t="n">
         <v>9468.610000000001</v>
+      </c>
+      <c r="H76" s="6" t="n">
+        <v>9447.07</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -1920,6 +2104,7 @@
       <c r="E77" s="4" t="n"/>
       <c r="F77" s="4" t="n"/>
       <c r="G77" s="4" t="n"/>
+      <c r="H77" s="4" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -1943,6 +2128,9 @@
       <c r="G78" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H78" s="6" t="n">
+        <v>13.78</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -1965,6 +2153,9 @@
       </c>
       <c r="G79" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="H79" s="6" t="n">
+        <v>1352.41</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -1975,6 +2166,7 @@
       <c r="E80" s="4" t="n"/>
       <c r="F80" s="4" t="n"/>
       <c r="G80" s="4" t="n"/>
+      <c r="H80" s="4" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -1998,6 +2190,9 @@
       <c r="G81" s="6" t="n">
         <v>56.04</v>
       </c>
+      <c r="H81" s="6" t="n">
+        <v>56.98</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -2020,6 +2215,9 @@
       </c>
       <c r="G82" s="6" t="n">
         <v>3076.44</v>
+      </c>
+      <c r="H82" s="6" t="n">
+        <v>3004.11</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -2030,6 +2228,7 @@
       <c r="E83" s="4" t="n"/>
       <c r="F83" s="4" t="n"/>
       <c r="G83" s="4" t="n"/>
+      <c r="H83" s="4" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -2053,6 +2252,9 @@
       <c r="G84" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H84" s="6" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -2075,6 +2277,9 @@
       </c>
       <c r="G85" s="6" t="n">
         <v>3158.76</v>
+      </c>
+      <c r="H85" s="6" t="n">
+        <v>3101.34</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -2085,6 +2290,7 @@
       <c r="E86" s="4" t="n"/>
       <c r="F86" s="4" t="n"/>
       <c r="G86" s="4" t="n"/>
+      <c r="H86" s="4" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -2108,6 +2314,9 @@
       <c r="G87" s="6" t="n">
         <v>51.86</v>
       </c>
+      <c r="H87" s="6" t="n">
+        <v>53.31</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -2130,6 +2339,9 @@
       </c>
       <c r="G88" s="6" t="n">
         <v>4117.83</v>
+      </c>
+      <c r="H88" s="6" t="n">
+        <v>4001.16</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -2140,6 +2352,7 @@
       <c r="E89" s="4" t="n"/>
       <c r="F89" s="4" t="n"/>
       <c r="G89" s="4" t="n"/>
+      <c r="H89" s="4" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -2163,6 +2376,9 @@
       <c r="G90" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H90" s="6" t="n">
+        <v>45.31</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -2185,6 +2401,9 @@
       </c>
       <c r="G91" s="6" t="n">
         <v>2075.4</v>
+      </c>
+      <c r="H91" s="6" t="n">
+        <v>2073.7</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -2195,6 +2414,7 @@
       <c r="E92" s="4" t="n"/>
       <c r="F92" s="4" t="n"/>
       <c r="G92" s="4" t="n"/>
+      <c r="H92" s="4" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -2218,6 +2438,9 @@
       <c r="G93" s="6" t="n">
         <v>28.25</v>
       </c>
+      <c r="H93" s="6" t="n">
+        <v>28.18</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -2240,6 +2463,9 @@
       </c>
       <c r="G94" s="6" t="n">
         <v>14198.75</v>
+      </c>
+      <c r="H94" s="6" t="n">
+        <v>14255.82</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -2250,6 +2476,7 @@
       <c r="E95" s="4" t="n"/>
       <c r="F95" s="4" t="n"/>
       <c r="G95" s="4" t="n"/>
+      <c r="H95" s="4" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -2273,6 +2500,9 @@
       <c r="G96" s="6" t="n">
         <v>85.78</v>
       </c>
+      <c r="H96" s="6" t="n">
+        <v>84.89</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -2295,6 +2525,9 @@
       </c>
       <c r="G97" s="6" t="n">
         <v>9121.799999999999</v>
+      </c>
+      <c r="H97" s="6" t="n">
+        <v>8787.389999999999</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -2305,6 +2538,7 @@
       <c r="E98" s="4" t="n"/>
       <c r="F98" s="4" t="n"/>
       <c r="G98" s="4" t="n"/>
+      <c r="H98" s="4" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -2328,6 +2562,9 @@
       <c r="G99" s="6" t="n">
         <v>56.31</v>
       </c>
+      <c r="H99" s="6" t="n">
+        <v>56.35</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -2350,6 +2587,9 @@
       </c>
       <c r="G100" s="6" t="n">
         <v>12067.47</v>
+      </c>
+      <c r="H100" s="6" t="n">
+        <v>11962.63</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -2360,6 +2600,7 @@
       <c r="E101" s="4" t="n"/>
       <c r="F101" s="4" t="n"/>
       <c r="G101" s="4" t="n"/>
+      <c r="H101" s="4" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -2383,6 +2624,9 @@
       <c r="G102" s="6" t="n">
         <v>6.14</v>
       </c>
+      <c r="H102" s="6" t="n">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -2405,6 +2649,9 @@
       </c>
       <c r="G103" s="6" t="n">
         <v>2306.9</v>
+      </c>
+      <c r="H103" s="6" t="n">
+        <v>2312.06</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -2415,6 +2662,7 @@
       <c r="E104" s="4" t="n"/>
       <c r="F104" s="4" t="n"/>
       <c r="G104" s="4" t="n"/>
+      <c r="H104" s="4" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -2438,6 +2686,9 @@
       <c r="G105" s="6" t="n">
         <v>25.81</v>
       </c>
+      <c r="H105" s="6" t="n">
+        <v>25.74</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -2460,6 +2711,9 @@
       </c>
       <c r="G106" s="6" t="n">
         <v>873.11</v>
+      </c>
+      <c r="H106" s="6" t="n">
+        <v>866.77</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -2470,6 +2724,7 @@
       <c r="E107" s="4" t="n"/>
       <c r="F107" s="4" t="n"/>
       <c r="G107" s="4" t="n"/>
+      <c r="H107" s="4" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -2493,6 +2748,9 @@
       <c r="G108" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H108" s="6" t="n">
+        <v>29.67</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -2515,6 +2773,9 @@
       </c>
       <c r="G109" s="6" t="n">
         <v>2925.23</v>
+      </c>
+      <c r="H109" s="6" t="n">
+        <v>2844.63</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -2525,6 +2786,7 @@
       <c r="E110" s="4" t="n"/>
       <c r="F110" s="4" t="n"/>
       <c r="G110" s="4" t="n"/>
+      <c r="H110" s="4" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -2548,6 +2810,9 @@
       <c r="G111" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="H111" s="6" t="n">
+        <v>21.18</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -2570,6 +2835,9 @@
       </c>
       <c r="G112" s="6" t="n">
         <v>4021.92</v>
+      </c>
+      <c r="H112" s="6" t="n">
+        <v>3985</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -2580,6 +2848,7 @@
       <c r="E113" s="4" t="n"/>
       <c r="F113" s="4" t="n"/>
       <c r="G113" s="4" t="n"/>
+      <c r="H113" s="4" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -2603,6 +2872,9 @@
       <c r="G114" s="6" t="n">
         <v>29.02</v>
       </c>
+      <c r="H114" s="6" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -2625,6 +2897,9 @@
       </c>
       <c r="G115" s="6" t="n">
         <v>3410</v>
+      </c>
+      <c r="H115" s="6" t="n">
+        <v>3409.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-15 03:50:58]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -465,11 +465,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="4"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="1" max="4"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -513,6 +517,11 @@
           <t>2025/11/15</t>
         </is>
       </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>2025/11/15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -555,6 +564,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -581,6 +595,9 @@
       <c r="H3" s="6" t="n">
         <v>63.04</v>
       </c>
+      <c r="I3" s="6" t="n">
+        <v>63.04</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -605,6 +622,9 @@
         <v>4017.94</v>
       </c>
       <c r="H4" s="6" t="n">
+        <v>3990.49</v>
+      </c>
+      <c r="I4" s="6" t="n">
         <v>3990.49</v>
       </c>
     </row>
@@ -617,6 +637,7 @@
       <c r="F5" s="4" t="n"/>
       <c r="G5" s="4" t="n"/>
       <c r="H5" s="4" t="n"/>
+      <c r="I5" s="4" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -643,6 +664,9 @@
       <c r="H6" s="6" t="n">
         <v>49.48</v>
       </c>
+      <c r="I6" s="6" t="n">
+        <v>49.48</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -667,6 +691,9 @@
         <v>5648.68</v>
       </c>
       <c r="H7" s="6" t="n">
+        <v>5563.5</v>
+      </c>
+      <c r="I7" s="6" t="n">
         <v>5563.5</v>
       </c>
     </row>
@@ -679,6 +706,7 @@
       <c r="F8" s="4" t="n"/>
       <c r="G8" s="4" t="n"/>
       <c r="H8" s="4" t="n"/>
+      <c r="I8" s="4" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -705,6 +733,9 @@
       <c r="H9" s="6" t="n">
         <v>54.86</v>
       </c>
+      <c r="I9" s="6" t="n">
+        <v>54.86</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -729,6 +760,9 @@
         <v>4690.71</v>
       </c>
       <c r="H10" s="6" t="n">
+        <v>4628.14</v>
+      </c>
+      <c r="I10" s="6" t="n">
         <v>4628.14</v>
       </c>
     </row>
@@ -741,6 +775,7 @@
       <c r="F11" s="4" t="n"/>
       <c r="G11" s="4" t="n"/>
       <c r="H11" s="4" t="n"/>
+      <c r="I11" s="4" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -767,6 +802,9 @@
       <c r="H12" s="6" t="n">
         <v>57.09</v>
       </c>
+      <c r="I12" s="6" t="n">
+        <v>57.09</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -791,6 +829,9 @@
         <v>7363.44</v>
       </c>
       <c r="H13" s="6" t="n">
+        <v>7235.46</v>
+      </c>
+      <c r="I13" s="6" t="n">
         <v>7235.46</v>
       </c>
     </row>
@@ -803,6 +844,7 @@
       <c r="F14" s="4" t="n"/>
       <c r="G14" s="4" t="n"/>
       <c r="H14" s="4" t="n"/>
+      <c r="I14" s="4" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -829,6 +871,9 @@
       <c r="H15" s="6" t="n">
         <v>30.11</v>
       </c>
+      <c r="I15" s="6" t="n">
+        <v>28.22</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -853,6 +898,9 @@
         <v>2755.62</v>
       </c>
       <c r="H16" s="6" t="n">
+        <v>2724.97</v>
+      </c>
+      <c r="I16" s="6" t="n">
         <v>2724.97</v>
       </c>
     </row>
@@ -865,6 +913,7 @@
       <c r="F17" s="4" t="n"/>
       <c r="G17" s="4" t="n"/>
       <c r="H17" s="4" t="n"/>
+      <c r="I17" s="4" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -891,6 +940,9 @@
       <c r="H18" s="6" t="n">
         <v>96.08</v>
       </c>
+      <c r="I18" s="6" t="n">
+        <v>96.06</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -915,6 +967,9 @@
         <v>6850.92</v>
       </c>
       <c r="H19" s="6" t="n">
+        <v>6734.11</v>
+      </c>
+      <c r="I19" s="6" t="n">
         <v>6734.11</v>
       </c>
     </row>
@@ -927,6 +982,7 @@
       <c r="F20" s="4" t="n"/>
       <c r="G20" s="4" t="n"/>
       <c r="H20" s="4" t="n"/>
+      <c r="I20" s="4" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -953,6 +1009,9 @@
       <c r="H21" s="6" t="n">
         <v>63.44</v>
       </c>
+      <c r="I21" s="6" t="n">
+        <v>65.04000000000001</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -977,6 +1036,9 @@
         <v>84525.89</v>
       </c>
       <c r="H22" s="6" t="n">
+        <v>84562.78</v>
+      </c>
+      <c r="I22" s="6" t="n">
         <v>84562.78</v>
       </c>
     </row>
@@ -989,6 +1051,7 @@
       <c r="F23" s="4" t="n"/>
       <c r="G23" s="4" t="n"/>
       <c r="H23" s="4" t="n"/>
+      <c r="I23" s="4" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1015,6 +1078,9 @@
       <c r="H24" s="6" t="n">
         <v>84.14</v>
       </c>
+      <c r="I24" s="6" t="n">
+        <v>85.41</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1039,6 +1105,9 @@
         <v>19909.14</v>
       </c>
       <c r="H25" s="6" t="n">
+        <v>19909.14</v>
+      </c>
+      <c r="I25" s="6" t="n">
         <v>19909.14</v>
       </c>
     </row>
@@ -1051,6 +1120,7 @@
       <c r="F26" s="4" t="n"/>
       <c r="G26" s="4" t="n"/>
       <c r="H26" s="4" t="n"/>
+      <c r="I26" s="4" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1077,6 +1147,9 @@
       <c r="H27" s="6" t="n">
         <v>71.64</v>
       </c>
+      <c r="I27" s="6" t="n">
+        <v>71.84999999999999</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1101,6 +1174,9 @@
         <v>39894.54</v>
       </c>
       <c r="H28" s="6" t="n">
+        <v>39894.54</v>
+      </c>
+      <c r="I28" s="6" t="n">
         <v>39894.54</v>
       </c>
     </row>
@@ -1113,6 +1189,7 @@
       <c r="F29" s="4" t="n"/>
       <c r="G29" s="4" t="n"/>
       <c r="H29" s="4" t="n"/>
+      <c r="I29" s="4" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1139,6 +1216,9 @@
       <c r="H30" s="6" t="n">
         <v>59.08</v>
       </c>
+      <c r="I30" s="6" t="n">
+        <v>59.08</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1163,6 +1243,9 @@
         <v>5774</v>
       </c>
       <c r="H31" s="6" t="n">
+        <v>5767.56</v>
+      </c>
+      <c r="I31" s="6" t="n">
         <v>5767.56</v>
       </c>
     </row>
@@ -1175,6 +1258,7 @@
       <c r="F32" s="4" t="n"/>
       <c r="G32" s="4" t="n"/>
       <c r="H32" s="4" t="n"/>
+      <c r="I32" s="4" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1201,6 +1285,9 @@
       <c r="H33" s="6" t="n">
         <v>11.76</v>
       </c>
+      <c r="I33" s="6" t="n">
+        <v>11.76</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1225,6 +1312,9 @@
         <v>32685.54</v>
       </c>
       <c r="H34" s="6" t="n">
+        <v>32244.89</v>
+      </c>
+      <c r="I34" s="6" t="n">
         <v>32244.89</v>
       </c>
     </row>
@@ -1237,6 +1327,7 @@
       <c r="F35" s="4" t="n"/>
       <c r="G35" s="4" t="n"/>
       <c r="H35" s="4" t="n"/>
+      <c r="I35" s="4" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1263,6 +1354,9 @@
       <c r="H36" s="6" t="n">
         <v>28.05</v>
       </c>
+      <c r="I36" s="6" t="n">
+        <v>28.05</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1287,6 +1381,9 @@
         <v>3381.23</v>
       </c>
       <c r="H37" s="6" t="n">
+        <v>3273.7</v>
+      </c>
+      <c r="I37" s="6" t="n">
         <v>3273.7</v>
       </c>
     </row>
@@ -1299,6 +1396,7 @@
       <c r="F38" s="4" t="n"/>
       <c r="G38" s="4" t="n"/>
       <c r="H38" s="4" t="n"/>
+      <c r="I38" s="4" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1325,6 +1423,9 @@
       <c r="H39" s="6" t="n">
         <v>45.7</v>
       </c>
+      <c r="I39" s="6" t="n">
+        <v>45.7</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1349,6 +1450,9 @@
         <v>3205.76</v>
       </c>
       <c r="H40" s="6" t="n">
+        <v>3111.51</v>
+      </c>
+      <c r="I40" s="6" t="n">
         <v>3111.51</v>
       </c>
     </row>
@@ -1361,6 +1465,7 @@
       <c r="F41" s="4" t="n"/>
       <c r="G41" s="4" t="n"/>
       <c r="H41" s="4" t="n"/>
+      <c r="I41" s="4" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1387,6 +1492,9 @@
       <c r="H42" s="6" t="n">
         <v>18.22</v>
       </c>
+      <c r="I42" s="6" t="n">
+        <v>18.22</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1411,6 +1519,9 @@
         <v>7305.09</v>
       </c>
       <c r="H43" s="6" t="n">
+        <v>7271.82</v>
+      </c>
+      <c r="I43" s="6" t="n">
         <v>7271.82</v>
       </c>
     </row>
@@ -1423,6 +1534,7 @@
       <c r="F44" s="4" t="n"/>
       <c r="G44" s="4" t="n"/>
       <c r="H44" s="4" t="n"/>
+      <c r="I44" s="4" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1449,6 +1561,9 @@
       <c r="H45" s="6" t="n">
         <v>31.57</v>
       </c>
+      <c r="I45" s="6" t="n">
+        <v>31.57</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1473,6 +1588,9 @@
         <v>8880.959999999999</v>
       </c>
       <c r="H46" s="6" t="n">
+        <v>8839.17</v>
+      </c>
+      <c r="I46" s="6" t="n">
         <v>8839.17</v>
       </c>
     </row>
@@ -1485,6 +1603,7 @@
       <c r="F47" s="4" t="n"/>
       <c r="G47" s="4" t="n"/>
       <c r="H47" s="4" t="n"/>
+      <c r="I47" s="4" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1511,6 +1630,9 @@
       <c r="H48" s="6" t="n">
         <v>13.62</v>
       </c>
+      <c r="I48" s="6" t="n">
+        <v>13.62</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1535,6 +1657,9 @@
         <v>13055.99</v>
       </c>
       <c r="H49" s="6" t="n">
+        <v>12977.24</v>
+      </c>
+      <c r="I49" s="6" t="n">
         <v>12977.24</v>
       </c>
     </row>
@@ -1547,6 +1672,7 @@
       <c r="F50" s="4" t="n"/>
       <c r="G50" s="4" t="n"/>
       <c r="H50" s="4" t="n"/>
+      <c r="I50" s="4" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1573,6 +1699,9 @@
       <c r="H51" s="6" t="n">
         <v>25.01</v>
       </c>
+      <c r="I51" s="6" t="n">
+        <v>25.01</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -1597,6 +1726,9 @@
         <v>12603.71</v>
       </c>
       <c r="H52" s="6" t="n">
+        <v>12439.99</v>
+      </c>
+      <c r="I52" s="6" t="n">
         <v>12439.99</v>
       </c>
     </row>
@@ -1609,6 +1741,7 @@
       <c r="F53" s="4" t="n"/>
       <c r="G53" s="4" t="n"/>
       <c r="H53" s="4" t="n"/>
+      <c r="I53" s="4" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -1635,6 +1768,9 @@
       <c r="H54" s="6" t="n">
         <v>22.95</v>
       </c>
+      <c r="I54" s="6" t="n">
+        <v>22.95</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -1659,6 +1795,9 @@
         <v>10004.5</v>
       </c>
       <c r="H55" s="6" t="n">
+        <v>9937.41</v>
+      </c>
+      <c r="I55" s="6" t="n">
         <v>9937.41</v>
       </c>
     </row>
@@ -1671,6 +1810,7 @@
       <c r="F56" s="4" t="n"/>
       <c r="G56" s="4" t="n"/>
       <c r="H56" s="4" t="n"/>
+      <c r="I56" s="4" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -1697,6 +1837,9 @@
       <c r="H57" s="6" t="n">
         <v>27.41</v>
       </c>
+      <c r="I57" s="6" t="n">
+        <v>27.41</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -1721,6 +1864,9 @@
         <v>16387.97</v>
       </c>
       <c r="H58" s="6" t="n">
+        <v>16333.64</v>
+      </c>
+      <c r="I58" s="6" t="n">
         <v>16333.64</v>
       </c>
     </row>
@@ -1733,6 +1879,7 @@
       <c r="F59" s="4" t="n"/>
       <c r="G59" s="4" t="n"/>
       <c r="H59" s="4" t="n"/>
+      <c r="I59" s="4" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -1759,6 +1906,9 @@
       <c r="H60" s="6" t="n">
         <v>32.83</v>
       </c>
+      <c r="I60" s="6" t="n">
+        <v>32.67</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -1783,6 +1933,9 @@
         <v>17526.85</v>
       </c>
       <c r="H61" s="6" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="I61" s="6" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1795,6 +1948,7 @@
       <c r="F62" s="4" t="n"/>
       <c r="G62" s="4" t="n"/>
       <c r="H62" s="4" t="n"/>
+      <c r="I62" s="4" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -1821,6 +1975,9 @@
       <c r="H63" s="6" t="n">
         <v>21.07</v>
       </c>
+      <c r="I63" s="6" t="n">
+        <v>20.09</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -1845,6 +2002,9 @@
         <v>10214.48</v>
       </c>
       <c r="H64" s="6" t="n">
+        <v>10102.71</v>
+      </c>
+      <c r="I64" s="6" t="n">
         <v>10102.71</v>
       </c>
     </row>
@@ -1857,6 +2017,7 @@
       <c r="F65" s="4" t="n"/>
       <c r="G65" s="4" t="n"/>
       <c r="H65" s="4" t="n"/>
+      <c r="I65" s="4" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -1883,6 +2044,9 @@
       <c r="H66" s="6" t="n">
         <v>19.84</v>
       </c>
+      <c r="I66" s="6" t="n">
+        <v>19.84</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -1907,6 +2071,9 @@
         <v>10219.1</v>
       </c>
       <c r="H67" s="6" t="n">
+        <v>10352.68</v>
+      </c>
+      <c r="I67" s="6" t="n">
         <v>10352.68</v>
       </c>
     </row>
@@ -1919,6 +2086,7 @@
       <c r="F68" s="4" t="n"/>
       <c r="G68" s="4" t="n"/>
       <c r="H68" s="4" t="n"/>
+      <c r="I68" s="4" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -1945,6 +2113,9 @@
       <c r="H69" s="6" t="n">
         <v>21.2</v>
       </c>
+      <c r="I69" s="6" t="n">
+        <v>20.04</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -1969,6 +2140,9 @@
         <v>3100.16</v>
       </c>
       <c r="H70" s="6" t="n">
+        <v>3044.37</v>
+      </c>
+      <c r="I70" s="6" t="n">
         <v>3044.37</v>
       </c>
     </row>
@@ -1981,6 +2155,7 @@
       <c r="F71" s="4" t="n"/>
       <c r="G71" s="4" t="n"/>
       <c r="H71" s="4" t="n"/>
+      <c r="I71" s="4" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -2007,6 +2182,9 @@
       <c r="H72" s="6" t="n">
         <v>42.42</v>
       </c>
+      <c r="I72" s="6" t="n">
+        <v>42.42</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -2031,6 +2209,9 @@
         <v>5886.87</v>
       </c>
       <c r="H73" s="6" t="n">
+        <v>5812.8</v>
+      </c>
+      <c r="I73" s="6" t="n">
         <v>5812.8</v>
       </c>
     </row>
@@ -2043,6 +2224,7 @@
       <c r="F74" s="4" t="n"/>
       <c r="G74" s="4" t="n"/>
       <c r="H74" s="4" t="n"/>
+      <c r="I74" s="4" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -2069,6 +2251,9 @@
       <c r="H75" s="6" t="n">
         <v>28.12</v>
       </c>
+      <c r="I75" s="6" t="n">
+        <v>28.12</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -2093,6 +2278,9 @@
         <v>9468.610000000001</v>
       </c>
       <c r="H76" s="6" t="n">
+        <v>9447.07</v>
+      </c>
+      <c r="I76" s="6" t="n">
         <v>9447.07</v>
       </c>
     </row>
@@ -2105,6 +2293,7 @@
       <c r="F77" s="4" t="n"/>
       <c r="G77" s="4" t="n"/>
       <c r="H77" s="4" t="n"/>
+      <c r="I77" s="4" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -2131,6 +2320,9 @@
       <c r="H78" s="6" t="n">
         <v>13.78</v>
       </c>
+      <c r="I78" s="6" t="n">
+        <v>13.78</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -2155,6 +2347,9 @@
         <v>0</v>
       </c>
       <c r="H79" s="6" t="n">
+        <v>1352.41</v>
+      </c>
+      <c r="I79" s="6" t="n">
         <v>1352.41</v>
       </c>
     </row>
@@ -2167,6 +2362,7 @@
       <c r="F80" s="4" t="n"/>
       <c r="G80" s="4" t="n"/>
       <c r="H80" s="4" t="n"/>
+      <c r="I80" s="4" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -2193,6 +2389,9 @@
       <c r="H81" s="6" t="n">
         <v>56.98</v>
       </c>
+      <c r="I81" s="6" t="n">
+        <v>56.98</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -2217,6 +2416,9 @@
         <v>3076.44</v>
       </c>
       <c r="H82" s="6" t="n">
+        <v>3004.11</v>
+      </c>
+      <c r="I82" s="6" t="n">
         <v>3004.11</v>
       </c>
     </row>
@@ -2229,6 +2431,7 @@
       <c r="F83" s="4" t="n"/>
       <c r="G83" s="4" t="n"/>
       <c r="H83" s="4" t="n"/>
+      <c r="I83" s="4" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -2255,6 +2458,9 @@
       <c r="H84" s="6" t="n">
         <v>58.79</v>
       </c>
+      <c r="I84" s="6" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -2279,6 +2485,9 @@
         <v>3158.76</v>
       </c>
       <c r="H85" s="6" t="n">
+        <v>3101.34</v>
+      </c>
+      <c r="I85" s="6" t="n">
         <v>3101.34</v>
       </c>
     </row>
@@ -2291,6 +2500,7 @@
       <c r="F86" s="4" t="n"/>
       <c r="G86" s="4" t="n"/>
       <c r="H86" s="4" t="n"/>
+      <c r="I86" s="4" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -2317,6 +2527,9 @@
       <c r="H87" s="6" t="n">
         <v>53.31</v>
       </c>
+      <c r="I87" s="6" t="n">
+        <v>53.31</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -2341,6 +2554,9 @@
         <v>4117.83</v>
       </c>
       <c r="H88" s="6" t="n">
+        <v>4001.16</v>
+      </c>
+      <c r="I88" s="6" t="n">
         <v>4001.16</v>
       </c>
     </row>
@@ -2353,6 +2569,7 @@
       <c r="F89" s="4" t="n"/>
       <c r="G89" s="4" t="n"/>
       <c r="H89" s="4" t="n"/>
+      <c r="I89" s="4" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -2379,6 +2596,9 @@
       <c r="H90" s="6" t="n">
         <v>45.31</v>
       </c>
+      <c r="I90" s="6" t="n">
+        <v>45.31</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -2403,6 +2623,9 @@
         <v>2075.4</v>
       </c>
       <c r="H91" s="6" t="n">
+        <v>2073.7</v>
+      </c>
+      <c r="I91" s="6" t="n">
         <v>2073.7</v>
       </c>
     </row>
@@ -2415,6 +2638,7 @@
       <c r="F92" s="4" t="n"/>
       <c r="G92" s="4" t="n"/>
       <c r="H92" s="4" t="n"/>
+      <c r="I92" s="4" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -2441,6 +2665,9 @@
       <c r="H93" s="6" t="n">
         <v>28.18</v>
       </c>
+      <c r="I93" s="6" t="n">
+        <v>28.18</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -2465,6 +2692,9 @@
         <v>14198.75</v>
       </c>
       <c r="H94" s="6" t="n">
+        <v>14255.82</v>
+      </c>
+      <c r="I94" s="6" t="n">
         <v>14255.82</v>
       </c>
     </row>
@@ -2477,6 +2707,7 @@
       <c r="F95" s="4" t="n"/>
       <c r="G95" s="4" t="n"/>
       <c r="H95" s="4" t="n"/>
+      <c r="I95" s="4" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -2503,6 +2734,9 @@
       <c r="H96" s="6" t="n">
         <v>84.89</v>
       </c>
+      <c r="I96" s="6" t="n">
+        <v>84.89</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -2527,6 +2761,9 @@
         <v>9121.799999999999</v>
       </c>
       <c r="H97" s="6" t="n">
+        <v>8787.389999999999</v>
+      </c>
+      <c r="I97" s="6" t="n">
         <v>8787.389999999999</v>
       </c>
     </row>
@@ -2539,6 +2776,7 @@
       <c r="F98" s="4" t="n"/>
       <c r="G98" s="4" t="n"/>
       <c r="H98" s="4" t="n"/>
+      <c r="I98" s="4" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -2565,6 +2803,9 @@
       <c r="H99" s="6" t="n">
         <v>56.35</v>
       </c>
+      <c r="I99" s="6" t="n">
+        <v>56.35</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -2589,6 +2830,9 @@
         <v>12067.47</v>
       </c>
       <c r="H100" s="6" t="n">
+        <v>11962.63</v>
+      </c>
+      <c r="I100" s="6" t="n">
         <v>11962.63</v>
       </c>
     </row>
@@ -2601,6 +2845,7 @@
       <c r="F101" s="4" t="n"/>
       <c r="G101" s="4" t="n"/>
       <c r="H101" s="4" t="n"/>
+      <c r="I101" s="4" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -2627,6 +2872,9 @@
       <c r="H102" s="6" t="n">
         <v>6.1</v>
       </c>
+      <c r="I102" s="6" t="n">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -2651,6 +2899,9 @@
         <v>2306.9</v>
       </c>
       <c r="H103" s="6" t="n">
+        <v>2312.06</v>
+      </c>
+      <c r="I103" s="6" t="n">
         <v>2312.06</v>
       </c>
     </row>
@@ -2663,6 +2914,7 @@
       <c r="F104" s="4" t="n"/>
       <c r="G104" s="4" t="n"/>
       <c r="H104" s="4" t="n"/>
+      <c r="I104" s="4" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -2689,6 +2941,9 @@
       <c r="H105" s="6" t="n">
         <v>25.74</v>
       </c>
+      <c r="I105" s="6" t="n">
+        <v>25.74</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -2713,6 +2968,9 @@
         <v>873.11</v>
       </c>
       <c r="H106" s="6" t="n">
+        <v>866.77</v>
+      </c>
+      <c r="I106" s="6" t="n">
         <v>866.77</v>
       </c>
     </row>
@@ -2725,6 +2983,7 @@
       <c r="F107" s="4" t="n"/>
       <c r="G107" s="4" t="n"/>
       <c r="H107" s="4" t="n"/>
+      <c r="I107" s="4" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -2751,6 +3010,9 @@
       <c r="H108" s="6" t="n">
         <v>29.67</v>
       </c>
+      <c r="I108" s="6" t="n">
+        <v>29.67</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -2775,6 +3037,9 @@
         <v>2925.23</v>
       </c>
       <c r="H109" s="6" t="n">
+        <v>2844.63</v>
+      </c>
+      <c r="I109" s="6" t="n">
         <v>2844.63</v>
       </c>
     </row>
@@ -2787,6 +3052,7 @@
       <c r="F110" s="4" t="n"/>
       <c r="G110" s="4" t="n"/>
       <c r="H110" s="4" t="n"/>
+      <c r="I110" s="4" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -2813,6 +3079,9 @@
       <c r="H111" s="6" t="n">
         <v>21.18</v>
       </c>
+      <c r="I111" s="6" t="n">
+        <v>21.18</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -2837,6 +3106,9 @@
         <v>4021.92</v>
       </c>
       <c r="H112" s="6" t="n">
+        <v>3985</v>
+      </c>
+      <c r="I112" s="6" t="n">
         <v>3985</v>
       </c>
     </row>
@@ -2849,6 +3121,7 @@
       <c r="F113" s="4" t="n"/>
       <c r="G113" s="4" t="n"/>
       <c r="H113" s="4" t="n"/>
+      <c r="I113" s="4" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -2875,6 +3148,9 @@
       <c r="H114" s="6" t="n">
         <v>29.02</v>
       </c>
+      <c r="I114" s="6" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -2899,6 +3175,9 @@
         <v>3410</v>
       </c>
       <c r="H115" s="6" t="n">
+        <v>3409.93</v>
+      </c>
+      <c r="I115" s="6" t="n">
         <v>3409.93</v>
       </c>
     </row>

</xml_diff>